<commit_message>
Citation data update, structure annotation fixes
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
-    <sheet name="Deprecated" sheetId="2" r:id="rId2"/>
+    <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
+    <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -540,9 +541,6 @@
     <t>https://gpcrdb.org/structure/g_protein_structure_browser</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/arrestin_structure_browser</t>
-  </si>
-  <si>
     <t>GPCR-G protein interface mutations</t>
   </si>
   <si>
@@ -619,6 +617,9 @@
   </si>
   <si>
     <t>Ligand site mutations</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/structure</t>
   </si>
 </sst>
 </file>
@@ -1200,11 +1201,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1273,7 @@
         <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>67</v>
@@ -1348,7 +1349,7 @@
         <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
@@ -1383,7 +1384,7 @@
         <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>70</v>
@@ -1421,7 +1422,7 @@
         <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>71</v>
@@ -1492,7 +1493,7 @@
         <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>72</v>
@@ -1524,10 +1525,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>73</v>
@@ -1559,10 +1560,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
         <v>179</v>
-      </c>
-      <c r="D10" t="s">
-        <v>180</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>80</v>
@@ -1594,10 +1595,10 @@
         <v>19</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>79</v>
@@ -1773,7 +1774,7 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>81</v>
@@ -1799,49 +1800,77 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="H17" s="28" t="b">
         <v>0</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17">
+        <v>2018</v>
+      </c>
+      <c r="L17" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>186</v>
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="H18" s="28" t="b">
         <v>0</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" t="s">
+        <v>122</v>
+      </c>
+      <c r="K18">
+        <v>2018</v>
+      </c>
+      <c r="L18" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -1850,10 +1879,10 @@
         <v>132</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>157</v>
@@ -1861,7 +1890,7 @@
       <c r="H19" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="16" t="s">
         <v>123</v>
       </c>
       <c r="J19" t="s">
@@ -1876,149 +1905,138 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H20" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>123</v>
+      <c r="I20" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="J20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K20">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>132</v>
-      </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>187</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>157</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="G21" s="5"/>
       <c r="H21" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" t="s">
-        <v>122</v>
-      </c>
-      <c r="K21">
-        <v>2018</v>
-      </c>
-      <c r="L21" t="s">
-        <v>129</v>
+      <c r="I21" s="16"/>
+      <c r="J21" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>146</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="J22" t="s">
-        <v>124</v>
-      </c>
-      <c r="K22">
-        <v>2017</v>
-      </c>
-      <c r="L22" t="s">
-        <v>126</v>
+      <c r="J22" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H23" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="13" t="s">
-        <v>134</v>
+      <c r="I23" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23">
+        <v>2017</v>
+      </c>
+      <c r="L23" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="28" t="b">
@@ -2030,54 +2048,43 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G25" s="5"/>
       <c r="H25" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J25" t="s">
-        <v>124</v>
-      </c>
-      <c r="K25">
-        <v>2017</v>
-      </c>
-      <c r="L25" t="s">
-        <v>126</v>
+      <c r="J25" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="28" t="b">
@@ -2089,43 +2096,54 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H27" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="13" t="s">
-        <v>134</v>
+      <c r="I27" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J27" t="s">
+        <v>124</v>
+      </c>
+      <c r="K27">
+        <v>2017</v>
+      </c>
+      <c r="L27" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>188</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>172</v>
+        <v>54</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="28" t="b">
@@ -2135,58 +2153,47 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>188</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D29" t="s">
-        <v>171</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J29" t="s">
-        <v>124</v>
-      </c>
-      <c r="K29">
-        <v>2017</v>
-      </c>
-      <c r="L29" t="s">
-        <v>126</v>
+      <c r="J29" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>196</v>
+      </c>
+      <c r="G30" s="6"/>
       <c r="H30" s="28" t="b">
         <v>0</v>
       </c>
@@ -2194,47 +2201,59 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="H31" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="13" t="s">
-        <v>134</v>
+      <c r="I31" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J31" t="s">
+        <v>119</v>
+      </c>
+      <c r="K31">
+        <v>2016</v>
+      </c>
+      <c r="L31" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>59</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G32" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="G32" s="5"/>
       <c r="H32" s="28" t="b">
         <v>0</v>
       </c>
@@ -2244,43 +2263,31 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G33" s="5"/>
       <c r="H33" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J33" t="s">
-        <v>119</v>
-      </c>
-      <c r="K33">
-        <v>2016</v>
-      </c>
-      <c r="L33" t="s">
-        <v>121</v>
+      <c r="J33" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -2289,10 +2296,10 @@
         <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="28" t="b">
@@ -2304,19 +2311,19 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="28" t="b">
@@ -2328,67 +2335,83 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G36" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="H36" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J36" s="13" t="s">
-        <v>134</v>
+      <c r="I36" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J36" t="s">
+        <v>127</v>
+      </c>
+      <c r="K36">
+        <v>2017</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G37" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="H37" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>134</v>
+      <c r="I37" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" t="s">
+        <v>127</v>
+      </c>
+      <c r="K37">
+        <v>2017</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>193</v>
+        <v>31</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>161</v>
@@ -2408,121 +2431,130 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H39" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="15" t="s">
-        <v>128</v>
+      <c r="I39" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="J39" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K39">
-        <v>2017</v>
+        <v>2018</v>
+      </c>
+      <c r="L39" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H40" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>128</v>
+      <c r="I40" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="J40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K40">
-        <v>2017</v>
+        <v>2018</v>
+      </c>
+      <c r="L40" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H41" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J41" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="K41">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="L41" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>179</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H42" s="28" t="b">
         <v>0</v>
@@ -2530,142 +2562,142 @@
       <c r="I42" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J42" t="s">
-        <v>114</v>
+      <c r="J42" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K42">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L42" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D43" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>26</v>
+        <v>79</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H43" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J43" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K43">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L43" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H44" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J44" s="23" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="J44" t="s">
+        <v>111</v>
       </c>
       <c r="K44">
         <v>2016</v>
       </c>
       <c r="L44" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H45" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>107</v>
+        <v>120</v>
+      </c>
+      <c r="J45" t="s">
+        <v>119</v>
       </c>
       <c r="K45">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L45" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>155</v>
@@ -2688,151 +2720,151 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H47" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J47" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="K47">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L47" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>93</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F48" s="4"/>
       <c r="G48" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H48" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J48" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K48">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L48" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H49" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="J49" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="K49">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L49" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G50" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H50" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="J50" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="K50">
         <v>2019</v>
       </c>
       <c r="L50" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
@@ -2841,10 +2873,10 @@
         <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>159</v>
@@ -2867,22 +2899,19 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>159</v>
@@ -2905,19 +2934,19 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>159</v>
@@ -2940,7 +2969,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
         <v>32</v>
@@ -2949,10 +2978,10 @@
         <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>159</v>
@@ -2975,19 +3004,19 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D55" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>159</v>
@@ -3010,19 +3039,19 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>159</v>
@@ -3045,7 +3074,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>32</v>
@@ -3054,10 +3083,10 @@
         <v>153</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>159</v>
@@ -3079,124 +3108,54 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" t="s">
-        <v>40</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H58" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J58" t="s">
-        <v>139</v>
-      </c>
-      <c r="K58">
-        <v>2019</v>
-      </c>
-      <c r="L58" t="s">
-        <v>140</v>
-      </c>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D59" t="s">
-        <v>41</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H59" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J59" t="s">
-        <v>139</v>
-      </c>
-      <c r="K59">
-        <v>2019</v>
-      </c>
-      <c r="L59" t="s">
-        <v>140</v>
-      </c>
+      <c r="B59" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
+      <c r="B60" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="B61" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G62" s="26"/>
       <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
+      <c r="B63" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G64" s="26"/>
       <c r="H64" s="26"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
     </row>
   </sheetData>
   <sortState ref="A2:L69">
@@ -3204,32 +3163,32 @@
     <sortCondition ref="I2:I69"/>
     <sortCondition ref="J2:J69"/>
   </sortState>
-  <conditionalFormatting sqref="H52:H1046758 H1:H50">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="H50:H1046756 H1:H48">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H51)))</formula>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H51)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1"/>
-    <hyperlink ref="F52" r:id="rId2"/>
-    <hyperlink ref="E50" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E28" r:id="rId4"/>
-    <hyperlink ref="E30" r:id="rId5"/>
-    <hyperlink ref="E31" r:id="rId6"/>
-    <hyperlink ref="E34" r:id="rId7"/>
-    <hyperlink ref="E35" r:id="rId8"/>
-    <hyperlink ref="E37" r:id="rId9"/>
+    <hyperlink ref="F43" r:id="rId1"/>
+    <hyperlink ref="F50" r:id="rId2"/>
+    <hyperlink ref="E48" r:id="rId3" location="mutation-data-submission"/>
+    <hyperlink ref="E26" r:id="rId4"/>
+    <hyperlink ref="E28" r:id="rId5"/>
+    <hyperlink ref="E29" r:id="rId6"/>
+    <hyperlink ref="E32" r:id="rId7"/>
+    <hyperlink ref="E33" r:id="rId8"/>
+    <hyperlink ref="E35" r:id="rId9"/>
     <hyperlink ref="E3" r:id="rId10"/>
     <hyperlink ref="E4" r:id="rId11"/>
     <hyperlink ref="E7" r:id="rId12"/>
@@ -3244,86 +3203,157 @@
     <hyperlink ref="E11" r:id="rId21"/>
     <hyperlink ref="E10" r:id="rId22"/>
     <hyperlink ref="E16" r:id="rId23"/>
-    <hyperlink ref="E33" r:id="rId24"/>
-    <hyperlink ref="E47" r:id="rId25"/>
-    <hyperlink ref="E19" r:id="rId26"/>
-    <hyperlink ref="E20" r:id="rId27"/>
-    <hyperlink ref="E21" r:id="rId28"/>
-    <hyperlink ref="E22" r:id="rId29"/>
-    <hyperlink ref="E23" r:id="rId30"/>
-    <hyperlink ref="E24" r:id="rId31"/>
-    <hyperlink ref="E25" r:id="rId32"/>
-    <hyperlink ref="E27" r:id="rId33"/>
-    <hyperlink ref="E41" r:id="rId34"/>
-    <hyperlink ref="E42" r:id="rId35"/>
-    <hyperlink ref="E43" r:id="rId36"/>
-    <hyperlink ref="E45" r:id="rId37"/>
-    <hyperlink ref="E44" r:id="rId38"/>
-    <hyperlink ref="E46" r:id="rId39"/>
-    <hyperlink ref="E48" r:id="rId40"/>
-    <hyperlink ref="E49" r:id="rId41"/>
-    <hyperlink ref="E40" r:id="rId42"/>
-    <hyperlink ref="E39" r:id="rId43"/>
-    <hyperlink ref="E38" r:id="rId44"/>
-    <hyperlink ref="E51" r:id="rId45"/>
-    <hyperlink ref="E52" r:id="rId46"/>
-    <hyperlink ref="E53" r:id="rId47"/>
-    <hyperlink ref="E54" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E55" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E56" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E57" r:id="rId51"/>
-    <hyperlink ref="E58" r:id="rId52"/>
-    <hyperlink ref="E59" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G49" r:id="rId54"/>
-    <hyperlink ref="G48" r:id="rId55"/>
+    <hyperlink ref="E31" r:id="rId24"/>
+    <hyperlink ref="E45" r:id="rId25"/>
+    <hyperlink ref="E17" r:id="rId26"/>
+    <hyperlink ref="E18" r:id="rId27"/>
+    <hyperlink ref="E19" r:id="rId28"/>
+    <hyperlink ref="E20" r:id="rId29"/>
+    <hyperlink ref="E21" r:id="rId30"/>
+    <hyperlink ref="E22" r:id="rId31"/>
+    <hyperlink ref="E23" r:id="rId32"/>
+    <hyperlink ref="E25" r:id="rId33"/>
+    <hyperlink ref="E39" r:id="rId34"/>
+    <hyperlink ref="E40" r:id="rId35"/>
+    <hyperlink ref="E41" r:id="rId36"/>
+    <hyperlink ref="E43" r:id="rId37"/>
+    <hyperlink ref="E42" r:id="rId38"/>
+    <hyperlink ref="E44" r:id="rId39"/>
+    <hyperlink ref="E46" r:id="rId40"/>
+    <hyperlink ref="E47" r:id="rId41"/>
+    <hyperlink ref="E38" r:id="rId42"/>
+    <hyperlink ref="E37" r:id="rId43"/>
+    <hyperlink ref="E36" r:id="rId44"/>
+    <hyperlink ref="E49" r:id="rId45"/>
+    <hyperlink ref="E50" r:id="rId46"/>
+    <hyperlink ref="E51" r:id="rId47"/>
+    <hyperlink ref="E52" r:id="rId48" location="truncations"/>
+    <hyperlink ref="E53" r:id="rId49" location="fusions"/>
+    <hyperlink ref="E54" r:id="rId50" location="loopdeletions"/>
+    <hyperlink ref="E55" r:id="rId51"/>
+    <hyperlink ref="E56" r:id="rId52"/>
+    <hyperlink ref="E57" r:id="rId53" location="mutations"/>
+    <hyperlink ref="G47" r:id="rId54"/>
+    <hyperlink ref="G46" r:id="rId55"/>
     <hyperlink ref="G9" r:id="rId56"/>
-    <hyperlink ref="G46" r:id="rId57"/>
+    <hyperlink ref="G44" r:id="rId57"/>
     <hyperlink ref="G8" r:id="rId58"/>
     <hyperlink ref="G6" r:id="rId59"/>
     <hyperlink ref="G12" r:id="rId60"/>
     <hyperlink ref="G3" r:id="rId61"/>
     <hyperlink ref="G4" r:id="rId62"/>
     <hyperlink ref="G7" r:id="rId63"/>
-    <hyperlink ref="G33" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G50" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G43" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G47" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G31" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G48" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G41" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G45" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
     <hyperlink ref="G14" r:id="rId68"/>
-    <hyperlink ref="G41" r:id="rId69"/>
-    <hyperlink ref="G42" r:id="rId70"/>
-    <hyperlink ref="G51" r:id="rId71"/>
-    <hyperlink ref="G52" r:id="rId72"/>
-    <hyperlink ref="G53" r:id="rId73"/>
-    <hyperlink ref="G54" r:id="rId74"/>
-    <hyperlink ref="G55" r:id="rId75"/>
-    <hyperlink ref="G56" r:id="rId76"/>
-    <hyperlink ref="G57" r:id="rId77"/>
-    <hyperlink ref="G58" r:id="rId78"/>
-    <hyperlink ref="G59" r:id="rId79"/>
-    <hyperlink ref="G22" r:id="rId80"/>
-    <hyperlink ref="G25" r:id="rId81"/>
-    <hyperlink ref="G29" r:id="rId82"/>
-    <hyperlink ref="G40" r:id="rId83"/>
-    <hyperlink ref="G39" r:id="rId84"/>
-    <hyperlink ref="G38" r:id="rId85"/>
+    <hyperlink ref="G39" r:id="rId69"/>
+    <hyperlink ref="G40" r:id="rId70"/>
+    <hyperlink ref="G49" r:id="rId71"/>
+    <hyperlink ref="G50" r:id="rId72"/>
+    <hyperlink ref="G51" r:id="rId73"/>
+    <hyperlink ref="G52" r:id="rId74"/>
+    <hyperlink ref="G53" r:id="rId75"/>
+    <hyperlink ref="G54" r:id="rId76"/>
+    <hyperlink ref="G55" r:id="rId77"/>
+    <hyperlink ref="G56" r:id="rId78"/>
+    <hyperlink ref="G57" r:id="rId79"/>
+    <hyperlink ref="G20" r:id="rId80"/>
+    <hyperlink ref="G23" r:id="rId81"/>
+    <hyperlink ref="G27" r:id="rId82"/>
+    <hyperlink ref="G38" r:id="rId83"/>
+    <hyperlink ref="G37" r:id="rId84"/>
+    <hyperlink ref="G36" r:id="rId85"/>
     <hyperlink ref="G16" r:id="rId86"/>
     <hyperlink ref="G5" r:id="rId87"/>
     <hyperlink ref="G11" r:id="rId88"/>
     <hyperlink ref="G15" r:id="rId89"/>
     <hyperlink ref="G10" r:id="rId90"/>
-    <hyperlink ref="G45" r:id="rId91"/>
-    <hyperlink ref="G44" r:id="rId92"/>
-    <hyperlink ref="E26" r:id="rId93"/>
-    <hyperlink ref="E32" r:id="rId94"/>
-    <hyperlink ref="E17" r:id="rId95"/>
-    <hyperlink ref="E18" r:id="rId96"/>
-    <hyperlink ref="E36" r:id="rId97"/>
+    <hyperlink ref="G43" r:id="rId91"/>
+    <hyperlink ref="G42" r:id="rId92"/>
+    <hyperlink ref="E24" r:id="rId93"/>
+    <hyperlink ref="E30" r:id="rId94"/>
+    <hyperlink ref="E34" r:id="rId95"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L2"/>
   <sheetViews>

</xml_diff>

<commit_message>
2 new structures, little citation and annotation cleanup
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -839,7 +839,47 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1201,11 +1241,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2179,67 +2219,67 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G30" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="H30" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="13" t="s">
-        <v>134</v>
+      <c r="I30" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K30">
+        <v>2016</v>
+      </c>
+      <c r="L30" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G31" s="5"/>
       <c r="H31" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J31" t="s">
-        <v>119</v>
-      </c>
-      <c r="K31">
-        <v>2016</v>
-      </c>
-      <c r="L31" t="s">
-        <v>121</v>
+      <c r="J31" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
@@ -2248,10 +2288,10 @@
         <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="28" t="b">
@@ -2263,7 +2303,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
@@ -2272,10 +2312,10 @@
         <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="28" t="b">
@@ -2287,19 +2327,19 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>190</v>
+        <v>65</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="28" t="b">
@@ -2311,31 +2351,39 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="H35" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>134</v>
+      <c r="I35" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J35" t="s">
+        <v>127</v>
+      </c>
+      <c r="K35">
+        <v>2017</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>191</v>
@@ -2344,10 +2392,10 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>161</v>
@@ -2367,7 +2415,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>191</v>
@@ -2376,10 +2424,10 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>193</v>
+        <v>31</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>161</v>
@@ -2399,39 +2447,42 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>191</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H38" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="15" t="s">
-        <v>128</v>
+      <c r="I38" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="J38" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K38">
-        <v>2017</v>
+        <v>2018</v>
+      </c>
+      <c r="L38" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>191</v>
@@ -2440,10 +2491,10 @@
         <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>158</v>
@@ -2466,42 +2517,45 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>191</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>92</v>
+        <v>66</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H40" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J40" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="K40">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="L40" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>191</v>
@@ -2510,36 +2564,33 @@
         <v>194</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H41" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J41" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K41">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L41" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
         <v>191</v>
@@ -2548,10 +2599,13 @@
         <v>194</v>
       </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>154</v>
@@ -2574,45 +2628,42 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D43" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H43" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="J43" t="s">
+        <v>111</v>
       </c>
       <c r="K43">
         <v>2016</v>
       </c>
       <c r="L43" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
         <v>191</v>
@@ -2621,33 +2672,36 @@
         <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H44" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J44" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K44">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L44" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
         <v>191</v>
@@ -2656,36 +2710,33 @@
         <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H45" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J45" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="K45">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L45" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>191</v>
@@ -2694,10 +2745,10 @@
         <v>195</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>155</v>
@@ -2720,7 +2771,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
         <v>191</v>
@@ -2729,69 +2780,69 @@
         <v>195</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>94</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F47" s="4"/>
       <c r="G47" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H47" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J47" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K47">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L47" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>32</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="4"/>
+        <v>98</v>
+      </c>
       <c r="G48" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H48" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="J48" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="K48">
         <v>2019</v>
       </c>
       <c r="L48" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
         <v>32</v>
@@ -2800,10 +2851,13 @@
         <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>159</v>
@@ -2826,7 +2880,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
@@ -2835,13 +2889,10 @@
         <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>159</v>
@@ -2864,19 +2915,19 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>159</v>
@@ -2899,7 +2950,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
@@ -2908,10 +2959,10 @@
         <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>159</v>
@@ -2934,7 +2985,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
@@ -2943,10 +2994,10 @@
         <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>159</v>
@@ -2969,19 +3020,19 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>32</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D54" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>159</v>
@@ -3004,7 +3055,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
@@ -3013,10 +3064,10 @@
         <v>153</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>159</v>
@@ -3039,7 +3090,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
@@ -3048,10 +3099,10 @@
         <v>153</v>
       </c>
       <c r="D56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>159</v>
@@ -3073,89 +3124,54 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" t="s">
-        <v>41</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H57" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J57" t="s">
-        <v>139</v>
-      </c>
-      <c r="K57">
-        <v>2019</v>
-      </c>
-      <c r="L57" t="s">
-        <v>140</v>
-      </c>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
+      <c r="B58" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B59" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="B59" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
+      <c r="B60" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
+      <c r="B61" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G62" s="26"/>
       <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G63" s="26"/>
       <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B64" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26"/>
-    </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G65" s="24"/>
-      <c r="H65" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
     </row>
   </sheetData>
   <sortState ref="A2:L69">
@@ -3163,32 +3179,32 @@
     <sortCondition ref="I2:I69"/>
     <sortCondition ref="J2:J69"/>
   </sortState>
-  <conditionalFormatting sqref="H50:H1046756 H1:H48">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="H49:H1046755 H1:H47">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H49)))</formula>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H49)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F43" r:id="rId1"/>
-    <hyperlink ref="F50" r:id="rId2"/>
-    <hyperlink ref="E48" r:id="rId3" location="mutation-data-submission"/>
+    <hyperlink ref="F42" r:id="rId1"/>
+    <hyperlink ref="F49" r:id="rId2"/>
+    <hyperlink ref="E47" r:id="rId3" location="mutation-data-submission"/>
     <hyperlink ref="E26" r:id="rId4"/>
     <hyperlink ref="E28" r:id="rId5"/>
     <hyperlink ref="E29" r:id="rId6"/>
-    <hyperlink ref="E32" r:id="rId7"/>
-    <hyperlink ref="E33" r:id="rId8"/>
-    <hyperlink ref="E35" r:id="rId9"/>
+    <hyperlink ref="E31" r:id="rId7"/>
+    <hyperlink ref="E32" r:id="rId8"/>
+    <hyperlink ref="E34" r:id="rId9"/>
     <hyperlink ref="E3" r:id="rId10"/>
     <hyperlink ref="E4" r:id="rId11"/>
     <hyperlink ref="E7" r:id="rId12"/>
@@ -3203,8 +3219,8 @@
     <hyperlink ref="E11" r:id="rId21"/>
     <hyperlink ref="E10" r:id="rId22"/>
     <hyperlink ref="E16" r:id="rId23"/>
-    <hyperlink ref="E31" r:id="rId24"/>
-    <hyperlink ref="E45" r:id="rId25"/>
+    <hyperlink ref="E30" r:id="rId24"/>
+    <hyperlink ref="E44" r:id="rId25"/>
     <hyperlink ref="E17" r:id="rId26"/>
     <hyperlink ref="E18" r:id="rId27"/>
     <hyperlink ref="E19" r:id="rId28"/>
@@ -3213,68 +3229,67 @@
     <hyperlink ref="E22" r:id="rId31"/>
     <hyperlink ref="E23" r:id="rId32"/>
     <hyperlink ref="E25" r:id="rId33"/>
-    <hyperlink ref="E39" r:id="rId34"/>
-    <hyperlink ref="E40" r:id="rId35"/>
-    <hyperlink ref="E41" r:id="rId36"/>
-    <hyperlink ref="E43" r:id="rId37"/>
-    <hyperlink ref="E42" r:id="rId38"/>
-    <hyperlink ref="E44" r:id="rId39"/>
-    <hyperlink ref="E46" r:id="rId40"/>
-    <hyperlink ref="E47" r:id="rId41"/>
-    <hyperlink ref="E38" r:id="rId42"/>
-    <hyperlink ref="E37" r:id="rId43"/>
-    <hyperlink ref="E36" r:id="rId44"/>
-    <hyperlink ref="E49" r:id="rId45"/>
-    <hyperlink ref="E50" r:id="rId46"/>
-    <hyperlink ref="E51" r:id="rId47"/>
-    <hyperlink ref="E52" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E53" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E54" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E55" r:id="rId51"/>
-    <hyperlink ref="E56" r:id="rId52"/>
-    <hyperlink ref="E57" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G47" r:id="rId54"/>
-    <hyperlink ref="G46" r:id="rId55"/>
+    <hyperlink ref="E38" r:id="rId34"/>
+    <hyperlink ref="E39" r:id="rId35"/>
+    <hyperlink ref="E40" r:id="rId36"/>
+    <hyperlink ref="E42" r:id="rId37"/>
+    <hyperlink ref="E41" r:id="rId38"/>
+    <hyperlink ref="E43" r:id="rId39"/>
+    <hyperlink ref="E45" r:id="rId40"/>
+    <hyperlink ref="E46" r:id="rId41"/>
+    <hyperlink ref="E37" r:id="rId42"/>
+    <hyperlink ref="E36" r:id="rId43"/>
+    <hyperlink ref="E35" r:id="rId44"/>
+    <hyperlink ref="E48" r:id="rId45"/>
+    <hyperlink ref="E49" r:id="rId46"/>
+    <hyperlink ref="E50" r:id="rId47"/>
+    <hyperlink ref="E51" r:id="rId48" location="truncations"/>
+    <hyperlink ref="E52" r:id="rId49" location="fusions"/>
+    <hyperlink ref="E53" r:id="rId50" location="loopdeletions"/>
+    <hyperlink ref="E54" r:id="rId51"/>
+    <hyperlink ref="E55" r:id="rId52"/>
+    <hyperlink ref="E56" r:id="rId53" location="mutations"/>
+    <hyperlink ref="G46" r:id="rId54"/>
+    <hyperlink ref="G45" r:id="rId55"/>
     <hyperlink ref="G9" r:id="rId56"/>
-    <hyperlink ref="G44" r:id="rId57"/>
+    <hyperlink ref="G43" r:id="rId57"/>
     <hyperlink ref="G8" r:id="rId58"/>
     <hyperlink ref="G6" r:id="rId59"/>
     <hyperlink ref="G12" r:id="rId60"/>
     <hyperlink ref="G3" r:id="rId61"/>
     <hyperlink ref="G4" r:id="rId62"/>
     <hyperlink ref="G7" r:id="rId63"/>
-    <hyperlink ref="G31" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G48" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G41" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G45" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G30" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G47" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G40" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G44" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
     <hyperlink ref="G14" r:id="rId68"/>
-    <hyperlink ref="G39" r:id="rId69"/>
-    <hyperlink ref="G40" r:id="rId70"/>
-    <hyperlink ref="G49" r:id="rId71"/>
-    <hyperlink ref="G50" r:id="rId72"/>
-    <hyperlink ref="G51" r:id="rId73"/>
-    <hyperlink ref="G52" r:id="rId74"/>
-    <hyperlink ref="G53" r:id="rId75"/>
-    <hyperlink ref="G54" r:id="rId76"/>
-    <hyperlink ref="G55" r:id="rId77"/>
-    <hyperlink ref="G56" r:id="rId78"/>
-    <hyperlink ref="G57" r:id="rId79"/>
+    <hyperlink ref="G38" r:id="rId69"/>
+    <hyperlink ref="G39" r:id="rId70"/>
+    <hyperlink ref="G48" r:id="rId71"/>
+    <hyperlink ref="G49" r:id="rId72"/>
+    <hyperlink ref="G50" r:id="rId73"/>
+    <hyperlink ref="G51" r:id="rId74"/>
+    <hyperlink ref="G52" r:id="rId75"/>
+    <hyperlink ref="G53" r:id="rId76"/>
+    <hyperlink ref="G54" r:id="rId77"/>
+    <hyperlink ref="G55" r:id="rId78"/>
+    <hyperlink ref="G56" r:id="rId79"/>
     <hyperlink ref="G20" r:id="rId80"/>
     <hyperlink ref="G23" r:id="rId81"/>
     <hyperlink ref="G27" r:id="rId82"/>
-    <hyperlink ref="G38" r:id="rId83"/>
-    <hyperlink ref="G37" r:id="rId84"/>
-    <hyperlink ref="G36" r:id="rId85"/>
+    <hyperlink ref="G37" r:id="rId83"/>
+    <hyperlink ref="G36" r:id="rId84"/>
+    <hyperlink ref="G35" r:id="rId85"/>
     <hyperlink ref="G16" r:id="rId86"/>
     <hyperlink ref="G5" r:id="rId87"/>
     <hyperlink ref="G11" r:id="rId88"/>
     <hyperlink ref="G15" r:id="rId89"/>
     <hyperlink ref="G10" r:id="rId90"/>
-    <hyperlink ref="G43" r:id="rId91"/>
-    <hyperlink ref="G42" r:id="rId92"/>
+    <hyperlink ref="G42" r:id="rId91"/>
+    <hyperlink ref="G41" r:id="rId92"/>
     <hyperlink ref="E24" r:id="rId93"/>
-    <hyperlink ref="E30" r:id="rId94"/>
-    <hyperlink ref="E34" r:id="rId95"/>
+    <hyperlink ref="E33" r:id="rId94"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3282,15 +3297,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I3"/>
+  <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>16</v>
       </c>
@@ -3313,7 +3328,7 @@
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>17</v>
       </c>
@@ -3336,18 +3351,53 @@
       </c>
       <c r="I3" s="12"/>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: reference for isoform resource
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/common_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE23048F-A1FA-AF4A-813E-2B7316FDF8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="32480" windowHeight="19860" tabRatio="500"/>
+    <workbookView xWindow="9480" yWindow="460" windowWidth="39240" windowHeight="28320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
     <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
     <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -620,12 +630,24 @@
   </si>
   <si>
     <t>https://gpcrdb.org/structure</t>
+  </si>
+  <si>
+    <t>Isoforms</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/protein/isoforms</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41586-020-2888-2</t>
+  </si>
+  <si>
+    <t>Combinatorial expression of GPCR isoforms affects signalling and drug responses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -839,27 +861,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1240,12 +1242,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,31 +1567,31 @@
         <v>19</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>73</v>
+        <v>198</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="H9" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="K9">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1603,28 +1605,28 @@
         <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H10" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="J10" t="s">
+        <v>111</v>
       </c>
       <c r="K10">
         <v>2016</v>
       </c>
       <c r="L10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1638,13 +1640,10 @@
         <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>154</v>
@@ -1673,34 +1672,34 @@
         <v>19</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K12">
         <v>2016</v>
       </c>
       <c r="L12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1714,23 +1713,31 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="H13" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>137</v>
+      <c r="I13" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" t="s">
+        <v>111</v>
       </c>
       <c r="K13">
-        <v>2021</v>
+        <v>2016</v>
+      </c>
+      <c r="L13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1744,28 +1751,23 @@
         <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H14" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="J14" t="s">
-        <v>114</v>
+      <c r="J14" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="K14">
-        <v>2018</v>
-      </c>
-      <c r="L14" t="s">
-        <v>115</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1779,28 +1781,28 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H15" s="28" t="b">
-        <v>0</v>
+        <v>158</v>
+      </c>
+      <c r="H15" s="29" t="b">
+        <v>1</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J15" s="23" t="s">
-        <v>107</v>
+      <c r="J15" t="s">
+        <v>114</v>
       </c>
       <c r="K15">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L15" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1814,63 +1816,63 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H16" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K16">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="H17" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K17">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="L17" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1884,10 +1886,10 @@
         <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>157</v>
@@ -1919,10 +1921,10 @@
         <v>132</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>157</v>
@@ -1930,7 +1932,7 @@
       <c r="H19" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="12" t="s">
         <v>123</v>
       </c>
       <c r="J19" t="s">
@@ -1948,34 +1950,34 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H20" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K20">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L20" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1986,21 +1988,31 @@
         <v>48</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H21" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="13" t="s">
-        <v>134</v>
+      <c r="I21" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21">
+        <v>2017</v>
+      </c>
+      <c r="L21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2014,15 +2026,16 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="28" t="b">
         <v>0</v>
       </c>
+      <c r="I22" s="16"/>
       <c r="J22" s="13" t="s">
         <v>134</v>
       </c>
@@ -2035,31 +2048,20 @@
         <v>48</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J23" t="s">
-        <v>124</v>
-      </c>
-      <c r="K23">
-        <v>2017</v>
-      </c>
-      <c r="L23" t="s">
-        <v>126</v>
+      <c r="J23" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2070,20 +2072,31 @@
         <v>48</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H24" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>134</v>
+      <c r="I24" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J24" t="s">
+        <v>124</v>
+      </c>
+      <c r="K24">
+        <v>2017</v>
+      </c>
+      <c r="L24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2097,10 +2110,10 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="28" t="b">
@@ -2118,13 +2131,13 @@
         <v>48</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>44</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="28" t="b">
@@ -2142,31 +2155,20 @@
         <v>48</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="5"/>
       <c r="H27" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J27" t="s">
-        <v>124</v>
-      </c>
-      <c r="K27">
-        <v>2017</v>
-      </c>
-      <c r="L27" t="s">
-        <v>126</v>
+      <c r="J27" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2174,26 +2176,37 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>48</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H28" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J28" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K28">
+        <v>2017</v>
+      </c>
+      <c r="L28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>30</v>
       </c>
@@ -2201,13 +2214,13 @@
         <v>188</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="28" t="b">
@@ -2217,59 +2230,47 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G30" s="5"/>
       <c r="H30" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J30" t="s">
-        <v>119</v>
-      </c>
-      <c r="K30">
-        <v>2016</v>
-      </c>
-      <c r="L30" t="s">
-        <v>121</v>
+      <c r="J30" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>196</v>
+      </c>
+      <c r="G31" s="6"/>
       <c r="H31" s="28" t="b">
         <v>0</v>
       </c>
@@ -2279,31 +2280,43 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="H32" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>134</v>
+      <c r="I32" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J32" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32">
+        <v>2016</v>
+      </c>
+      <c r="L32" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
@@ -2312,10 +2325,10 @@
         <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>189</v>
+        <v>61</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="28" t="b">
@@ -2327,19 +2340,19 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="28" t="b">
@@ -2351,71 +2364,55 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>161</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="G35" s="5"/>
       <c r="H35" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="J35" t="s">
-        <v>127</v>
-      </c>
-      <c r="K35">
-        <v>2017</v>
+      <c r="J35" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>161</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G36" s="5"/>
       <c r="H36" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="J36" t="s">
-        <v>127</v>
-      </c>
-      <c r="K36">
-        <v>2017</v>
+      <c r="J36" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>191</v>
@@ -2424,10 +2421,10 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>161</v>
@@ -2447,130 +2444,121 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>191</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H38" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="12" t="s">
-        <v>108</v>
+      <c r="I38" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="J38" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="K38">
-        <v>2018</v>
-      </c>
-      <c r="L38" t="s">
-        <v>115</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
         <v>191</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H39" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="12" t="s">
-        <v>108</v>
+      <c r="I39" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="J39" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="K39">
-        <v>2018</v>
-      </c>
-      <c r="L39" t="s">
-        <v>115</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>191</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>194</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H40" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="J40" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K40">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="L40" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>191</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>194</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>24</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H41" s="28" t="b">
         <v>0</v>
@@ -2578,19 +2566,19 @@
       <c r="I41" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J41" s="23" t="s">
-        <v>107</v>
+      <c r="J41" t="s">
+        <v>114</v>
       </c>
       <c r="K41">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L41" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>191</v>
@@ -2599,109 +2587,109 @@
         <v>194</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H42" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J42" s="23" t="s">
-        <v>107</v>
+        <v>120</v>
+      </c>
+      <c r="J42" t="s">
+        <v>119</v>
       </c>
       <c r="K42">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="L42" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H43" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="J43" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K43">
         <v>2016</v>
       </c>
       <c r="L43" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
         <v>191</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H44" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="J44" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K44">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L44" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
         <v>191</v>
@@ -2710,10 +2698,10 @@
         <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>155</v>
@@ -2736,7 +2724,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
         <v>191</v>
@@ -2745,33 +2733,36 @@
         <v>195</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H46" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J46" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K46">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L46" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
         <v>191</v>
@@ -2780,107 +2771,104 @@
         <v>195</v>
       </c>
       <c r="D47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" s="4"/>
+        <v>93</v>
+      </c>
       <c r="G47" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H47" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J47" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="K47">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="L47" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H48" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="J48" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="K48">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="L48" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F49" s="4"/>
       <c r="G49" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H49" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="J49" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="K49">
         <v>2019</v>
       </c>
       <c r="L49" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
@@ -2889,10 +2877,10 @@
         <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>159</v>
@@ -2915,19 +2903,22 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>159</v>
@@ -2950,19 +2941,19 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>159</v>
@@ -2985,7 +2976,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
@@ -2994,10 +2985,10 @@
         <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>159</v>
@@ -3020,19 +3011,19 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
         <v>32</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>159</v>
@@ -3055,19 +3046,19 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>159</v>
@@ -3090,7 +3081,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
@@ -3099,10 +3090,10 @@
         <v>153</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>159</v>
@@ -3124,188 +3115,273 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
+      <c r="A57">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H57" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J57" t="s">
+        <v>139</v>
+      </c>
+      <c r="K57">
+        <v>2019</v>
+      </c>
+      <c r="L57" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B58" s="17" t="s">
+      <c r="A58">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H58" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J58" t="s">
+        <v>139</v>
+      </c>
+      <c r="K58">
+        <v>2019</v>
+      </c>
+      <c r="L58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B60" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B59" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G61" s="26"/>
       <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
+      <c r="B62" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G63" s="26"/>
       <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
+      <c r="B64" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
     </row>
   </sheetData>
-  <sortState ref="A2:L69">
-    <sortCondition ref="A2:A69"/>
-    <sortCondition ref="I2:I69"/>
-    <sortCondition ref="J2:J69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L70">
+    <sortCondition ref="A2:A70"/>
+    <sortCondition ref="I2:I70"/>
+    <sortCondition ref="J2:J70"/>
   </sortState>
-  <conditionalFormatting sqref="H49:H1046755 H1:H47">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="H51:H1046757 H1:H8 H10:H49">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H48)))</formula>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H48)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F42" r:id="rId1"/>
-    <hyperlink ref="F49" r:id="rId2"/>
-    <hyperlink ref="E47" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E26" r:id="rId4"/>
-    <hyperlink ref="E28" r:id="rId5"/>
-    <hyperlink ref="E29" r:id="rId6"/>
-    <hyperlink ref="E31" r:id="rId7"/>
-    <hyperlink ref="E32" r:id="rId8"/>
-    <hyperlink ref="E34" r:id="rId9"/>
-    <hyperlink ref="E3" r:id="rId10"/>
-    <hyperlink ref="E4" r:id="rId11"/>
-    <hyperlink ref="E7" r:id="rId12"/>
-    <hyperlink ref="E5" r:id="rId13"/>
-    <hyperlink ref="E6" r:id="rId14"/>
-    <hyperlink ref="E8" r:id="rId15"/>
-    <hyperlink ref="E9" r:id="rId16"/>
-    <hyperlink ref="E12" r:id="rId17"/>
-    <hyperlink ref="E13" r:id="rId18"/>
-    <hyperlink ref="E14" r:id="rId19"/>
-    <hyperlink ref="E15" r:id="rId20"/>
-    <hyperlink ref="E11" r:id="rId21"/>
-    <hyperlink ref="E10" r:id="rId22"/>
-    <hyperlink ref="E16" r:id="rId23"/>
-    <hyperlink ref="E30" r:id="rId24"/>
-    <hyperlink ref="E44" r:id="rId25"/>
-    <hyperlink ref="E17" r:id="rId26"/>
-    <hyperlink ref="E18" r:id="rId27"/>
-    <hyperlink ref="E19" r:id="rId28"/>
-    <hyperlink ref="E20" r:id="rId29"/>
-    <hyperlink ref="E21" r:id="rId30"/>
-    <hyperlink ref="E22" r:id="rId31"/>
-    <hyperlink ref="E23" r:id="rId32"/>
-    <hyperlink ref="E25" r:id="rId33"/>
-    <hyperlink ref="E38" r:id="rId34"/>
-    <hyperlink ref="E39" r:id="rId35"/>
-    <hyperlink ref="E40" r:id="rId36"/>
-    <hyperlink ref="E42" r:id="rId37"/>
-    <hyperlink ref="E41" r:id="rId38"/>
-    <hyperlink ref="E43" r:id="rId39"/>
-    <hyperlink ref="E45" r:id="rId40"/>
-    <hyperlink ref="E46" r:id="rId41"/>
-    <hyperlink ref="E37" r:id="rId42"/>
-    <hyperlink ref="E36" r:id="rId43"/>
-    <hyperlink ref="E35" r:id="rId44"/>
-    <hyperlink ref="E48" r:id="rId45"/>
-    <hyperlink ref="E49" r:id="rId46"/>
-    <hyperlink ref="E50" r:id="rId47"/>
-    <hyperlink ref="E51" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E52" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E53" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E54" r:id="rId51"/>
-    <hyperlink ref="E55" r:id="rId52"/>
-    <hyperlink ref="E56" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G46" r:id="rId54"/>
-    <hyperlink ref="G45" r:id="rId55"/>
-    <hyperlink ref="G9" r:id="rId56"/>
-    <hyperlink ref="G43" r:id="rId57"/>
-    <hyperlink ref="G8" r:id="rId58"/>
-    <hyperlink ref="G6" r:id="rId59"/>
-    <hyperlink ref="G12" r:id="rId60"/>
-    <hyperlink ref="G3" r:id="rId61"/>
-    <hyperlink ref="G4" r:id="rId62"/>
-    <hyperlink ref="G7" r:id="rId63"/>
-    <hyperlink ref="G30" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G47" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G40" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G44" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G14" r:id="rId68"/>
-    <hyperlink ref="G38" r:id="rId69"/>
-    <hyperlink ref="G39" r:id="rId70"/>
-    <hyperlink ref="G48" r:id="rId71"/>
-    <hyperlink ref="G49" r:id="rId72"/>
-    <hyperlink ref="G50" r:id="rId73"/>
-    <hyperlink ref="G51" r:id="rId74"/>
-    <hyperlink ref="G52" r:id="rId75"/>
-    <hyperlink ref="G53" r:id="rId76"/>
-    <hyperlink ref="G54" r:id="rId77"/>
-    <hyperlink ref="G55" r:id="rId78"/>
-    <hyperlink ref="G56" r:id="rId79"/>
-    <hyperlink ref="G20" r:id="rId80"/>
-    <hyperlink ref="G23" r:id="rId81"/>
-    <hyperlink ref="G27" r:id="rId82"/>
-    <hyperlink ref="G37" r:id="rId83"/>
-    <hyperlink ref="G36" r:id="rId84"/>
-    <hyperlink ref="G35" r:id="rId85"/>
-    <hyperlink ref="G16" r:id="rId86"/>
-    <hyperlink ref="G5" r:id="rId87"/>
-    <hyperlink ref="G11" r:id="rId88"/>
-    <hyperlink ref="G15" r:id="rId89"/>
-    <hyperlink ref="G10" r:id="rId90"/>
-    <hyperlink ref="G42" r:id="rId91"/>
-    <hyperlink ref="G41" r:id="rId92"/>
-    <hyperlink ref="E24" r:id="rId93"/>
-    <hyperlink ref="E33" r:id="rId94"/>
+    <hyperlink ref="F44" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F51" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E49" r:id="rId3" location="mutation-data-submission" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E29" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E33" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E36" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E15" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E46" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E19" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E21" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E22" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E23" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E24" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E26" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E44" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E43" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E45" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E47" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E37" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E50" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E51" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E53" r:id="rId48" location="truncations" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E54" r:id="rId49" location="fusions" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E55" r:id="rId50" location="loopdeletions" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E56" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E57" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E58" r:id="rId53" location="mutations" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G48" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G47" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G10" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G45" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G8" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G6" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="G13" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G3" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G4" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G7" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="G32" r:id="rId64" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="G49" r:id="rId65" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G42" r:id="rId66" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G46" r:id="rId67" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G15" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G40" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G41" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G50" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G51" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G52" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G53" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G54" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G55" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G56" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G57" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G58" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G21" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="G24" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="G28" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="G39" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="G38" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="G37" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="G17" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="G5" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="G12" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="G16" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="G11" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="G44" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="G43" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E25" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E31" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E35" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E9" r:id="rId96" xr:uid="{433CEF65-C40D-FF41-8BFE-4D4BD692C1E1}"/>
+    <hyperlink ref="G9" r:id="rId97" xr:uid="{078A35B2-0307-D942-9030-03EBF2A2A83A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>16</v>
       </c>
@@ -3328,7 +3404,7 @@
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>17</v>
       </c>
@@ -3351,67 +3427,36 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -3459,8 +3504,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: alignment update, new structures
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE23048F-A1FA-AF4A-813E-2B7316FDF8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="460" windowWidth="39240" windowHeight="28320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="39240" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
     <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
     <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,15 +33,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="204">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -642,12 +641,21 @@
   </si>
   <si>
     <t>Combinatorial expression of GPCR isoforms affects signalling and drug responses</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/structure/model_statistics</t>
+  </si>
+  <si>
+    <t>Structure model statistics</t>
+  </si>
+  <si>
+    <t>Homology model quality table based on RMSD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -861,7 +869,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1242,12 +1270,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1799,10 +1827,10 @@
         <v>114</v>
       </c>
       <c r="K15">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="L15" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1816,28 +1844,26 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H16" s="28" t="b">
+        <v>201</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="23" t="s">
-        <v>107</v>
+      <c r="J16" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="K16">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L16" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1851,68 +1877,68 @@
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H17" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J17" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="K17">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="L17" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="H18" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K18">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="L18" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -1921,10 +1947,10 @@
         <v>132</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>157</v>
@@ -1947,7 +1973,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1956,10 +1982,10 @@
         <v>132</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>157</v>
@@ -1967,7 +1993,7 @@
       <c r="H20" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="12" t="s">
         <v>123</v>
       </c>
       <c r="J20" t="s">
@@ -1982,67 +2008,77 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H21" s="28" t="b">
         <v>0</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K21">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L21" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H22" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="13" t="s">
-        <v>134</v>
+      <c r="I22" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" t="s">
+        <v>124</v>
+      </c>
+      <c r="K22">
+        <v>2017</v>
+      </c>
+      <c r="L22" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
@@ -2051,81 +2087,82 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="28" t="b">
         <v>0</v>
       </c>
+      <c r="I23" s="16"/>
       <c r="J23" s="13" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J24" t="s">
-        <v>124</v>
-      </c>
-      <c r="K24">
-        <v>2017</v>
-      </c>
-      <c r="L24" t="s">
-        <v>126</v>
+      <c r="J24" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H25" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>134</v>
+      <c r="I25" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" t="s">
+        <v>124</v>
+      </c>
+      <c r="K25">
+        <v>2017</v>
+      </c>
+      <c r="L25" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
@@ -2134,10 +2171,10 @@
         <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="28" t="b">
@@ -2149,19 +2186,19 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>171</v>
+        <v>44</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="28" t="b">
@@ -2173,78 +2210,78 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="J28" t="s">
-        <v>124</v>
-      </c>
-      <c r="K28">
-        <v>2017</v>
-      </c>
-      <c r="L28" t="s">
-        <v>126</v>
+      <c r="J28" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>48</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>170</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H29" s="28" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J29" t="s">
+        <v>124</v>
+      </c>
+      <c r="K29">
+        <v>2017</v>
+      </c>
+      <c r="L29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>188</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="28" t="b">
@@ -2254,23 +2291,23 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>188</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G31" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="G31" s="5"/>
       <c r="H31" s="28" t="b">
         <v>0</v>
       </c>
@@ -2280,7 +2317,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -2316,7 +2353,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
@@ -2340,7 +2377,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -2364,7 +2401,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
@@ -2388,7 +2425,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>59</v>
@@ -2412,7 +2449,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>191</v>
@@ -2444,7 +2481,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>191</v>
@@ -2476,7 +2513,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>191</v>
@@ -2508,7 +2545,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>191</v>
@@ -2543,7 +2580,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>191</v>
@@ -2578,7 +2615,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>191</v>
@@ -2616,7 +2653,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
@@ -2651,7 +2688,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>191</v>
@@ -2689,7 +2726,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>191</v>
@@ -2724,7 +2761,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>191</v>
@@ -2762,7 +2799,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>191</v>
@@ -2797,7 +2834,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>191</v>
@@ -2832,7 +2869,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>191</v>
@@ -2868,7 +2905,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
@@ -2903,7 +2940,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
@@ -2941,7 +2978,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
@@ -2976,7 +3013,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
@@ -3011,7 +3048,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>32</v>
@@ -3046,7 +3083,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
@@ -3081,7 +3118,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
@@ -3116,7 +3153,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>32</v>
@@ -3151,7 +3188,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>32</v>
@@ -3235,144 +3272,144 @@
       <c r="H66" s="24"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L70">
+  <sortState ref="A2:L70">
     <sortCondition ref="A2:A70"/>
     <sortCondition ref="I2:I70"/>
     <sortCondition ref="J2:J70"/>
   </sortState>
   <conditionalFormatting sqref="H51:H1046757 H1:H8 H10:H49">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F44" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F51" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E49" r:id="rId3" location="mutation-data-submission" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E29" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E33" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E36" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E15" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E11" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E46" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E19" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="E20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E21" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E22" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="E23" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E24" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="E26" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="E44" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="E43" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E45" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="E47" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="E37" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E50" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E51" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E53" r:id="rId48" location="truncations" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E54" r:id="rId49" location="fusions" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E55" r:id="rId50" location="loopdeletions" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E56" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="E57" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="E58" r:id="rId53" location="mutations" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G48" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="G47" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="G10" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="G45" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="G8" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="G6" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="G13" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G3" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="G4" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G7" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="G32" r:id="rId64" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="G49" r:id="rId65" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="G42" r:id="rId66" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="G46" r:id="rId67" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="G15" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G40" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="G41" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="G50" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="G51" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="G52" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G53" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="G54" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="G55" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="G56" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="G57" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="G58" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="G21" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="G24" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="G28" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="G39" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="G38" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="G37" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="G17" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="G5" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="G12" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="G16" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="G11" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="G44" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="G43" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="E25" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="E31" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="E35" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="E9" r:id="rId96" xr:uid="{433CEF65-C40D-FF41-8BFE-4D4BD692C1E1}"/>
-    <hyperlink ref="G9" r:id="rId97" xr:uid="{078A35B2-0307-D942-9030-03EBF2A2A83A}"/>
+    <hyperlink ref="F44" r:id="rId1"/>
+    <hyperlink ref="F51" r:id="rId2"/>
+    <hyperlink ref="E49" r:id="rId3" location="mutation-data-submission"/>
+    <hyperlink ref="E28" r:id="rId4"/>
+    <hyperlink ref="E30" r:id="rId5"/>
+    <hyperlink ref="E31" r:id="rId6"/>
+    <hyperlink ref="E33" r:id="rId7"/>
+    <hyperlink ref="E34" r:id="rId8"/>
+    <hyperlink ref="E36" r:id="rId9"/>
+    <hyperlink ref="E3" r:id="rId10"/>
+    <hyperlink ref="E4" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
+    <hyperlink ref="E5" r:id="rId13"/>
+    <hyperlink ref="E6" r:id="rId14"/>
+    <hyperlink ref="E8" r:id="rId15"/>
+    <hyperlink ref="E10" r:id="rId16"/>
+    <hyperlink ref="E13" r:id="rId17"/>
+    <hyperlink ref="E14" r:id="rId18"/>
+    <hyperlink ref="E15" r:id="rId19"/>
+    <hyperlink ref="E17" r:id="rId20"/>
+    <hyperlink ref="E12" r:id="rId21"/>
+    <hyperlink ref="E11" r:id="rId22"/>
+    <hyperlink ref="E18" r:id="rId23"/>
+    <hyperlink ref="E32" r:id="rId24"/>
+    <hyperlink ref="E46" r:id="rId25"/>
+    <hyperlink ref="E19" r:id="rId26"/>
+    <hyperlink ref="E20" r:id="rId27"/>
+    <hyperlink ref="E21" r:id="rId28"/>
+    <hyperlink ref="E22" r:id="rId29"/>
+    <hyperlink ref="E23" r:id="rId30"/>
+    <hyperlink ref="E24" r:id="rId31"/>
+    <hyperlink ref="E25" r:id="rId32"/>
+    <hyperlink ref="E27" r:id="rId33"/>
+    <hyperlink ref="E40" r:id="rId34"/>
+    <hyperlink ref="E41" r:id="rId35"/>
+    <hyperlink ref="E42" r:id="rId36"/>
+    <hyperlink ref="E44" r:id="rId37"/>
+    <hyperlink ref="E43" r:id="rId38"/>
+    <hyperlink ref="E45" r:id="rId39"/>
+    <hyperlink ref="E47" r:id="rId40"/>
+    <hyperlink ref="E48" r:id="rId41"/>
+    <hyperlink ref="E39" r:id="rId42"/>
+    <hyperlink ref="E38" r:id="rId43"/>
+    <hyperlink ref="E37" r:id="rId44"/>
+    <hyperlink ref="E50" r:id="rId45"/>
+    <hyperlink ref="E51" r:id="rId46"/>
+    <hyperlink ref="E52" r:id="rId47"/>
+    <hyperlink ref="E53" r:id="rId48" location="truncations"/>
+    <hyperlink ref="E54" r:id="rId49" location="fusions"/>
+    <hyperlink ref="E55" r:id="rId50" location="loopdeletions"/>
+    <hyperlink ref="E56" r:id="rId51"/>
+    <hyperlink ref="E57" r:id="rId52"/>
+    <hyperlink ref="E58" r:id="rId53" location="mutations"/>
+    <hyperlink ref="G48" r:id="rId54"/>
+    <hyperlink ref="G47" r:id="rId55"/>
+    <hyperlink ref="G10" r:id="rId56"/>
+    <hyperlink ref="G45" r:id="rId57"/>
+    <hyperlink ref="G8" r:id="rId58"/>
+    <hyperlink ref="G6" r:id="rId59"/>
+    <hyperlink ref="G13" r:id="rId60"/>
+    <hyperlink ref="G3" r:id="rId61"/>
+    <hyperlink ref="G4" r:id="rId62"/>
+    <hyperlink ref="G7" r:id="rId63"/>
+    <hyperlink ref="G32" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G49" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G42" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G46" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G15" r:id="rId68"/>
+    <hyperlink ref="G40" r:id="rId69"/>
+    <hyperlink ref="G41" r:id="rId70"/>
+    <hyperlink ref="G50" r:id="rId71"/>
+    <hyperlink ref="G51" r:id="rId72"/>
+    <hyperlink ref="G52" r:id="rId73"/>
+    <hyperlink ref="G53" r:id="rId74"/>
+    <hyperlink ref="G54" r:id="rId75"/>
+    <hyperlink ref="G55" r:id="rId76"/>
+    <hyperlink ref="G56" r:id="rId77"/>
+    <hyperlink ref="G57" r:id="rId78"/>
+    <hyperlink ref="G58" r:id="rId79"/>
+    <hyperlink ref="G22" r:id="rId80"/>
+    <hyperlink ref="G25" r:id="rId81"/>
+    <hyperlink ref="G29" r:id="rId82"/>
+    <hyperlink ref="G39" r:id="rId83"/>
+    <hyperlink ref="G38" r:id="rId84"/>
+    <hyperlink ref="G37" r:id="rId85"/>
+    <hyperlink ref="G18" r:id="rId86"/>
+    <hyperlink ref="G5" r:id="rId87"/>
+    <hyperlink ref="G12" r:id="rId88"/>
+    <hyperlink ref="G17" r:id="rId89"/>
+    <hyperlink ref="G11" r:id="rId90"/>
+    <hyperlink ref="G44" r:id="rId91"/>
+    <hyperlink ref="G43" r:id="rId92"/>
+    <hyperlink ref="E26" r:id="rId93"/>
+    <hyperlink ref="E35" r:id="rId94"/>
+    <hyperlink ref="E9" r:id="rId95"/>
+    <hyperlink ref="G9" r:id="rId96"/>
+    <hyperlink ref="E16" r:id="rId97"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3381,7 +3418,7 @@
     <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>16</v>
       </c>
@@ -3404,7 +3441,7 @@
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>17</v>
       </c>
@@ -3427,25 +3464,60 @@
       </c>
       <c r="I3" s="12"/>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3504,8 +3576,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MIX: Update of Structures documentation, fix of some G prot structure info, update references with NAR 2021 paper
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="39240" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="205">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -451,9 +451,6 @@
     <t>similarity search …</t>
   </si>
   <si>
-    <t>GPCRdb in 2021: …...</t>
-  </si>
-  <si>
     <t>Nat Methods</t>
   </si>
   <si>
@@ -650,13 +647,19 @@
   </si>
   <si>
     <t>Homology model quality table based on RMSD</t>
+  </si>
+  <si>
+    <t>GPCRdb in 2021: integrating GPCR sequence, structure and function</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/nar/gkaa1080</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -747,22 +750,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -826,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -843,13 +830,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -861,7 +846,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -1273,16 +1258,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
@@ -1301,7 +1286,7 @@
       <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>131</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1314,22 +1299,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>168</v>
-      </c>
       <c r="I1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1339,11 +1324,11 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>146</v>
+      <c r="C2" s="20" t="s">
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>67</v>
@@ -1352,9 +1337,9 @@
         <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H2" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -1377,8 +1362,8 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>147</v>
+      <c r="C3" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
@@ -1390,9 +1375,9 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H3" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="12" t="s">
@@ -1415,19 +1400,19 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>147</v>
+      <c r="C4" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H4" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="12" t="s">
@@ -1450,11 +1435,11 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>147</v>
+      <c r="C5" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>70</v>
@@ -1463,15 +1448,15 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H5" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H5" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="21" t="s">
         <v>135</v>
       </c>
       <c r="K5">
@@ -1488,19 +1473,19 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>147</v>
+      <c r="C6" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H6" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -1523,8 +1508,8 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>147</v>
+      <c r="C7" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1532,11 +1517,11 @@
       <c r="E7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="30"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H7" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H7" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="12" t="s">
@@ -1559,19 +1544,19 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>147</v>
+      <c r="C8" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H8" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="12" t="s">
@@ -1594,32 +1579,32 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>147</v>
+      <c r="C9" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H9" s="28" t="b">
+      <c r="H9" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K9">
         <v>2020</v>
       </c>
       <c r="L9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1629,19 +1614,19 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>178</v>
+      <c r="C10" s="20" t="s">
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H10" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H10" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="12" t="s">
@@ -1664,25 +1649,25 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
         <v>178</v>
-      </c>
-      <c r="D11" t="s">
-        <v>179</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H11" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="21" t="s">
         <v>107</v>
       </c>
       <c r="K11">
@@ -1699,11 +1684,11 @@
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>178</v>
+      <c r="C12" s="20" t="s">
+        <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>79</v>
@@ -1712,15 +1697,15 @@
         <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H12" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="21" t="s">
         <v>107</v>
       </c>
       <c r="K12">
@@ -1737,7 +1722,7 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D13" t="s">
@@ -1750,9 +1735,9 @@
         <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H13" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H13" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="12" t="s">
@@ -1775,7 +1760,7 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D14" t="s">
@@ -1784,18 +1769,20 @@
       <c r="E14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="20" t="s">
+      <c r="G14" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>137</v>
+      <c r="J14" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="K14">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1805,7 +1792,7 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D15" t="s">
@@ -1815,10 +1802,10 @@
         <v>76</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" s="29" t="b">
-        <v>1</v>
+        <v>157</v>
+      </c>
+      <c r="H15" s="27" t="b">
+        <v>0</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>108</v>
@@ -1827,10 +1814,10 @@
         <v>114</v>
       </c>
       <c r="K15">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="L15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1840,30 +1827,32 @@
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="29" t="b">
+        <v>200</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="27" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>137</v>
+      <c r="J16" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="K16">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="L16" t="s">
-        <v>115</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1873,7 +1862,7 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D17" t="s">
@@ -1883,15 +1872,15 @@
         <v>77</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H17" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H17" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="21" t="s">
         <v>107</v>
       </c>
       <c r="K17">
@@ -1908,19 +1897,19 @@
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H18" s="28" t="b">
+        <v>161</v>
+      </c>
+      <c r="H18" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="12" t="s">
@@ -1943,7 +1932,7 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D19" t="s">
@@ -1953,9 +1942,9 @@
         <v>85</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H19" s="28" t="b">
+        <v>156</v>
+      </c>
+      <c r="H19" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="12" t="s">
@@ -1978,7 +1967,7 @@
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D20" t="s">
@@ -1988,9 +1977,9 @@
         <v>86</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H20" s="28" t="b">
+        <v>156</v>
+      </c>
+      <c r="H20" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="12" t="s">
@@ -2013,7 +2002,7 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D21" t="s">
@@ -2023,12 +2012,12 @@
         <v>87</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H21" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>123</v>
       </c>
       <c r="J21" t="s">
@@ -2048,8 +2037,8 @@
       <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>146</v>
+      <c r="C22" s="20" t="s">
+        <v>145</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
@@ -2058,12 +2047,12 @@
         <v>88</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H22" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>125</v>
       </c>
       <c r="J22" t="s">
@@ -2083,20 +2072,20 @@
       <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="G23" s="5"/>
-      <c r="H23" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="16"/>
+      <c r="H23" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15"/>
       <c r="J23" s="13" t="s">
         <v>134</v>
       </c>
@@ -2108,7 +2097,7 @@
       <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
@@ -2118,7 +2107,7 @@
         <v>50</v>
       </c>
       <c r="G24" s="5"/>
-      <c r="H24" s="28" t="b">
+      <c r="H24" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J24" s="13" t="s">
@@ -2132,8 +2121,8 @@
       <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>147</v>
+      <c r="C25" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
@@ -2142,9 +2131,9 @@
         <v>90</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H25" s="28" t="b">
+        <v>159</v>
+      </c>
+      <c r="H25" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I25" s="12" t="s">
@@ -2167,17 +2156,17 @@
       <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="28" t="b">
+      <c r="H26" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J26" s="13" t="s">
@@ -2191,7 +2180,7 @@
       <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D27" t="s">
@@ -2201,7 +2190,7 @@
         <v>51</v>
       </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="28" t="b">
+      <c r="H27" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J27" s="13" t="s">
@@ -2215,17 +2204,17 @@
       <c r="B28" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>148</v>
+      <c r="C28" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="28" t="b">
+      <c r="H28" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J28" s="13" t="s">
@@ -2239,19 +2228,19 @@
       <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>149</v>
+      <c r="C29" s="20" t="s">
+        <v>148</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H29" s="28" t="b">
+        <v>159</v>
+      </c>
+      <c r="H29" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="12" t="s">
@@ -2272,10 +2261,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>146</v>
+        <v>187</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>145</v>
       </c>
       <c r="D30" t="s">
         <v>54</v>
@@ -2284,7 +2273,7 @@
         <v>55</v>
       </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="28" t="b">
+      <c r="H30" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J30" s="13" t="s">
@@ -2296,10 +2285,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>147</v>
+        <v>187</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
@@ -2308,7 +2297,7 @@
         <v>57</v>
       </c>
       <c r="G31" s="5"/>
-      <c r="H31" s="28" t="b">
+      <c r="H31" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="13" t="s">
@@ -2322,7 +2311,7 @@
       <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="20" t="s">
         <v>121</v>
       </c>
       <c r="D32" t="s">
@@ -2333,9 +2322,9 @@
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H32" s="28" t="b">
+        <v>155</v>
+      </c>
+      <c r="H32" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I32" s="12" t="s">
@@ -2358,8 +2347,8 @@
       <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>150</v>
+      <c r="C33" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -2368,7 +2357,7 @@
         <v>60</v>
       </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="28" t="b">
+      <c r="H33" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J33" s="13" t="s">
@@ -2382,8 +2371,8 @@
       <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>150</v>
+      <c r="C34" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="D34" t="s">
         <v>62</v>
@@ -2392,7 +2381,7 @@
         <v>63</v>
       </c>
       <c r="G34" s="5"/>
-      <c r="H34" s="28" t="b">
+      <c r="H34" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J34" s="13" t="s">
@@ -2406,17 +2395,17 @@
       <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>150</v>
+      <c r="C35" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="D35" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="G35" s="5"/>
-      <c r="H35" s="28" t="b">
+      <c r="H35" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J35" s="13" t="s">
@@ -2430,7 +2419,7 @@
       <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D36" t="s">
@@ -2440,7 +2429,7 @@
         <v>65</v>
       </c>
       <c r="G36" s="5"/>
-      <c r="H36" s="28" t="b">
+      <c r="H36" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J36" s="13" t="s">
@@ -2452,24 +2441,24 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
         <v>191</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" t="s">
-        <v>192</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>128</v>
       </c>
       <c r="J37" t="s">
@@ -2484,24 +2473,24 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
-      </c>
-      <c r="C38" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>96</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H38" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="14" t="s">
         <v>128</v>
       </c>
       <c r="J38" t="s">
@@ -2516,9 +2505,9 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D39" t="s">
@@ -2528,12 +2517,12 @@
         <v>95</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H39" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H39" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="14" t="s">
         <v>128</v>
       </c>
       <c r="J39" t="s">
@@ -2548,9 +2537,9 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D40" t="s">
@@ -2560,9 +2549,9 @@
         <v>91</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H40" s="28" t="b">
+        <v>157</v>
+      </c>
+      <c r="H40" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I40" s="12" t="s">
@@ -2583,9 +2572,9 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D41" t="s">
@@ -2595,9 +2584,9 @@
         <v>92</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H41" s="28" t="b">
+        <v>157</v>
+      </c>
+      <c r="H41" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I41" s="12" t="s">
@@ -2618,10 +2607,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -2633,9 +2622,9 @@
         <v>26</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H42" s="28" t="b">
+        <v>155</v>
+      </c>
+      <c r="H42" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="12" t="s">
@@ -2656,27 +2645,27 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>191</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H43" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H43" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J43" s="23" t="s">
+      <c r="J43" s="21" t="s">
         <v>107</v>
       </c>
       <c r="K43">
@@ -2691,13 +2680,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>191</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>79</v>
@@ -2706,15 +2695,15 @@
         <v>10</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H44" s="28" t="b">
+        <v>153</v>
+      </c>
+      <c r="H44" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="21" t="s">
         <v>107</v>
       </c>
       <c r="K44">
@@ -2729,10 +2718,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -2741,9 +2730,9 @@
         <v>83</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H45" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H45" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="12" t="s">
@@ -2764,10 +2753,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -2779,9 +2768,9 @@
         <v>14</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H46" s="28" t="b">
+        <v>155</v>
+      </c>
+      <c r="H46" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="12" t="s">
@@ -2802,10 +2791,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>191</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
@@ -2814,9 +2803,9 @@
         <v>93</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H47" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H47" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="12" t="s">
@@ -2837,10 +2826,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D48" t="s">
         <v>28</v>
@@ -2849,9 +2838,9 @@
         <v>94</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H48" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H48" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
@@ -2872,10 +2861,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D49" t="s">
         <v>29</v>
@@ -2885,9 +2874,9 @@
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H49" s="28" t="b">
+        <v>155</v>
+      </c>
+      <c r="H49" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
@@ -2910,8 +2899,8 @@
       <c r="B50" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>151</v>
+      <c r="C50" s="20" t="s">
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>33</v>
@@ -2920,22 +2909,22 @@
         <v>98</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H50" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J50" t="s">
         <v>138</v>
-      </c>
-      <c r="J50" t="s">
-        <v>139</v>
       </c>
       <c r="K50">
         <v>2019</v>
       </c>
       <c r="L50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2945,8 +2934,8 @@
       <c r="B51" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="22" t="s">
-        <v>151</v>
+      <c r="C51" s="20" t="s">
+        <v>150</v>
       </c>
       <c r="D51" t="s">
         <v>34</v>
@@ -2958,22 +2947,22 @@
         <v>35</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H51" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H51" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I51" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J51" t="s">
         <v>138</v>
-      </c>
-      <c r="J51" t="s">
-        <v>139</v>
       </c>
       <c r="K51">
         <v>2019</v>
       </c>
       <c r="L51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2983,8 +2972,8 @@
       <c r="B52" t="s">
         <v>32</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>151</v>
+      <c r="C52" s="20" t="s">
+        <v>150</v>
       </c>
       <c r="D52" t="s">
         <v>36</v>
@@ -2993,22 +2982,22 @@
         <v>100</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H52" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H52" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I52" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J52" t="s">
         <v>138</v>
-      </c>
-      <c r="J52" t="s">
-        <v>139</v>
       </c>
       <c r="K52">
         <v>2019</v>
       </c>
       <c r="L52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3018,8 +3007,8 @@
       <c r="B53" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="22" t="s">
-        <v>152</v>
+      <c r="C53" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="D53" t="s">
         <v>37</v>
@@ -3028,22 +3017,22 @@
         <v>101</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H53" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H53" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I53" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J53" t="s">
         <v>138</v>
-      </c>
-      <c r="J53" t="s">
-        <v>139</v>
       </c>
       <c r="K53">
         <v>2019</v>
       </c>
       <c r="L53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3053,8 +3042,8 @@
       <c r="B54" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>152</v>
+      <c r="C54" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="D54" t="s">
         <v>38</v>
@@ -3063,22 +3052,22 @@
         <v>102</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H54" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H54" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I54" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J54" t="s">
         <v>138</v>
-      </c>
-      <c r="J54" t="s">
-        <v>139</v>
       </c>
       <c r="K54">
         <v>2019</v>
       </c>
       <c r="L54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3088,8 +3077,8 @@
       <c r="B55" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>152</v>
+      <c r="C55" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="D55" t="s">
         <v>39</v>
@@ -3098,22 +3087,22 @@
         <v>103</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H55" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H55" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I55" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J55" t="s">
         <v>138</v>
-      </c>
-      <c r="J55" t="s">
-        <v>139</v>
       </c>
       <c r="K55">
         <v>2019</v>
       </c>
       <c r="L55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3123,8 +3112,8 @@
       <c r="B56" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>153</v>
+      <c r="C56" s="20" t="s">
+        <v>152</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3133,22 +3122,22 @@
         <v>82</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H56" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H56" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I56" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J56" t="s">
         <v>138</v>
-      </c>
-      <c r="J56" t="s">
-        <v>139</v>
       </c>
       <c r="K56">
         <v>2019</v>
       </c>
       <c r="L56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -3158,8 +3147,8 @@
       <c r="B57" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>153</v>
+      <c r="C57" s="20" t="s">
+        <v>152</v>
       </c>
       <c r="D57" t="s">
         <v>40</v>
@@ -3168,22 +3157,22 @@
         <v>104</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H57" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H57" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I57" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J57" t="s">
         <v>138</v>
-      </c>
-      <c r="J57" t="s">
-        <v>139</v>
       </c>
       <c r="K57">
         <v>2019</v>
       </c>
       <c r="L57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -3193,8 +3182,8 @@
       <c r="B58" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>153</v>
+      <c r="C58" s="20" t="s">
+        <v>152</v>
       </c>
       <c r="D58" t="s">
         <v>41</v>
@@ -3203,73 +3192,73 @@
         <v>105</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H58" s="28" t="b">
+        <v>158</v>
+      </c>
+      <c r="H58" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I58" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J58" t="s">
         <v>138</v>
-      </c>
-      <c r="J58" t="s">
-        <v>139</v>
       </c>
       <c r="K58">
         <v>2019</v>
       </c>
       <c r="L58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B60" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B61" s="17" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="18" t="s">
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B62" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="19" t="s">
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B63" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="18" t="s">
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B64" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B64" s="18" t="s">
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G66" s="24"/>
-      <c r="H66" s="24"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:L70">
@@ -3425,18 +3414,18 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
         <v>182</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="28" t="b">
+      <c r="H2" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12"/>
@@ -3448,18 +3437,18 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="28" t="b">
+      <c r="H3" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="12"/>
@@ -3469,20 +3458,20 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="28" t="b">
+      <c r="H4" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="12"/>
@@ -3537,7 +3526,7 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="D2" t="s">
@@ -3548,9 +3537,9 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" s="28" t="b">
+        <v>154</v>
+      </c>
+      <c r="H2" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12" t="s">

</xml_diff>

<commit_message>
UPDATE: change menu system
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/common_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA84BF-30B3-FC42-A009-C8A0BE06AD3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="50080" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
     <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
     <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,15 +25,6 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -481,12 +473,6 @@
     <t>Sequences</t>
   </si>
   <si>
-    <t>Structure sites (interface)</t>
-  </si>
-  <si>
-    <t>Mutations (interface)</t>
-  </si>
-  <si>
     <t>Ligand bias</t>
   </si>
   <si>
@@ -550,9 +536,6 @@
     <t>GPCR-G protein interface mutations</t>
   </si>
   <si>
-    <t>GPCR-G protein interactions</t>
-  </si>
-  <si>
     <t>Receptor page</t>
   </si>
   <si>
@@ -653,12 +636,21 @@
   </si>
   <si>
     <t>https://doi.org/10.1093/nar/gkaa1080</t>
+  </si>
+  <si>
+    <t>Structure Comparison</t>
+  </si>
+  <si>
+    <t>GPCR-G protein interactions &amp; profiling</t>
+  </si>
+  <si>
+    <t>Determinants &amp; Mutations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1255,12 +1247,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,22 +1291,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1328,7 +1320,7 @@
         <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>67</v>
@@ -1337,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H2" s="26" t="b">
         <v>0</v>
@@ -1375,7 +1367,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H3" s="26" t="b">
         <v>0</v>
@@ -1404,13 +1396,13 @@
         <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H4" s="26" t="b">
         <v>0</v>
@@ -1439,7 +1431,7 @@
         <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>70</v>
@@ -1448,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H5" s="26" t="b">
         <v>0</v>
@@ -1477,13 +1469,13 @@
         <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H6" s="26" t="b">
         <v>0</v>
@@ -1519,7 +1511,7 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H7" s="26" t="b">
         <v>0</v>
@@ -1548,13 +1540,13 @@
         <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H8" s="26" t="b">
         <v>0</v>
@@ -1583,13 +1575,13 @@
         <v>146</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H9" s="26" t="b">
         <v>0</v>
@@ -1598,13 +1590,13 @@
         <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K9">
         <v>2020</v>
       </c>
       <c r="L9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1615,16 +1607,16 @@
         <v>19</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H10" s="26" t="b">
         <v>0</v>
@@ -1650,16 +1642,16 @@
         <v>19</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H11" s="26" t="b">
         <v>0</v>
@@ -1685,10 +1677,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>79</v>
@@ -1697,7 +1689,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H12" s="26" t="b">
         <v>0</v>
@@ -1735,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H13" s="26" t="b">
         <v>0</v>
@@ -1770,7 +1762,7 @@
         <v>75</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H14" s="26" t="b">
         <v>1</v>
@@ -1779,7 +1771,7 @@
         <v>108</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K14">
         <v>2020</v>
@@ -1802,7 +1794,7 @@
         <v>76</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H15" s="27" t="b">
         <v>0</v>
@@ -1817,7 +1809,7 @@
         <v>2017</v>
       </c>
       <c r="L15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1831,13 +1823,13 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="H16" s="27" t="b">
         <v>0</v>
@@ -1846,13 +1838,13 @@
         <v>108</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K16">
         <v>2020</v>
       </c>
       <c r="L16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1872,7 +1864,7 @@
         <v>77</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H17" s="26" t="b">
         <v>0</v>
@@ -1901,13 +1893,13 @@
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H18" s="26" t="b">
         <v>0</v>
@@ -1942,7 +1934,7 @@
         <v>85</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H19" s="26" t="b">
         <v>0</v>
@@ -1977,7 +1969,7 @@
         <v>86</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H20" s="26" t="b">
         <v>0</v>
@@ -2012,7 +2004,7 @@
         <v>87</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H21" s="26" t="b">
         <v>0</v>
@@ -2047,7 +2039,7 @@
         <v>88</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H22" s="26" t="b">
         <v>0</v>
@@ -2076,7 +2068,7 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>89</v>
@@ -2131,7 +2123,7 @@
         <v>90</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H25" s="26" t="b">
         <v>0</v>
@@ -2163,7 +2155,7 @@
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="26" t="b">
@@ -2205,10 +2197,10 @@
         <v>48</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>52</v>
@@ -2229,16 +2221,16 @@
         <v>48</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>148</v>
+        <v>204</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H29" s="26" t="b">
         <v>0</v>
@@ -2261,7 +2253,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>145</v>
@@ -2285,7 +2277,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>146</v>
@@ -2322,7 +2314,7 @@
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H32" s="26" t="b">
         <v>0</v>
@@ -2348,7 +2340,7 @@
         <v>59</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -2372,7 +2364,7 @@
         <v>59</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
         <v>62</v>
@@ -2396,13 +2388,13 @@
         <v>59</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="26" t="b">
@@ -2441,19 +2433,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H37" s="26" t="b">
         <v>0</v>
@@ -2473,19 +2465,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>96</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H38" s="26" t="b">
         <v>0</v>
@@ -2505,7 +2497,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>30</v>
@@ -2517,7 +2509,7 @@
         <v>95</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H39" s="26" t="b">
         <v>0</v>
@@ -2537,7 +2529,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>22</v>
@@ -2549,7 +2541,7 @@
         <v>91</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H40" s="26" t="b">
         <v>0</v>
@@ -2572,7 +2564,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>22</v>
@@ -2584,7 +2576,7 @@
         <v>92</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H41" s="26" t="b">
         <v>0</v>
@@ -2607,10 +2599,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="20" t="s">
         <v>190</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>193</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -2622,7 +2614,7 @@
         <v>26</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H42" s="26" t="b">
         <v>0</v>
@@ -2645,19 +2637,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>193</v>
-      </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H43" s="26" t="b">
         <v>0</v>
@@ -2680,13 +2672,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>193</v>
-      </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>79</v>
@@ -2695,7 +2687,7 @@
         <v>10</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H44" s="26" t="b">
         <v>0</v>
@@ -2718,10 +2710,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -2730,7 +2722,7 @@
         <v>83</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H45" s="26" t="b">
         <v>0</v>
@@ -2753,10 +2745,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -2768,7 +2760,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H46" s="26" t="b">
         <v>0</v>
@@ -2791,10 +2783,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
@@ -2803,7 +2795,7 @@
         <v>93</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H47" s="26" t="b">
         <v>0</v>
@@ -2826,10 +2818,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D48" t="s">
         <v>28</v>
@@ -2838,7 +2830,7 @@
         <v>94</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H48" s="26" t="b">
         <v>0</v>
@@ -2861,10 +2853,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
         <v>29</v>
@@ -2874,7 +2866,7 @@
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H49" s="26" t="b">
         <v>0</v>
@@ -2900,7 +2892,7 @@
         <v>32</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D50" t="s">
         <v>33</v>
@@ -2909,7 +2901,7 @@
         <v>98</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H50" s="26" t="b">
         <v>0</v>
@@ -2935,7 +2927,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D51" t="s">
         <v>34</v>
@@ -2947,7 +2939,7 @@
         <v>35</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H51" s="26" t="b">
         <v>0</v>
@@ -2973,7 +2965,7 @@
         <v>32</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D52" t="s">
         <v>36</v>
@@ -2982,7 +2974,7 @@
         <v>100</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H52" s="26" t="b">
         <v>0</v>
@@ -3008,7 +3000,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D53" t="s">
         <v>37</v>
@@ -3017,7 +3009,7 @@
         <v>101</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H53" s="26" t="b">
         <v>0</v>
@@ -3043,7 +3035,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D54" t="s">
         <v>38</v>
@@ -3052,7 +3044,7 @@
         <v>102</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H54" s="26" t="b">
         <v>0</v>
@@ -3078,7 +3070,7 @@
         <v>32</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
         <v>39</v>
@@ -3087,7 +3079,7 @@
         <v>103</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H55" s="26" t="b">
         <v>0</v>
@@ -3113,7 +3105,7 @@
         <v>32</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3122,7 +3114,7 @@
         <v>82</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H56" s="26" t="b">
         <v>0</v>
@@ -3148,7 +3140,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D57" t="s">
         <v>40</v>
@@ -3157,7 +3149,7 @@
         <v>104</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H57" s="26" t="b">
         <v>0</v>
@@ -3183,7 +3175,7 @@
         <v>32</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D58" t="s">
         <v>41</v>
@@ -3192,7 +3184,7 @@
         <v>105</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H58" s="26" t="b">
         <v>0</v>
@@ -3261,7 +3253,7 @@
       <c r="H66" s="22"/>
     </row>
   </sheetData>
-  <sortState ref="A2:L70">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L70">
     <sortCondition ref="A2:A70"/>
     <sortCondition ref="I2:I70"/>
     <sortCondition ref="J2:J70"/>
@@ -3291,110 +3283,110 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F44" r:id="rId1"/>
-    <hyperlink ref="F51" r:id="rId2"/>
-    <hyperlink ref="E49" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E28" r:id="rId4"/>
-    <hyperlink ref="E30" r:id="rId5"/>
-    <hyperlink ref="E31" r:id="rId6"/>
-    <hyperlink ref="E33" r:id="rId7"/>
-    <hyperlink ref="E34" r:id="rId8"/>
-    <hyperlink ref="E36" r:id="rId9"/>
-    <hyperlink ref="E3" r:id="rId10"/>
-    <hyperlink ref="E4" r:id="rId11"/>
-    <hyperlink ref="E7" r:id="rId12"/>
-    <hyperlink ref="E5" r:id="rId13"/>
-    <hyperlink ref="E6" r:id="rId14"/>
-    <hyperlink ref="E8" r:id="rId15"/>
-    <hyperlink ref="E10" r:id="rId16"/>
-    <hyperlink ref="E13" r:id="rId17"/>
-    <hyperlink ref="E14" r:id="rId18"/>
-    <hyperlink ref="E15" r:id="rId19"/>
-    <hyperlink ref="E17" r:id="rId20"/>
-    <hyperlink ref="E12" r:id="rId21"/>
-    <hyperlink ref="E11" r:id="rId22"/>
-    <hyperlink ref="E18" r:id="rId23"/>
-    <hyperlink ref="E32" r:id="rId24"/>
-    <hyperlink ref="E46" r:id="rId25"/>
-    <hyperlink ref="E19" r:id="rId26"/>
-    <hyperlink ref="E20" r:id="rId27"/>
-    <hyperlink ref="E21" r:id="rId28"/>
-    <hyperlink ref="E22" r:id="rId29"/>
-    <hyperlink ref="E23" r:id="rId30"/>
-    <hyperlink ref="E24" r:id="rId31"/>
-    <hyperlink ref="E25" r:id="rId32"/>
-    <hyperlink ref="E27" r:id="rId33"/>
-    <hyperlink ref="E40" r:id="rId34"/>
-    <hyperlink ref="E41" r:id="rId35"/>
-    <hyperlink ref="E42" r:id="rId36"/>
-    <hyperlink ref="E44" r:id="rId37"/>
-    <hyperlink ref="E43" r:id="rId38"/>
-    <hyperlink ref="E45" r:id="rId39"/>
-    <hyperlink ref="E47" r:id="rId40"/>
-    <hyperlink ref="E48" r:id="rId41"/>
-    <hyperlink ref="E39" r:id="rId42"/>
-    <hyperlink ref="E38" r:id="rId43"/>
-    <hyperlink ref="E37" r:id="rId44"/>
-    <hyperlink ref="E50" r:id="rId45"/>
-    <hyperlink ref="E51" r:id="rId46"/>
-    <hyperlink ref="E52" r:id="rId47"/>
-    <hyperlink ref="E53" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E54" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E55" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E56" r:id="rId51"/>
-    <hyperlink ref="E57" r:id="rId52"/>
-    <hyperlink ref="E58" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G48" r:id="rId54"/>
-    <hyperlink ref="G47" r:id="rId55"/>
-    <hyperlink ref="G10" r:id="rId56"/>
-    <hyperlink ref="G45" r:id="rId57"/>
-    <hyperlink ref="G8" r:id="rId58"/>
-    <hyperlink ref="G6" r:id="rId59"/>
-    <hyperlink ref="G13" r:id="rId60"/>
-    <hyperlink ref="G3" r:id="rId61"/>
-    <hyperlink ref="G4" r:id="rId62"/>
-    <hyperlink ref="G7" r:id="rId63"/>
-    <hyperlink ref="G32" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G49" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G42" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G46" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G15" r:id="rId68"/>
-    <hyperlink ref="G40" r:id="rId69"/>
-    <hyperlink ref="G41" r:id="rId70"/>
-    <hyperlink ref="G50" r:id="rId71"/>
-    <hyperlink ref="G51" r:id="rId72"/>
-    <hyperlink ref="G52" r:id="rId73"/>
-    <hyperlink ref="G53" r:id="rId74"/>
-    <hyperlink ref="G54" r:id="rId75"/>
-    <hyperlink ref="G55" r:id="rId76"/>
-    <hyperlink ref="G56" r:id="rId77"/>
-    <hyperlink ref="G57" r:id="rId78"/>
-    <hyperlink ref="G58" r:id="rId79"/>
-    <hyperlink ref="G22" r:id="rId80"/>
-    <hyperlink ref="G25" r:id="rId81"/>
-    <hyperlink ref="G29" r:id="rId82"/>
-    <hyperlink ref="G39" r:id="rId83"/>
-    <hyperlink ref="G38" r:id="rId84"/>
-    <hyperlink ref="G37" r:id="rId85"/>
-    <hyperlink ref="G18" r:id="rId86"/>
-    <hyperlink ref="G5" r:id="rId87"/>
-    <hyperlink ref="G12" r:id="rId88"/>
-    <hyperlink ref="G17" r:id="rId89"/>
-    <hyperlink ref="G11" r:id="rId90"/>
-    <hyperlink ref="G44" r:id="rId91"/>
-    <hyperlink ref="G43" r:id="rId92"/>
-    <hyperlink ref="E26" r:id="rId93"/>
-    <hyperlink ref="E35" r:id="rId94"/>
-    <hyperlink ref="E9" r:id="rId95"/>
-    <hyperlink ref="G9" r:id="rId96"/>
-    <hyperlink ref="E16" r:id="rId97"/>
+    <hyperlink ref="F44" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F51" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E49" r:id="rId3" location="mutation-data-submission" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E31" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E33" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E36" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E15" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E17" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E18" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E46" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E20" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E21" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E23" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E24" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E25" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E27" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E44" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E43" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E45" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E47" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E38" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E37" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E50" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E51" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E53" r:id="rId48" location="truncations" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E54" r:id="rId49" location="fusions" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E55" r:id="rId50" location="loopdeletions" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E56" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E57" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E58" r:id="rId53" location="mutations" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G48" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G47" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G10" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G45" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G8" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G6" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="G13" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G3" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G4" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G7" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="G32" r:id="rId64" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="G49" r:id="rId65" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G42" r:id="rId66" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G46" r:id="rId67" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G15" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G40" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G41" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G50" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G51" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G52" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G53" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G54" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G55" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G56" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G57" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G58" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G22" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="G25" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="G29" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="G39" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="G38" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="G37" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="G18" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="G5" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="G12" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="G17" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="G11" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="G44" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="G43" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E26" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E35" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E9" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="G9" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E16" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3415,13 +3407,13 @@
         <v>19</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
@@ -3438,13 +3430,13 @@
         <v>19</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>184</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
@@ -3458,7 +3450,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>43</v>
@@ -3467,7 +3459,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
@@ -3497,16 +3489,16 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3537,7 +3529,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H2" s="26" t="b">
         <v>0</v>
@@ -3565,8 +3557,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: added STE2 Nature paper to references
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="211">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -653,6 +653,24 @@
   </si>
   <si>
     <t>https://doi.org/10.1093/nar/gkaa1080</t>
+  </si>
+  <si>
+    <t>Class D1</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/protein/ste2_yeast/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41586-020-2994-1</t>
+  </si>
+  <si>
+    <t>Structure of the class D GPCR Ste2 dimer coupled to two G proteins</t>
+  </si>
+  <si>
+    <t>Class D1, STE2</t>
+  </si>
+  <si>
+    <t>Class D1 - STE2</t>
   </si>
 </sst>
 </file>
@@ -1256,11 +1274,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,54 +3229,89 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H59" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J59" t="s">
+        <v>208</v>
+      </c>
+      <c r="K59">
+        <v>2020</v>
+      </c>
+      <c r="L59" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="16" t="s">
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B61" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="17" t="s">
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B62" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="18" t="s">
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B63" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G66" s="22"/>
-      <c r="H66" s="22"/>
+      <c r="B66" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:L70">
@@ -3266,7 +3319,7 @@
     <sortCondition ref="I2:I70"/>
     <sortCondition ref="J2:J70"/>
   </sortState>
-  <conditionalFormatting sqref="H51:H1046757 H1:H8 H10:H49">
+  <conditionalFormatting sqref="H51:H1046758 H1:H8 H10:H49">
     <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
@@ -3388,6 +3441,7 @@
     <hyperlink ref="E9" r:id="rId95"/>
     <hyperlink ref="G9" r:id="rId96"/>
     <hyperlink ref="E16" r:id="rId97"/>
+    <hyperlink ref="G59" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FIX: recommiting change after merge issue
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="211">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -653,6 +653,24 @@
   </si>
   <si>
     <t>https://doi.org/10.1093/nar/gkaa1080</t>
+  </si>
+  <si>
+    <t>Class D1</t>
+  </si>
+  <si>
+    <t>Class D1 - STE2</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/protein/ste2_yeast/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41586-020-2994-1</t>
+  </si>
+  <si>
+    <t>Structure of the class D GPCR Ste2 dimer coupled to two G proteins</t>
+  </si>
+  <si>
+    <t>Class D1, STE2</t>
   </si>
 </sst>
 </file>
@@ -854,7 +872,47 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1256,7 +1314,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
@@ -3211,54 +3269,89 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D59" t="s">
+        <v>206</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H59" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K59">
+        <v>2020</v>
+      </c>
+      <c r="L59" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="16" t="s">
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B61" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="17" t="s">
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B62" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="18" t="s">
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B63" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G66" s="22"/>
-      <c r="H66" s="22"/>
+      <c r="B66" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:L70">
@@ -3266,28 +3359,36 @@
     <sortCondition ref="I2:I70"/>
     <sortCondition ref="J2:J70"/>
   </sortState>
-  <conditionalFormatting sqref="H1:H8 H10:H49 H51:H1046757">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="H1:H8 H10:H49 H51:H58 H60:H1046758">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3388,6 +3489,7 @@
     <hyperlink ref="E9" r:id="rId95"/>
     <hyperlink ref="G9" r:id="rId96"/>
     <hyperlink ref="E16" r:id="rId97"/>
+    <hyperlink ref="G59" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3481,18 +3583,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3557,10 +3659,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FIX: depracated arrestin ortholog sequences fixed, citation excel updated
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -196,15 +196,6 @@
     <t>https://gpcrdb.org/ligand/biasedbrowser</t>
   </si>
   <si>
-    <t>Ligand bias for G protein family or arrestin</t>
-  </si>
-  <si>
-    <t>Ligand bias for G protein subtype</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/ligand/biasedgbrowser</t>
-  </si>
-  <si>
     <t>Pathway effects</t>
   </si>
   <si>
@@ -655,9 +646,6 @@
     <t>Sequence signature tool</t>
   </si>
   <si>
-    <t>State stabilizing mutation design tool</t>
-  </si>
-  <si>
     <t>https://gpcrdb.org/mutations/state_stabilizing</t>
   </si>
   <si>
@@ -703,9 +691,6 @@
     <t>https://gpcrdb.org/residue/residuetable_arrestin</t>
   </si>
   <si>
-    <t>Ligand bias statistics</t>
-  </si>
-  <si>
     <t>http://gpcrdb.org/ligand/bias_statistics</t>
   </si>
   <si>
@@ -722,6 +707,21 @@
   </si>
   <si>
     <t>Stabilising mutations</t>
+  </si>
+  <si>
+    <t>Biased ligand statistics</t>
+  </si>
+  <si>
+    <t>Biased ligands (effector family)</t>
+  </si>
+  <si>
+    <t>Biased ligands (subtypes)</t>
+  </si>
+  <si>
+    <t>https://gpcrdb.org/ligand/biasedsubtypesbrowser</t>
+  </si>
+  <si>
+    <t>State stabilizing mutation design</t>
   </si>
 </sst>
 </file>
@@ -922,167 +922,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1627,8 +1467,8 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1649,16 +1489,16 @@
   <sheetData>
     <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1667,22 +1507,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1690,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -1706,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1714,10 +1554,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -1730,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1738,16 +1578,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="25" t="b">
@@ -1755,7 +1595,7 @@
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1763,16 +1603,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="b">
@@ -1780,7 +1620,7 @@
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1791,10 +1631,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -1804,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1815,20 +1655,20 @@
         <v>50</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>225</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1839,20 +1679,20 @@
         <v>50</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1863,20 +1703,20 @@
         <v>50</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1884,28 +1724,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H10" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K10">
         <v>2017</v>
@@ -1916,28 +1756,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H11" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K11">
         <v>2017</v>
@@ -1948,28 +1788,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H12" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K12">
         <v>2017</v>
@@ -1980,34 +1820,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H13" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K13">
         <v>2016</v>
       </c>
       <c r="L13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2015,37 +1855,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H14" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K14">
         <v>2018</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2053,34 +1893,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H15" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K15">
         <v>2016</v>
       </c>
       <c r="L15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2088,34 +1928,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H16" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K16">
         <v>2016</v>
       </c>
       <c r="L16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -2123,10 +1963,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -2136,22 +1976,22 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H17" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K17">
         <v>2019</v>
       </c>
       <c r="L17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2159,37 +1999,37 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>175</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H18" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K18">
         <v>2020</v>
       </c>
       <c r="L18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -2197,34 +2037,34 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>175</v>
-      </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H19" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K19">
         <v>2016</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2232,37 +2072,37 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>175</v>
-      </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H20" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K20">
         <v>2016</v>
       </c>
       <c r="L20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2270,7 +2110,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>19</v>
@@ -2279,25 +2119,25 @@
         <v>20</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H21" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K21">
         <v>2018</v>
       </c>
       <c r="L21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2305,34 +2145,34 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H22" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K22">
         <v>2018</v>
       </c>
       <c r="L22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2343,31 +2183,31 @@
         <v>41</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H23" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K23">
         <v>2017</v>
       </c>
       <c r="L23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2378,13 +2218,13 @@
         <v>41</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="25" t="b">
@@ -2392,7 +2232,7 @@
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2403,13 +2243,13 @@
         <v>41</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="25" t="b">
@@ -2417,7 +2257,7 @@
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2428,13 +2268,13 @@
         <v>41</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="25" t="b">
@@ -2442,7 +2282,7 @@
       </c>
       <c r="I26" s="15"/>
       <c r="J26" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2453,13 +2293,13 @@
         <v>41</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="25" t="b">
@@ -2467,7 +2307,7 @@
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2478,31 +2318,31 @@
         <v>41</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H28" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K28">
         <v>2017</v>
       </c>
       <c r="L28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2513,31 +2353,31 @@
         <v>41</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H29" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K29">
         <v>2017</v>
       </c>
       <c r="L29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2548,13 +2388,13 @@
         <v>41</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="25" t="b">
@@ -2562,7 +2402,7 @@
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -2573,10 +2413,10 @@
         <v>41</v>
       </c>
       <c r="C31" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" t="s">
         <v>193</v>
-      </c>
-      <c r="D31" t="s">
-        <v>196</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>43</v>
@@ -2586,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2603,14 +2443,14 @@
         <v>36</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2634,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2645,31 +2485,31 @@
         <v>18</v>
       </c>
       <c r="C34" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J34" t="s">
         <v>188</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="H34" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J34" t="s">
-        <v>191</v>
       </c>
       <c r="K34">
         <v>2020</v>
       </c>
       <c r="L34" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -2680,32 +2520,32 @@
         <v>18</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H35" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K35">
         <v>2016</v>
       </c>
       <c r="L35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2716,34 +2556,34 @@
         <v>18</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H36" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K36">
         <v>2016</v>
       </c>
       <c r="L36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2754,31 +2594,31 @@
         <v>18</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D37" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H37" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K37">
         <v>2016</v>
       </c>
       <c r="L37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2789,31 +2629,31 @@
         <v>18</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D38" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H38" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K38">
         <v>2016</v>
       </c>
       <c r="L38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2824,34 +2664,34 @@
         <v>18</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D39" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H39" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K39">
         <v>2016</v>
       </c>
       <c r="L39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2862,34 +2702,34 @@
         <v>18</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H40" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K40">
         <v>2014</v>
       </c>
       <c r="L40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2900,31 +2740,31 @@
         <v>18</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H41" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K41">
         <v>2016</v>
       </c>
       <c r="L41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2935,32 +2775,32 @@
         <v>18</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
         <v>0</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H42" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J42" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K42">
         <v>2016</v>
       </c>
       <c r="L42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2971,31 +2811,31 @@
         <v>18</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H43" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K43">
         <v>2016</v>
       </c>
       <c r="L43" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -3006,31 +2846,31 @@
         <v>18</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H44" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K44">
         <v>2016</v>
       </c>
       <c r="L44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -3041,34 +2881,34 @@
         <v>18</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D45" t="s">
         <v>35</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H45" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K45">
         <v>2016</v>
       </c>
       <c r="L45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -3079,31 +2919,31 @@
         <v>18</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H46" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J46" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K46">
         <v>2016</v>
       </c>
       <c r="L46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -3114,31 +2954,31 @@
         <v>18</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H47" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J47" t="s">
         <v>178</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H47" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J47" t="s">
-        <v>181</v>
       </c>
       <c r="K47">
         <v>2020</v>
       </c>
       <c r="L47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -3149,31 +2989,31 @@
         <v>18</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D48" t="s">
         <v>14</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H48" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J48" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K48">
         <v>2018</v>
       </c>
       <c r="L48" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -3184,31 +3024,31 @@
         <v>18</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H49" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J49" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K49">
         <v>2018</v>
       </c>
       <c r="L49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -3219,31 +3059,31 @@
         <v>18</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H50" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K50">
         <v>2018</v>
       </c>
       <c r="L50" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -3254,31 +3094,31 @@
         <v>18</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D51" t="s">
+        <v>192</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H51" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="J51" t="s">
         <v>195</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="H51" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="J51" t="s">
-        <v>198</v>
       </c>
       <c r="K51">
         <v>2021</v>
       </c>
       <c r="L51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3289,31 +3129,31 @@
         <v>18</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D52" t="s">
+        <v>196</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>202</v>
-      </c>
       <c r="H52" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J52" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K52">
         <v>2021</v>
       </c>
       <c r="L52" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3330,28 +3170,28 @@
         <v>6</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H53" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J53" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K53">
         <v>2016</v>
       </c>
       <c r="L53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3368,19 +3208,19 @@
         <v>36</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H54" s="25" t="b">
         <v>1</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K54">
         <v>2020</v>
@@ -3400,25 +3240,25 @@
         <v>37</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H55" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K55">
         <v>2017</v>
       </c>
       <c r="L55" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3432,28 +3272,28 @@
         <v>36</v>
       </c>
       <c r="D56" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="H56" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H56" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="K56">
         <v>2020</v>
       </c>
       <c r="L56" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -3470,25 +3310,25 @@
         <v>8</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H57" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J57" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K57">
         <v>2016</v>
       </c>
       <c r="L57" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -3502,28 +3342,28 @@
         <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H58" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K58">
         <v>2015</v>
       </c>
       <c r="L58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -3534,31 +3374,31 @@
         <v>25</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
         <v>26</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H59" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J59" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K59">
         <v>2019</v>
       </c>
       <c r="L59" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3569,34 +3409,34 @@
         <v>25</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H60" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J60" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K60">
         <v>2019</v>
       </c>
       <c r="L60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -3607,31 +3447,31 @@
         <v>25</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
         <v>29</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H61" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J61" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K61">
         <v>2019</v>
       </c>
       <c r="L61" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3642,31 +3482,31 @@
         <v>25</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D62" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H62" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J62" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K62">
         <v>2019</v>
       </c>
       <c r="L62" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -3677,31 +3517,31 @@
         <v>25</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s">
         <v>33</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H63" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J63" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K63">
         <v>2019</v>
       </c>
       <c r="L63" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -3712,31 +3552,31 @@
         <v>25</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D64" t="s">
         <v>34</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H64" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J64" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K64">
         <v>2019</v>
       </c>
       <c r="L64" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3747,31 +3587,31 @@
         <v>25</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D65" t="s">
         <v>30</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H65" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J65" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K65">
         <v>2019</v>
       </c>
       <c r="L65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -3782,31 +3622,31 @@
         <v>25</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
         <v>31</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H66" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K66">
         <v>2019</v>
       </c>
       <c r="L66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3817,31 +3657,31 @@
         <v>25</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
         <v>32</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H67" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K67">
         <v>2019</v>
       </c>
       <c r="L67" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3870,32 +3710,32 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B75" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B76" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B77" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B78" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B80" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3904,82 +3744,82 @@
     <sortCondition ref="C2:C61"/>
   </sortState>
   <conditionalFormatting sqref="H1:H3 H12:H23 H57:H64 H68:H1046764 H39:H55 H28:H29 H31:H37 H25:H26 H6:H10">
-    <cfRule type="containsText" dxfId="31" priority="19" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="20" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="containsText" dxfId="29" priority="17" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="18" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65:H67">
-    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="containsText" dxfId="23" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4120,13 +3960,13 @@
         <v>18</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
@@ -4143,13 +3983,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>169</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
@@ -4163,7 +4003,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>36</v>
@@ -4172,7 +4012,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
@@ -4181,23 +4021,23 @@
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4232,40 +4072,40 @@
         <v>18</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H2" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K2">
         <v>2016</v>
       </c>
       <c r="L2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
UPDATE: new alignment and structures
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -721,7 +721,7 @@
     <t>https://gpcrdb.org/ligand/biasedsubtypesbrowser</t>
   </si>
   <si>
-    <t>State stabilizing mutation design</t>
+    <t>State-affecting mutation design</t>
   </si>
 </sst>
 </file>
@@ -1467,8 +1467,8 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
UPDATE: site reference update
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="236">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -163,30 +163,12 @@
     <t>G protein page</t>
   </si>
   <si>
-    <t>G Proteins</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/structure/complex_models</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/signprot/matrix</t>
-  </si>
-  <si>
     <t>http://files.gpcrdb.org/GPCR-Gprotein_Mutations.xlsx</t>
   </si>
   <si>
     <t>Arrestin page</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/arrestin</t>
-  </si>
-  <si>
-    <t>Arrestin alignments</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/alignment/arrestinselection</t>
-  </si>
-  <si>
     <t>Arrestin structures</t>
   </si>
   <si>
@@ -268,15 +250,6 @@
     <t>https://gpcrdb.org/mutational_landscape/economicburden</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/signprot/couplings</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/alignment/gproteinselection</t>
-  </si>
-  <si>
     <t>https://gpcrdb.org/ligand/statistics</t>
   </si>
   <si>
@@ -499,9 +472,6 @@
     <t>Default reference</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/structure/g_protein_structure_browser</t>
-  </si>
-  <si>
     <t>Receptor page</t>
   </si>
   <si>
@@ -655,18 +625,12 @@
     <t>G protein selectivity Venn</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/statistics_venn</t>
-  </si>
-  <si>
     <t>G protein coupling</t>
   </si>
   <si>
     <t>G protein selectivity tree</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/statistics_tree</t>
-  </si>
-  <si>
     <t>https://gpcrdb.org/residue/residuetable_gprot</t>
   </si>
   <si>
@@ -676,21 +640,12 @@
     <t>Coupling determinant mutation design</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/mutations/gprot_coupling</t>
-  </si>
-  <si>
     <t>Arrestin coupling</t>
   </si>
   <si>
     <t>Arrestin couplings</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/signprot/arrestincouplings</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/residue/residuetable_arrestin</t>
-  </si>
-  <si>
     <t>http://gpcrdb.org/ligand/bias_statistics</t>
   </si>
   <si>
@@ -722,6 +677,75 @@
   </si>
   <si>
     <t>State-affecting mutation design</t>
+  </si>
+  <si>
+    <t>ArrestinDb</t>
+  </si>
+  <si>
+    <t>GproteinDb</t>
+  </si>
+  <si>
+    <t>GPCRdb</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/signprot/arrestin</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/alignment/arrestinselection</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/signprot/arrestincouplings</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/residue/residuetable_arrestin</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/mutations/gprot_coupling</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/signprot/couplings</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/signprot/statistics_venn</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/signprot/statistics_tree</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/alignment/gproteinselection</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/signprot/matrix</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/structure/g_protein_structure_browser</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/structure/complex_models</t>
+  </si>
+  <si>
+    <t>Arrestin selectivity Venn</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/signprot/arrestin_venn</t>
+  </si>
+  <si>
+    <t>https://arrestindb.org/signprot/arrestin_tree</t>
+  </si>
+  <si>
+    <t>Arrestin selectivity tree</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/structure/gprot_statistics</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>The G protein database, GproteinDb</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/signprot/gprotein</t>
   </si>
 </sst>
 </file>
@@ -922,7 +946,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1464,11 +1508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,16 +1533,16 @@
   <sheetData>
     <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1507,22 +1551,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1530,23 +1574,23 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1554,23 +1598,23 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>48</v>
+        <v>217</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1578,16 +1622,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>145</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="25" t="b">
@@ -1595,7 +1639,7 @@
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1603,16 +1647,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="b">
@@ -1620,7 +1664,7 @@
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1628,23 +1672,24 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>51</v>
+        <v>229</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="25" t="b">
         <v>0</v>
       </c>
+      <c r="I6" s="15"/>
       <c r="J6" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1652,23 +1697,24 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="25" t="b">
         <v>0</v>
       </c>
+      <c r="I7" s="15"/>
       <c r="J7" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1676,23 +1722,23 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1700,23 +1746,23 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>53</v>
+        <v>211</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1724,31 +1770,23 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>145</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J10" t="s">
-        <v>115</v>
-      </c>
-      <c r="K10">
-        <v>2017</v>
+      <c r="J10" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1756,31 +1794,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>218</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>46</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>145</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J11" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11">
-        <v>2017</v>
+      <c r="J11" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1788,28 +1818,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>160</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H12" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K12">
         <v>2017</v>
@@ -1820,34 +1850,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>161</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H13" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>100</v>
+      <c r="I13" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="K13">
-        <v>2016</v>
-      </c>
-      <c r="L13" t="s">
-        <v>101</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1855,37 +1882,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H14" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>108</v>
+      <c r="I14" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="J14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K14">
-        <v>2018</v>
-      </c>
-      <c r="L14" t="s">
-        <v>109</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1893,34 +1914,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H15" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K15">
         <v>2016</v>
       </c>
       <c r="L15" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1928,34 +1949,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>219</v>
+        <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H16" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16">
+        <v>2018</v>
+      </c>
+      <c r="L16" t="s">
         <v>100</v>
-      </c>
-      <c r="J16" t="s">
-        <v>99</v>
-      </c>
-      <c r="K16">
-        <v>2016</v>
-      </c>
-      <c r="L16" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1963,35 +1987,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>72</v>
+      </c>
       <c r="G17" s="5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H17" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="J17" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="K17">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="L17" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1999,37 +2022,34 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>204</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H18" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="K18">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L18" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -2037,34 +2057,35 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>68</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H19" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="J19" t="s">
+        <v>98</v>
       </c>
       <c r="K19">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L19" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2072,37 +2093,37 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H20" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="J20" t="s">
+        <v>98</v>
       </c>
       <c r="K20">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="L20" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2110,34 +2131,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="H21" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="K21">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L21" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2145,34 +2166,37 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>80</v>
+        <v>61</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="H22" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="K22">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L22" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2180,34 +2204,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H23" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="15" t="s">
-        <v>113</v>
+      <c r="I23" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="J23" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="K23">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L23" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2215,24 +2239,34 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="H24" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="13" t="s">
-        <v>121</v>
+      <c r="I24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24">
+        <v>2018</v>
+      </c>
+      <c r="L24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2240,24 +2274,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D25" t="s">
-        <v>203</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="H25" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="13" t="s">
-        <v>121</v>
+      <c r="I25" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" t="s">
+        <v>103</v>
+      </c>
+      <c r="K25">
+        <v>2017</v>
+      </c>
+      <c r="L25" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2265,24 +2309,29 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="13" t="s">
-        <v>121</v>
+      <c r="H26" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K26">
+        <v>2021</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2290,24 +2339,29 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="13" t="s">
-        <v>121</v>
+      <c r="I27" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K27">
+        <v>2021</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2315,34 +2369,29 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>144</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" t="s">
-        <v>112</v>
+      <c r="I28" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="K28">
-        <v>2017</v>
-      </c>
-      <c r="L28" t="s">
-        <v>114</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2350,34 +2399,29 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>144</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J29" t="s">
-        <v>112</v>
+      <c r="I29" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="K29">
-        <v>2017</v>
-      </c>
-      <c r="L29" t="s">
-        <v>114</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2385,24 +2429,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>235</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="H30" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="13" t="s">
-        <v>121</v>
+      <c r="I30" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" t="s">
+        <v>103</v>
+      </c>
+      <c r="K30">
+        <v>2017</v>
+      </c>
+      <c r="L30" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -2410,23 +2464,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="D31" t="s">
-        <v>193</v>
+        <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>224</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="H31" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="13" t="s">
-        <v>121</v>
+      <c r="I31" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31">
+        <v>2017</v>
+      </c>
+      <c r="L31" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2434,23 +2499,29 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>121</v>
+      <c r="I32" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K32">
+        <v>2021</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2458,23 +2529,29 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>183</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>42</v>
+        <v>225</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="J33" s="13" t="s">
-        <v>121</v>
+      <c r="I33" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K33">
+        <v>2021</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2482,34 +2559,29 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>214</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>184</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>36</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>187</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="G34" s="5"/>
       <c r="H34" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J34" t="s">
-        <v>188</v>
+        <v>233</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="K34">
-        <v>2020</v>
-      </c>
-      <c r="L34" t="s">
-        <v>189</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -2517,73 +2589,59 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>214</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="5" t="s">
-        <v>140</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="G35" s="5"/>
       <c r="H35" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="J35" t="s">
-        <v>107</v>
+        <v>233</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="K35">
-        <v>2016</v>
-      </c>
-      <c r="L35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>214</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>132</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>6</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>138</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="G36" s="5"/>
       <c r="H36" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J36" t="s">
-        <v>95</v>
+        <v>233</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="K36">
-        <v>2016</v>
-      </c>
-      <c r="L36" t="s">
-        <v>97</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2591,34 +2649,34 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D37" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>61</v>
+        <v>176</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="H37" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="J37" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="K37">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="L37" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2626,72 +2684,73 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>191</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>227</v>
+        <v>11</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>202</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F38" s="4"/>
       <c r="G38" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H38" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K38">
         <v>2016</v>
       </c>
       <c r="L38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H39" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J39" s="21" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="J39" t="s">
+        <v>86</v>
       </c>
       <c r="K39">
         <v>2016</v>
       </c>
       <c r="L39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2699,37 +2758,34 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H40" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J40" s="21" t="s">
-        <v>122</v>
+        <v>91</v>
+      </c>
+      <c r="J40" t="s">
+        <v>90</v>
       </c>
       <c r="K40">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="L40" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2737,34 +2793,34 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>59</v>
+        <v>192</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H41" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J41" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K41">
         <v>2016</v>
       </c>
       <c r="L41" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2772,35 +2828,37 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="27"/>
+        <v>61</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G42" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H42" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J42" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="K42">
         <v>2016</v>
       </c>
       <c r="L42" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2808,34 +2866,37 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="H43" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="J43" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="K43">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="L43" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2843,34 +2904,34 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H44" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J44" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="J44" t="s">
+        <v>90</v>
       </c>
       <c r="K44">
         <v>2016</v>
       </c>
       <c r="L44" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2878,37 +2939,35 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F45" s="27"/>
       <c r="G45" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H45" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="J45" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K45">
         <v>2016</v>
       </c>
       <c r="L45" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2916,34 +2975,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="D46" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H46" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J46" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K46">
         <v>2016</v>
       </c>
       <c r="L46" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2951,34 +3010,34 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="D47" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="H47" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J47" t="s">
-        <v>178</v>
+        <v>87</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="K47">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L47" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2986,34 +3045,37 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>73</v>
+        <v>50</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H48" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="J48" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="K48">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L48" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -3021,34 +3083,34 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H49" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="J49" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="K49">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L49" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -3056,34 +3118,34 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="H50" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J50" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="K50">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="L50" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -3091,34 +3153,34 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="H51" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="J51" t="s">
-        <v>195</v>
+        <v>101</v>
       </c>
       <c r="K51">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="L51" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3126,34 +3188,34 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>197</v>
+        <v>68</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="H52" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="J52" t="s">
-        <v>195</v>
+        <v>101</v>
       </c>
       <c r="K52">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="L52" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3161,37 +3223,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H53" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J53" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K53">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="L53" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3199,31 +3258,34 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="D54" t="s">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>63</v>
+        <v>184</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H54" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>182</v>
+        <v>188</v>
+      </c>
+      <c r="J54" t="s">
+        <v>185</v>
       </c>
       <c r="K54">
-        <v>2020</v>
+        <v>2021</v>
+      </c>
+      <c r="L54" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3231,34 +3293,34 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H55" s="26" t="b">
+        <v>189</v>
+      </c>
+      <c r="H55" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="J55" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="K55">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="L55" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3266,34 +3328,37 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>179</v>
+        <v>56</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H56" s="26" t="b">
+        <v>130</v>
+      </c>
+      <c r="H56" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>182</v>
+        <v>91</v>
+      </c>
+      <c r="J56" t="s">
+        <v>90</v>
       </c>
       <c r="K56">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L56" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -3301,34 +3366,31 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H57" s="25" t="b">
-        <v>0</v>
+        <v>173</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>215</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J57" s="21" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="K57">
-        <v>2016</v>
-      </c>
-      <c r="L57" t="s">
-        <v>97</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -3336,34 +3398,34 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H58" s="25" t="b">
+        <v>133</v>
+      </c>
+      <c r="H58" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="J58" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="K58">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="L58" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -3371,34 +3433,34 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>215</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H59" s="25" t="b">
+        <v>173</v>
+      </c>
+      <c r="H59" s="26" t="b">
         <v>0</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="J59" t="s">
-        <v>125</v>
+        <v>87</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="K59">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="L59" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3406,37 +3468,34 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>215</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E60" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H60" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H60" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="J60" t="s">
-        <v>125</v>
+      <c r="J60" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="K60">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="L60" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -3444,34 +3503,34 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>215</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="D61" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H61" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="J61" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="K61">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="L61" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3482,31 +3541,31 @@
         <v>25</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D62" t="s">
-        <v>222</v>
+        <v>26</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H62" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J62" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K62">
         <v>2019</v>
       </c>
       <c r="L62" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -3517,31 +3576,34 @@
         <v>25</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D63" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H63" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J63" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K63">
         <v>2019</v>
       </c>
       <c r="L63" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -3552,31 +3614,31 @@
         <v>25</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D64" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H64" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J64" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K64">
         <v>2019</v>
       </c>
       <c r="L64" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3587,31 +3649,31 @@
         <v>25</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D65" t="s">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H65" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J65" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K65">
         <v>2019</v>
       </c>
       <c r="L65" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -3622,31 +3684,31 @@
         <v>25</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H66" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J66" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K66">
         <v>2019</v>
       </c>
       <c r="L66" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3657,85 +3719,190 @@
         <v>25</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D67" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H67" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K67">
         <v>2019</v>
       </c>
       <c r="L67" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" t="s">
+        <v>30</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H68" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J68" t="s">
+        <v>116</v>
+      </c>
+      <c r="K68">
+        <v>2019</v>
+      </c>
+      <c r="L68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69">
+        <v>2019</v>
+      </c>
+      <c r="L69" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G70" s="22"/>
-      <c r="H70" s="22"/>
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H70" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J70" t="s">
+        <v>116</v>
+      </c>
+      <c r="K70">
+        <v>2019</v>
+      </c>
+      <c r="L70" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G71" s="23"/>
       <c r="H71" s="23"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-    </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G74" s="23"/>
       <c r="H74" s="23"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B75" s="18" t="s">
-        <v>128</v>
-      </c>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B76" s="17" t="s">
-        <v>131</v>
-      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B77" s="17" t="s">
-        <v>130</v>
-      </c>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B78" s="17" t="s">
-        <v>129</v>
+      <c r="B78" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B79" s="16" t="s">
-        <v>98</v>
+      <c r="B79" s="17" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B80" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="17" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3743,7 +3910,7 @@
     <sortCondition ref="B2:B61"/>
     <sortCondition ref="C2:C61"/>
   </sortState>
-  <conditionalFormatting sqref="H1:H3 H12:H23 H57:H64 H68:H1046764 H39:H55 H28:H29 H31:H37 H25:H26 H6:H10">
+  <conditionalFormatting sqref="H14:H25 H60:H67 H71:H1046767 H42:H58 H30:H31 H27:H28 H6:H12 H1:H4 H33:H40">
     <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
@@ -3751,188 +3918,183 @@
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H56">
+  <conditionalFormatting sqref="H59">
     <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H13">
     <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65:H67">
+  <conditionalFormatting sqref="H68:H70">
     <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
+  <conditionalFormatting sqref="H41">
     <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H29">
     <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30">
+  <conditionalFormatting sqref="H32">
     <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H30)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H32)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H30)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H26">
     <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",H26)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
-    <hyperlink ref="F60" r:id="rId2"/>
-    <hyperlink ref="E17" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E31" r:id="rId4"/>
+    <hyperlink ref="F22" r:id="rId1"/>
+    <hyperlink ref="F63" r:id="rId2"/>
+    <hyperlink ref="E19" r:id="rId3" location="mutation-data-submission"/>
+    <hyperlink ref="E33" r:id="rId4"/>
     <hyperlink ref="E2" r:id="rId5"/>
     <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E9" r:id="rId9"/>
-    <hyperlink ref="E45" r:id="rId10"/>
-    <hyperlink ref="E46" r:id="rId11"/>
-    <hyperlink ref="E42" r:id="rId12"/>
-    <hyperlink ref="E40" r:id="rId13"/>
-    <hyperlink ref="E41" r:id="rId14"/>
-    <hyperlink ref="E43" r:id="rId15"/>
-    <hyperlink ref="E37" r:id="rId16"/>
-    <hyperlink ref="E53" r:id="rId17"/>
-    <hyperlink ref="E54" r:id="rId18"/>
-    <hyperlink ref="E55" r:id="rId19"/>
-    <hyperlink ref="E57" r:id="rId20"/>
-    <hyperlink ref="E39" r:id="rId21"/>
-    <hyperlink ref="E44" r:id="rId22"/>
-    <hyperlink ref="E58" r:id="rId23"/>
-    <hyperlink ref="E35" r:id="rId24"/>
-    <hyperlink ref="E14" r:id="rId25"/>
-    <hyperlink ref="E48" r:id="rId26"/>
-    <hyperlink ref="E49" r:id="rId27"/>
-    <hyperlink ref="E50" r:id="rId28"/>
-    <hyperlink ref="E28" r:id="rId29"/>
-    <hyperlink ref="E25" r:id="rId30"/>
-    <hyperlink ref="E26" r:id="rId31"/>
-    <hyperlink ref="E29" r:id="rId32"/>
-    <hyperlink ref="E33" r:id="rId33"/>
-    <hyperlink ref="E21" r:id="rId34"/>
-    <hyperlink ref="E22" r:id="rId35"/>
-    <hyperlink ref="E18" r:id="rId36"/>
-    <hyperlink ref="E20" r:id="rId37"/>
-    <hyperlink ref="E19" r:id="rId38"/>
-    <hyperlink ref="E13" r:id="rId39"/>
-    <hyperlink ref="E15" r:id="rId40"/>
-    <hyperlink ref="E16" r:id="rId41"/>
-    <hyperlink ref="E12" r:id="rId42"/>
-    <hyperlink ref="E11" r:id="rId43"/>
-    <hyperlink ref="E10" r:id="rId44"/>
-    <hyperlink ref="E59" r:id="rId45"/>
-    <hyperlink ref="E60" r:id="rId46"/>
-    <hyperlink ref="E61" r:id="rId47"/>
-    <hyperlink ref="E65" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E66" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E67" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E62" r:id="rId51"/>
-    <hyperlink ref="E63" r:id="rId52"/>
-    <hyperlink ref="E64" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G16" r:id="rId54"/>
-    <hyperlink ref="G15" r:id="rId55"/>
-    <hyperlink ref="G37" r:id="rId56"/>
-    <hyperlink ref="G13" r:id="rId57"/>
-    <hyperlink ref="G43" r:id="rId58"/>
-    <hyperlink ref="G41" r:id="rId59"/>
-    <hyperlink ref="G53" r:id="rId60"/>
-    <hyperlink ref="G45" r:id="rId61"/>
-    <hyperlink ref="G46" r:id="rId62"/>
-    <hyperlink ref="G42" r:id="rId63"/>
-    <hyperlink ref="G35" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G17" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G18" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G14" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G55" r:id="rId68"/>
-    <hyperlink ref="G21" r:id="rId69"/>
-    <hyperlink ref="G22" r:id="rId70"/>
-    <hyperlink ref="G59" r:id="rId71"/>
-    <hyperlink ref="G60" r:id="rId72"/>
-    <hyperlink ref="G61" r:id="rId73"/>
-    <hyperlink ref="G65" r:id="rId74"/>
-    <hyperlink ref="G66" r:id="rId75"/>
-    <hyperlink ref="G67" r:id="rId76"/>
-    <hyperlink ref="G62" r:id="rId77"/>
-    <hyperlink ref="G63" r:id="rId78"/>
-    <hyperlink ref="G64" r:id="rId79"/>
-    <hyperlink ref="G28" r:id="rId80"/>
-    <hyperlink ref="G29" r:id="rId81"/>
-    <hyperlink ref="G23" r:id="rId82"/>
-    <hyperlink ref="G12" r:id="rId83"/>
-    <hyperlink ref="G11" r:id="rId84"/>
-    <hyperlink ref="G10" r:id="rId85"/>
-    <hyperlink ref="G58" r:id="rId86"/>
-    <hyperlink ref="G40" r:id="rId87"/>
-    <hyperlink ref="G39" r:id="rId88"/>
-    <hyperlink ref="G57" r:id="rId89"/>
-    <hyperlink ref="G44" r:id="rId90"/>
-    <hyperlink ref="G20" r:id="rId91"/>
-    <hyperlink ref="G19" r:id="rId92"/>
-    <hyperlink ref="E32" r:id="rId93"/>
-    <hyperlink ref="E8" r:id="rId94"/>
-    <hyperlink ref="E47" r:id="rId95"/>
-    <hyperlink ref="G47" r:id="rId96"/>
-    <hyperlink ref="E56" r:id="rId97"/>
-    <hyperlink ref="G34" r:id="rId98"/>
-    <hyperlink ref="E51" r:id="rId99"/>
-    <hyperlink ref="G52" r:id="rId100"/>
-    <hyperlink ref="E52" r:id="rId101"/>
-    <hyperlink ref="G51" r:id="rId102"/>
-    <hyperlink ref="E38" r:id="rId103"/>
-    <hyperlink ref="G38" r:id="rId104"/>
-    <hyperlink ref="E27" r:id="rId105"/>
-    <hyperlink ref="E30" r:id="rId106"/>
-    <hyperlink ref="E24" r:id="rId107"/>
-    <hyperlink ref="E4" r:id="rId108"/>
-    <hyperlink ref="E5" r:id="rId109"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E48" r:id="rId10"/>
+    <hyperlink ref="E49" r:id="rId11"/>
+    <hyperlink ref="E45" r:id="rId12"/>
+    <hyperlink ref="E43" r:id="rId13"/>
+    <hyperlink ref="E44" r:id="rId14"/>
+    <hyperlink ref="E46" r:id="rId15"/>
+    <hyperlink ref="E40" r:id="rId16"/>
+    <hyperlink ref="E56" r:id="rId17"/>
+    <hyperlink ref="E57" r:id="rId18"/>
+    <hyperlink ref="E58" r:id="rId19"/>
+    <hyperlink ref="E60" r:id="rId20"/>
+    <hyperlink ref="E42" r:id="rId21"/>
+    <hyperlink ref="E47" r:id="rId22"/>
+    <hyperlink ref="E61" r:id="rId23"/>
+    <hyperlink ref="E38" r:id="rId24"/>
+    <hyperlink ref="E16" r:id="rId25"/>
+    <hyperlink ref="E51" r:id="rId26"/>
+    <hyperlink ref="E52" r:id="rId27"/>
+    <hyperlink ref="E53" r:id="rId28"/>
+    <hyperlink ref="E30" r:id="rId29"/>
+    <hyperlink ref="E27" r:id="rId30"/>
+    <hyperlink ref="E28" r:id="rId31"/>
+    <hyperlink ref="E31" r:id="rId32"/>
+    <hyperlink ref="E35" r:id="rId33"/>
+    <hyperlink ref="E23" r:id="rId34"/>
+    <hyperlink ref="E24" r:id="rId35"/>
+    <hyperlink ref="E20" r:id="rId36"/>
+    <hyperlink ref="E22" r:id="rId37"/>
+    <hyperlink ref="E21" r:id="rId38"/>
+    <hyperlink ref="E15" r:id="rId39"/>
+    <hyperlink ref="E17" r:id="rId40"/>
+    <hyperlink ref="E18" r:id="rId41"/>
+    <hyperlink ref="E14" r:id="rId42"/>
+    <hyperlink ref="E13" r:id="rId43"/>
+    <hyperlink ref="E12" r:id="rId44"/>
+    <hyperlink ref="E62" r:id="rId45"/>
+    <hyperlink ref="E63" r:id="rId46"/>
+    <hyperlink ref="E64" r:id="rId47"/>
+    <hyperlink ref="E68" r:id="rId48" location="truncations"/>
+    <hyperlink ref="E69" r:id="rId49" location="fusions"/>
+    <hyperlink ref="E70" r:id="rId50" location="loopdeletions"/>
+    <hyperlink ref="E65" r:id="rId51"/>
+    <hyperlink ref="E66" r:id="rId52"/>
+    <hyperlink ref="E67" r:id="rId53" location="mutations"/>
+    <hyperlink ref="G18" r:id="rId54"/>
+    <hyperlink ref="G17" r:id="rId55"/>
+    <hyperlink ref="G40" r:id="rId56"/>
+    <hyperlink ref="G15" r:id="rId57"/>
+    <hyperlink ref="G46" r:id="rId58"/>
+    <hyperlink ref="G44" r:id="rId59"/>
+    <hyperlink ref="G56" r:id="rId60"/>
+    <hyperlink ref="G48" r:id="rId61"/>
+    <hyperlink ref="G49" r:id="rId62"/>
+    <hyperlink ref="G45" r:id="rId63"/>
+    <hyperlink ref="G38" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G19" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G20" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G16" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
+    <hyperlink ref="G58" r:id="rId68"/>
+    <hyperlink ref="G23" r:id="rId69"/>
+    <hyperlink ref="G24" r:id="rId70"/>
+    <hyperlink ref="G62" r:id="rId71"/>
+    <hyperlink ref="G63" r:id="rId72"/>
+    <hyperlink ref="G64" r:id="rId73"/>
+    <hyperlink ref="G68" r:id="rId74"/>
+    <hyperlink ref="G69" r:id="rId75"/>
+    <hyperlink ref="G70" r:id="rId76"/>
+    <hyperlink ref="G65" r:id="rId77"/>
+    <hyperlink ref="G66" r:id="rId78"/>
+    <hyperlink ref="G67" r:id="rId79"/>
+    <hyperlink ref="G30" r:id="rId80"/>
+    <hyperlink ref="G31" r:id="rId81"/>
+    <hyperlink ref="G25" r:id="rId82"/>
+    <hyperlink ref="G14" r:id="rId83"/>
+    <hyperlink ref="G13" r:id="rId84"/>
+    <hyperlink ref="G12" r:id="rId85"/>
+    <hyperlink ref="G61" r:id="rId86"/>
+    <hyperlink ref="G43" r:id="rId87"/>
+    <hyperlink ref="G42" r:id="rId88"/>
+    <hyperlink ref="G60" r:id="rId89"/>
+    <hyperlink ref="G47" r:id="rId90"/>
+    <hyperlink ref="G22" r:id="rId91"/>
+    <hyperlink ref="G21" r:id="rId92"/>
+    <hyperlink ref="E34" r:id="rId93"/>
+    <hyperlink ref="E10" r:id="rId94"/>
+    <hyperlink ref="E50" r:id="rId95"/>
+    <hyperlink ref="G50" r:id="rId96"/>
+    <hyperlink ref="E59" r:id="rId97"/>
+    <hyperlink ref="G37" r:id="rId98"/>
+    <hyperlink ref="E54" r:id="rId99"/>
+    <hyperlink ref="G55" r:id="rId100"/>
+    <hyperlink ref="E55" r:id="rId101"/>
+    <hyperlink ref="G54" r:id="rId102"/>
+    <hyperlink ref="E41" r:id="rId103"/>
+    <hyperlink ref="G41" r:id="rId104"/>
+    <hyperlink ref="E29" r:id="rId105"/>
+    <hyperlink ref="E32" r:id="rId106"/>
+    <hyperlink ref="E26" r:id="rId107"/>
+    <hyperlink ref="E5" r:id="rId108"/>
+    <hyperlink ref="E6" r:id="rId109"/>
+    <hyperlink ref="E7" r:id="rId110"/>
+    <hyperlink ref="E4" r:id="rId111"/>
+    <hyperlink ref="E36" r:id="rId112"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3960,13 +4122,13 @@
         <v>18</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
@@ -3983,13 +4145,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
@@ -4003,16 +4165,16 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
@@ -4021,23 +4183,23 @@
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4072,40 +4234,40 @@
         <v>18</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H2" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K2">
         <v>2016</v>
       </c>
       <c r="L2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FIX: gprotein residue tables URL
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/common_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A28C755-2685-174B-A5C2-3312700CB2BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="32560" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
     <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
     <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,15 +25,6 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -631,9 +623,6 @@
     <t>G protein selectivity tree</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/residue/residuetable_gprot</t>
-  </si>
-  <si>
     <t>Interface mutations &amp; chimeras</t>
   </si>
   <si>
@@ -746,12 +735,15 @@
   </si>
   <si>
     <t>https://gproteindb.org/signprot/gprotein</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org/residue/residuetable_gprot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -946,47 +938,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1507,12 +1459,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="B25:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>123</v>
@@ -1583,7 +1535,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="25" t="b">
@@ -1598,7 +1550,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>124</v>
@@ -1607,7 +1559,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="25" t="b">
@@ -1622,7 +1574,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>124</v>
@@ -1631,7 +1583,7 @@
         <v>145</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="25" t="b">
@@ -1647,16 +1599,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
         <v>200</v>
       </c>
-      <c r="D5" t="s">
-        <v>201</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="b">
@@ -1672,16 +1624,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>229</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="25" t="b">
@@ -1697,16 +1649,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="25" t="b">
@@ -1728,7 +1680,7 @@
         <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>45</v>
@@ -1752,10 +1704,10 @@
         <v>125</v>
       </c>
       <c r="D9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="25" t="b">
@@ -1776,10 +1728,10 @@
         <v>125</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="25" t="b">
@@ -1821,7 +1773,7 @@
         <v>159</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
         <v>160</v>
@@ -1853,7 +1805,7 @@
         <v>159</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13" t="s">
         <v>161</v>
@@ -1885,7 +1837,7 @@
         <v>159</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
@@ -1993,7 +1945,7 @@
         <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>72</v>
@@ -2028,7 +1980,7 @@
         <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>73</v>
@@ -2245,7 +2197,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>71</v>
@@ -2274,13 +2226,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>181</v>
       </c>
       <c r="D25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>41</v>
@@ -2309,26 +2261,26 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>181</v>
       </c>
       <c r="D26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I26" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K26">
         <v>2021</v>
@@ -2339,7 +2291,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>195</v>
@@ -2348,17 +2300,17 @@
         <v>193</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I27" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K27">
         <v>2021</v>
@@ -2369,7 +2321,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>195</v>
@@ -2378,17 +2330,17 @@
         <v>194</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I28" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K28">
         <v>2021</v>
@@ -2399,7 +2351,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>195</v>
@@ -2408,17 +2360,17 @@
         <v>196</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K29">
         <v>2021</v>
@@ -2429,7 +2381,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>123</v>
@@ -2438,7 +2390,7 @@
         <v>40</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>135</v>
@@ -2464,7 +2416,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>124</v>
@@ -2473,7 +2425,7 @@
         <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>135</v>
@@ -2499,7 +2451,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>124</v>
@@ -2508,17 +2460,17 @@
         <v>145</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I32" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K32">
         <v>2021</v>
@@ -2529,7 +2481,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>180</v>
@@ -2538,17 +2490,17 @@
         <v>183</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I33" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K33">
         <v>2021</v>
@@ -2559,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>36</v>
@@ -2568,17 +2520,17 @@
         <v>36</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I34" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K34">
         <v>2021</v>
@@ -2589,7 +2541,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>36</v>
@@ -2598,17 +2550,17 @@
         <v>37</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I35" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K35">
         <v>2021</v>
@@ -2619,7 +2571,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>36</v>
@@ -2628,17 +2580,17 @@
         <v>6</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I36" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="K36">
         <v>2021</v>
@@ -2649,7 +2601,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>174</v>
@@ -2684,7 +2636,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>100</v>
@@ -2720,7 +2672,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>123</v>
@@ -2758,7 +2710,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>181</v>
@@ -2793,13 +2745,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>181</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>192</v>
@@ -2828,7 +2780,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>149</v>
@@ -2866,7 +2818,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>190</v>
@@ -2904,7 +2856,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>190</v>
@@ -2939,7 +2891,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>190</v>
@@ -2975,7 +2927,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>190</v>
@@ -3010,7 +2962,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>190</v>
@@ -3045,7 +2997,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>124</v>
@@ -3083,7 +3035,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>124</v>
@@ -3118,7 +3070,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>124</v>
@@ -3153,7 +3105,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>124</v>
@@ -3188,7 +3140,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>124</v>
@@ -3223,7 +3175,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>124</v>
@@ -3258,7 +3210,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>180</v>
@@ -3293,7 +3245,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>180</v>
@@ -3328,7 +3280,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>36</v>
@@ -3366,7 +3318,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>36</v>
@@ -3381,7 +3333,7 @@
         <v>173</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>87</v>
@@ -3398,7 +3350,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>36</v>
@@ -3433,7 +3385,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>36</v>
@@ -3468,7 +3420,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>36</v>
@@ -3503,7 +3455,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>36</v>
@@ -3652,7 +3604,7 @@
         <v>128</v>
       </c>
       <c r="D65" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>64</v>
@@ -3906,202 +3858,202 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L61">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L61">
     <sortCondition ref="B2:B61"/>
     <sortCondition ref="C2:C61"/>
   </sortState>
   <conditionalFormatting sqref="H14:H25 H60:H67 H71:H1046767 H42:H58 H30:H31 H27:H28 H6:H12 H1:H4 H33:H40">
-    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:H70">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F22" r:id="rId1"/>
-    <hyperlink ref="F63" r:id="rId2"/>
-    <hyperlink ref="E19" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E33" r:id="rId4"/>
-    <hyperlink ref="E2" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E11" r:id="rId9"/>
-    <hyperlink ref="E48" r:id="rId10"/>
-    <hyperlink ref="E49" r:id="rId11"/>
-    <hyperlink ref="E45" r:id="rId12"/>
-    <hyperlink ref="E43" r:id="rId13"/>
-    <hyperlink ref="E44" r:id="rId14"/>
-    <hyperlink ref="E46" r:id="rId15"/>
-    <hyperlink ref="E40" r:id="rId16"/>
-    <hyperlink ref="E56" r:id="rId17"/>
-    <hyperlink ref="E57" r:id="rId18"/>
-    <hyperlink ref="E58" r:id="rId19"/>
-    <hyperlink ref="E60" r:id="rId20"/>
-    <hyperlink ref="E42" r:id="rId21"/>
-    <hyperlink ref="E47" r:id="rId22"/>
-    <hyperlink ref="E61" r:id="rId23"/>
-    <hyperlink ref="E38" r:id="rId24"/>
-    <hyperlink ref="E16" r:id="rId25"/>
-    <hyperlink ref="E51" r:id="rId26"/>
-    <hyperlink ref="E52" r:id="rId27"/>
-    <hyperlink ref="E53" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E27" r:id="rId30"/>
-    <hyperlink ref="E28" r:id="rId31"/>
-    <hyperlink ref="E31" r:id="rId32"/>
-    <hyperlink ref="E35" r:id="rId33"/>
-    <hyperlink ref="E23" r:id="rId34"/>
-    <hyperlink ref="E24" r:id="rId35"/>
-    <hyperlink ref="E20" r:id="rId36"/>
-    <hyperlink ref="E22" r:id="rId37"/>
-    <hyperlink ref="E21" r:id="rId38"/>
-    <hyperlink ref="E15" r:id="rId39"/>
-    <hyperlink ref="E17" r:id="rId40"/>
-    <hyperlink ref="E18" r:id="rId41"/>
-    <hyperlink ref="E14" r:id="rId42"/>
-    <hyperlink ref="E13" r:id="rId43"/>
-    <hyperlink ref="E12" r:id="rId44"/>
-    <hyperlink ref="E62" r:id="rId45"/>
-    <hyperlink ref="E63" r:id="rId46"/>
-    <hyperlink ref="E64" r:id="rId47"/>
-    <hyperlink ref="E68" r:id="rId48" location="truncations"/>
-    <hyperlink ref="E69" r:id="rId49" location="fusions"/>
-    <hyperlink ref="E70" r:id="rId50" location="loopdeletions"/>
-    <hyperlink ref="E65" r:id="rId51"/>
-    <hyperlink ref="E66" r:id="rId52"/>
-    <hyperlink ref="E67" r:id="rId53" location="mutations"/>
-    <hyperlink ref="G18" r:id="rId54"/>
-    <hyperlink ref="G17" r:id="rId55"/>
-    <hyperlink ref="G40" r:id="rId56"/>
-    <hyperlink ref="G15" r:id="rId57"/>
-    <hyperlink ref="G46" r:id="rId58"/>
-    <hyperlink ref="G44" r:id="rId59"/>
-    <hyperlink ref="G56" r:id="rId60"/>
-    <hyperlink ref="G48" r:id="rId61"/>
-    <hyperlink ref="G49" r:id="rId62"/>
-    <hyperlink ref="G45" r:id="rId63"/>
-    <hyperlink ref="G38" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G19" r:id="rId65" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G20" r:id="rId66" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G16" r:id="rId67" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G58" r:id="rId68"/>
-    <hyperlink ref="G23" r:id="rId69"/>
-    <hyperlink ref="G24" r:id="rId70"/>
-    <hyperlink ref="G62" r:id="rId71"/>
-    <hyperlink ref="G63" r:id="rId72"/>
-    <hyperlink ref="G64" r:id="rId73"/>
-    <hyperlink ref="G68" r:id="rId74"/>
-    <hyperlink ref="G69" r:id="rId75"/>
-    <hyperlink ref="G70" r:id="rId76"/>
-    <hyperlink ref="G65" r:id="rId77"/>
-    <hyperlink ref="G66" r:id="rId78"/>
-    <hyperlink ref="G67" r:id="rId79"/>
-    <hyperlink ref="G30" r:id="rId80"/>
-    <hyperlink ref="G31" r:id="rId81"/>
-    <hyperlink ref="G25" r:id="rId82"/>
-    <hyperlink ref="G14" r:id="rId83"/>
-    <hyperlink ref="G13" r:id="rId84"/>
-    <hyperlink ref="G12" r:id="rId85"/>
-    <hyperlink ref="G61" r:id="rId86"/>
-    <hyperlink ref="G43" r:id="rId87"/>
-    <hyperlink ref="G42" r:id="rId88"/>
-    <hyperlink ref="G60" r:id="rId89"/>
-    <hyperlink ref="G47" r:id="rId90"/>
-    <hyperlink ref="G22" r:id="rId91"/>
-    <hyperlink ref="G21" r:id="rId92"/>
-    <hyperlink ref="E34" r:id="rId93"/>
-    <hyperlink ref="E10" r:id="rId94"/>
-    <hyperlink ref="E50" r:id="rId95"/>
-    <hyperlink ref="G50" r:id="rId96"/>
-    <hyperlink ref="E59" r:id="rId97"/>
-    <hyperlink ref="G37" r:id="rId98"/>
-    <hyperlink ref="E54" r:id="rId99"/>
-    <hyperlink ref="G55" r:id="rId100"/>
-    <hyperlink ref="E55" r:id="rId101"/>
-    <hyperlink ref="G54" r:id="rId102"/>
-    <hyperlink ref="E41" r:id="rId103"/>
-    <hyperlink ref="G41" r:id="rId104"/>
-    <hyperlink ref="E29" r:id="rId105"/>
-    <hyperlink ref="E32" r:id="rId106"/>
-    <hyperlink ref="E26" r:id="rId107"/>
-    <hyperlink ref="E5" r:id="rId108"/>
-    <hyperlink ref="E6" r:id="rId109"/>
-    <hyperlink ref="E7" r:id="rId110"/>
-    <hyperlink ref="E4" r:id="rId111"/>
-    <hyperlink ref="E36" r:id="rId112"/>
+    <hyperlink ref="F22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F63" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E19" r:id="rId3" location="mutation-data-submission" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E33" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E48" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E49" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E45" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E43" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E44" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E46" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E56" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E57" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E58" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E60" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E42" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E47" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E61" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E38" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E16" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E51" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E52" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E53" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E31" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E23" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E24" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E20" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E22" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E21" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E15" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E17" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E18" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E14" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E13" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E12" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E62" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E63" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E64" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E68" r:id="rId48" location="truncations" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E69" r:id="rId49" location="fusions" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E70" r:id="rId50" location="loopdeletions" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E65" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E66" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E67" r:id="rId53" location="mutations" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G18" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G17" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G40" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G15" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G46" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G44" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="G56" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G48" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G49" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G45" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="G38" r:id="rId64" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="G19" r:id="rId65" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G20" r:id="rId66" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G16" r:id="rId67" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G58" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G23" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G24" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G62" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G63" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G64" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G68" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G69" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G70" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G65" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G66" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G67" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G30" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="G31" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="G25" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="G14" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="G13" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="G12" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="G61" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="G43" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="G42" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="G60" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="G47" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="G22" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="G21" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E34" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E10" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E50" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="G50" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E59" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="G37" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E54" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="G55" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E55" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="G54" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E41" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="G41" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E29" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="E32" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E26" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="E5" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="E6" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="E7" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E4" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="E36" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4188,32 +4140,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4264,16 +4216,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATED: video links for structure comparison tool
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A28C755-2685-174B-A5C2-3312700CB2BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6A3D48-4334-A34E-B1FA-3B33E9F6BD20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="32560" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="238">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -738,6 +738,12 @@
   </si>
   <si>
     <t>https://gproteindb.org/residue/residuetable_gprot</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X8j_xpryZ4U&amp;start=4880</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X8j_xpryZ4U&amp;start=4490</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1469,8 @@
   <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="B25:E36"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3221,6 +3227,9 @@
       <c r="E54" s="5" t="s">
         <v>184</v>
       </c>
+      <c r="F54" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G54" s="5" t="s">
         <v>189</v>
       </c>
@@ -3255,6 +3264,9 @@
       </c>
       <c r="E55" s="5" t="s">
         <v>187</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>189</v>
@@ -4047,6 +4059,7 @@
     <hyperlink ref="E7" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
     <hyperlink ref="E4" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
     <hyperlink ref="E36" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="F55" r:id="rId113" xr:uid="{F1097C89-7EC1-EA48-BFBF-747C38EAB109}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: BSA site references + guidelines paper
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/common_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C692169E-9326-654D-8B67-BC79068FCFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="32640" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="50240" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
     <sheet name="ToBeAdded" sheetId="3" r:id="rId2"/>
     <sheet name="Deprecated" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="275">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -151,15 +152,9 @@
     <t>Arrestin structures</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/ligand/biasedbrowser</t>
-  </si>
-  <si>
     <t>Pathway effects</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/ligand/biasedpathways</t>
-  </si>
-  <si>
     <t>https://gpcrdb.org/interaction/</t>
   </si>
   <si>
@@ -367,9 +362,6 @@
     <t>An online resource for GPCR structure determination and analysis</t>
   </si>
   <si>
-    <t>Structure determination ressource</t>
-  </si>
-  <si>
     <t>Red text needs to be updated</t>
   </si>
   <si>
@@ -391,9 +383,6 @@
     <t>Sequences</t>
   </si>
   <si>
-    <t>Ligand bias</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1093/nar/gkv1178</t>
   </si>
   <si>
@@ -613,15 +602,6 @@
     <t>Stabilising mutations</t>
   </si>
   <si>
-    <t>Biased ligands (effector family)</t>
-  </si>
-  <si>
-    <t>Biased ligands (subtypes)</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/ligand/biasedsubtypesbrowser</t>
-  </si>
-  <si>
     <t>State-affecting mutation design</t>
   </si>
   <si>
@@ -709,9 +689,6 @@
     <t>Nature Structural &amp; Molecular Biology</t>
   </si>
   <si>
-    <t>LigandBiasDb</t>
-  </si>
-  <si>
     <t>Drugs &amp; Ligands</t>
   </si>
   <si>
@@ -766,28 +743,124 @@
     <t>Ligand pathway profiles (Log(Emax/EC50))</t>
   </si>
   <si>
-    <t>https://gpcrdb.org/biased_signalling/path_preference_statistics</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/biased_signalling/pathwaypreferencebrowser</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/biased_signalling/path_preference_emax_rankorder_selection</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/biased_signalling/path_preference_emax_path_profiles_selection</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
     <t>Manuscript</t>
+  </si>
+  <si>
+    <t>BiasedSignalingAtlas</t>
+  </si>
+  <si>
+    <t>Biased Signaling Atlas</t>
+  </si>
+  <si>
+    <t>Guidelines</t>
+  </si>
+  <si>
+    <t>Community guidelines paper</t>
+  </si>
+  <si>
+    <t>Reference ligand selection</t>
+  </si>
+  <si>
+    <t>Biased ligands (transducer family)</t>
+  </si>
+  <si>
+    <t>Biased ligands (transducer subtype)</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/bias_guidelines</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/reference_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/bias_coverage</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/subtype_coverage</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/biasedbrowser</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/emax_rank_order_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/tau_rank_order_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/emax_path_profiles_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/tau_path_profiles_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/biasedsubtypesbrowser</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/subtype_emax_rank_order_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/subtype_tau_rank_order_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/subtype_emax_path_profiles_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/subtype_tau_path_profiles_selection</t>
+  </si>
+  <si>
+    <t>Biased ligand coverage</t>
+  </si>
+  <si>
+    <t>Biased ligands (∆∆log(Emax/EC50) &amp; ∆∆log(Tau/KA)</t>
+  </si>
+  <si>
+    <t>Ligand bias rank orders (ΔΔlog(Emax/EC50))</t>
+  </si>
+  <si>
+    <t>Ligand bias rank orders (ΔΔlog(Tau/KA))</t>
+  </si>
+  <si>
+    <t>Ligand pathway profiles (Δlog(Emax/EC50))</t>
+  </si>
+  <si>
+    <t>Ligand pathway profiles (Δlog(Tau/KA))</t>
+  </si>
+  <si>
+    <t>Biased ligands (subtype ∆∆log(Emax/EC50) &amp; ∆∆log(Tau/KA)</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/biasedpathways</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/path_preference_coverage</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/pathwaypreferencebrowser</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/path_preference_emax_rankorder_selection</t>
+  </si>
+  <si>
+    <t>https://biasedsignalingatlas.org/biased_signalling/path_preference_emax_path_profiles_selection</t>
+  </si>
+  <si>
+    <t>Community guidelines for GPCR ligand bias: IUPHAR review 32</t>
+  </si>
+  <si>
+    <t>Structure determination resource</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/bph.15811</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -982,127 +1055,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1623,20 +1576,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="67.1640625" customWidth="1"/>
     <col min="5" max="5" width="57.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
     <col min="7" max="7" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1649,16 +1602,16 @@
   <sheetData>
     <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1667,22 +1620,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1690,26 +1643,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="25" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="K2">
         <v>2022</v>
@@ -1720,23 +1673,23 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1744,16 +1697,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="25" t="b">
@@ -1761,7 +1714,7 @@
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1769,16 +1722,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="b">
@@ -1786,7 +1739,7 @@
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1794,16 +1747,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="25" t="b">
@@ -1811,7 +1764,7 @@
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1819,16 +1772,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="25" t="b">
@@ -1836,7 +1789,7 @@
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1844,7 +1797,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>32</v>
@@ -1853,7 +1806,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="25" t="b">
@@ -1861,7 +1814,7 @@
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1869,7 +1822,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>32</v>
@@ -1878,7 +1831,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="25" t="b">
@@ -1886,7 +1839,7 @@
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1894,16 +1847,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="25" t="b">
@@ -1911,7 +1864,7 @@
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1919,23 +1872,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>246</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="H11" s="25" t="b">
         <v>0</v>
       </c>
+      <c r="I11" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="J11" s="13" t="s">
-        <v>107</v>
+        <v>272</v>
+      </c>
+      <c r="K11">
+        <v>2022</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1943,23 +1904,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>196</v>
+        <v>247</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="25" t="b">
-        <v>0</v>
+      <c r="H12" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>237</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="K12">
+        <v>2022</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1967,23 +1934,23 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1991,23 +1958,23 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2015,23 +1982,23 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2039,562 +2006,423 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D16" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>264</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>42</v>
+        <v>253</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="25" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="G19" s="5"/>
       <c r="H19" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J19" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>266</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="G20" s="5"/>
       <c r="H20" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J20" t="s">
-        <v>101</v>
-      </c>
-      <c r="K20">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J20" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>262</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="G21" s="5"/>
       <c r="H21" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J21" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="D22" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>122</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22">
-        <v>2016</v>
-      </c>
-      <c r="L22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J22" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>264</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>123</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" t="s">
-        <v>93</v>
-      </c>
-      <c r="K23">
-        <v>2018</v>
-      </c>
-      <c r="L23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J23" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="D24" t="s">
-        <v>191</v>
+        <v>265</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>122</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J24" t="s">
-        <v>85</v>
-      </c>
-      <c r="K24">
-        <v>2016</v>
-      </c>
-      <c r="L24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J24" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>153</v>
+        <v>233</v>
       </c>
       <c r="D25" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>122</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="G25" s="5"/>
       <c r="H25" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J25" t="s">
-        <v>85</v>
-      </c>
-      <c r="K25">
-        <v>2016</v>
-      </c>
-      <c r="L25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J25" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>153</v>
+        <v>233</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5" t="s">
-        <v>123</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="G26" s="5"/>
       <c r="H26" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" t="s">
-        <v>93</v>
-      </c>
-      <c r="K26">
-        <v>2019</v>
-      </c>
-      <c r="L26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J26" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>235</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>123</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="G27" s="5"/>
       <c r="H27" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="J27" t="s">
-        <v>93</v>
-      </c>
-      <c r="K27">
-        <v>2020</v>
-      </c>
-      <c r="L27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J27" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>121</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K28">
-        <v>2016</v>
-      </c>
-      <c r="L28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J28" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>121</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K29">
-        <v>2016</v>
-      </c>
-      <c r="L29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J29" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>16</v>
+        <v>228</v>
       </c>
       <c r="D30" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="G30" s="5"/>
       <c r="H30" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J30" t="s">
-        <v>88</v>
-      </c>
-      <c r="K30">
-        <v>2018</v>
-      </c>
-      <c r="L30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J30" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>16</v>
+        <v>185</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H31" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>82</v>
+      <c r="I31" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="J31" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="K31">
-        <v>2018</v>
-      </c>
-      <c r="L31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>37</v>
+        <v>147</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H32" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" t="s">
         <v>99</v>
-      </c>
-      <c r="J32" t="s">
-        <v>98</v>
       </c>
       <c r="K32">
         <v>2017</v>
-      </c>
-      <c r="L32" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2602,31 +2430,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>205</v>
+        <v>67</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>218</v>
+        <v>124</v>
+      </c>
+      <c r="H33" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" t="s">
+        <v>99</v>
       </c>
       <c r="K33">
-        <v>2021</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2634,31 +2462,34 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H34" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>218</v>
+      <c r="I34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" t="s">
+        <v>83</v>
       </c>
       <c r="K34">
-        <v>2021</v>
+        <v>2016</v>
+      </c>
+      <c r="L34" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -2666,31 +2497,37 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>207</v>
+        <v>59</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="H35" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>218</v>
+      <c r="I35" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J35" t="s">
+        <v>91</v>
       </c>
       <c r="K35">
-        <v>2021</v>
+        <v>2018</v>
+      </c>
+      <c r="L35" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -2698,31 +2535,34 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>208</v>
+        <v>65</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H36" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>218</v>
+      <c r="I36" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J36" t="s">
+        <v>83</v>
       </c>
       <c r="K36">
-        <v>2021</v>
+        <v>2016</v>
+      </c>
+      <c r="L36" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2730,34 +2570,34 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C37" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="H37" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="J37" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K37">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="L37" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2765,34 +2605,35 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C38" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="H38" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J38" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K38">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="L38" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2800,31 +2641,37 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D39" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="H39" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>218</v>
+      <c r="I39" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J39" t="s">
+        <v>91</v>
       </c>
       <c r="K39">
-        <v>2021</v>
+        <v>2020</v>
+      </c>
+      <c r="L39" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2832,31 +2679,34 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>223</v>
+        <v>117</v>
       </c>
       <c r="H40" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>218</v>
+      <c r="I40" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="K40">
-        <v>2021</v>
+        <v>2016</v>
+      </c>
+      <c r="L40" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2864,31 +2714,37 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>211</v>
+        <v>54</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>223</v>
+        <v>117</v>
       </c>
       <c r="H41" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>218</v>
+      <c r="I41" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="K41">
-        <v>2021</v>
+        <v>2016</v>
+      </c>
+      <c r="L41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2896,31 +2752,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>226</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>212</v>
+        <v>63</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>223</v>
+        <v>121</v>
       </c>
       <c r="H42" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I42" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>218</v>
+      <c r="I42" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" t="s">
+        <v>86</v>
       </c>
       <c r="K42">
-        <v>2021</v>
+        <v>2018</v>
+      </c>
+      <c r="L42" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2928,31 +2787,34 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>188</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>217</v>
+        <v>64</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>223</v>
+        <v>121</v>
       </c>
       <c r="H43" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>218</v>
+      <c r="I43" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J43" t="s">
+        <v>86</v>
       </c>
       <c r="K43">
-        <v>2021</v>
+        <v>2018</v>
+      </c>
+      <c r="L43" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2960,72 +2822,66 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
-        <v>165</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>166</v>
+        <v>181</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="H44" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="12" t="s">
-        <v>99</v>
+      <c r="I44" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="J44" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="K44">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="L44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>3</v>
+        <v>198</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H45" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J45" t="s">
-        <v>81</v>
+        <v>216</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K45">
-        <v>2016</v>
-      </c>
-      <c r="L45" t="s">
-        <v>83</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -3033,34 +2889,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>50</v>
+        <v>199</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>122</v>
+        <v>216</v>
       </c>
       <c r="H46" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J46" t="s">
-        <v>85</v>
+      <c r="I46" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K46">
-        <v>2016</v>
-      </c>
-      <c r="L46" t="s">
-        <v>87</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -3068,34 +2921,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D47" t="s">
-        <v>197</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="G47" s="5" t="s">
-        <v>122</v>
+        <v>216</v>
       </c>
       <c r="H47" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I47" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J47" t="s">
-        <v>85</v>
+      <c r="I47" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K47">
-        <v>2016</v>
-      </c>
-      <c r="L47" t="s">
-        <v>87</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -3103,37 +2953,31 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="H48" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I48" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>108</v>
+      <c r="I48" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K48">
-        <v>2014</v>
-      </c>
-      <c r="L48" t="s">
-        <v>109</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -3141,34 +2985,34 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>48</v>
+        <v>212</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H49" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="J49" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="K49">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="L49" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -3176,35 +3020,34 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="D50" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" s="27"/>
+        <v>202</v>
+      </c>
       <c r="G50" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H50" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="J50" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="K50">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="L50" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -3212,34 +3055,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>122</v>
+        <v>216</v>
       </c>
       <c r="H51" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J51" t="s">
-        <v>85</v>
+      <c r="I51" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K51">
-        <v>2016</v>
-      </c>
-      <c r="L51" t="s">
-        <v>87</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3247,34 +3087,31 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>57</v>
+        <v>203</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="H52" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I52" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>81</v>
+      <c r="I52" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K52">
-        <v>2016</v>
-      </c>
-      <c r="L52" t="s">
-        <v>83</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3282,37 +3119,31 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="H53" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J53" t="s">
-        <v>81</v>
+      <c r="I53" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K53">
-        <v>2016</v>
-      </c>
-      <c r="L53" t="s">
-        <v>83</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3320,34 +3151,31 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>34</v>
+        <v>205</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="H54" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J54" t="s">
-        <v>81</v>
+      <c r="I54" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K54">
-        <v>2016</v>
-      </c>
-      <c r="L54" t="s">
-        <v>83</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3355,34 +3183,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="H55" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="I55" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J55" t="s">
-        <v>158</v>
+      <c r="I55" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K55">
-        <v>2020</v>
-      </c>
-      <c r="L55" t="s">
-        <v>155</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3390,19 +3215,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="D56" t="s">
-        <v>233</v>
+        <v>161</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="H56" s="25" t="b">
         <v>0</v>
@@ -3411,48 +3236,51 @@
         <v>97</v>
       </c>
       <c r="J56" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="K56">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="L56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H57" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="J57" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K57">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L57" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -3460,34 +3288,34 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>175</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H58" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="J58" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="K58">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L58" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -3495,37 +3323,34 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>224</v>
+        <v>118</v>
       </c>
       <c r="H59" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>225</v>
+        <v>84</v>
       </c>
       <c r="J59" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="K59">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="L59" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3533,37 +3358,37 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D60" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>222</v>
+        <v>45</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="H60" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="J60" t="s">
-        <v>175</v>
+        <v>80</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="K60">
-        <v>2021</v>
+        <v>2014</v>
       </c>
       <c r="L60" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -3571,37 +3396,34 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="D61" t="s">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H61" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J61" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K61">
         <v>2016</v>
       </c>
       <c r="L61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3609,31 +3431,35 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F62" s="27"/>
       <c r="G62" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="H62" s="25" t="s">
-        <v>200</v>
+        <v>117</v>
+      </c>
+      <c r="H62" s="25" t="b">
+        <v>0</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>162</v>
+        <v>80</v>
+      </c>
+      <c r="J62" t="s">
+        <v>79</v>
       </c>
       <c r="K62">
-        <v>2020</v>
+        <v>2016</v>
+      </c>
+      <c r="L62" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -3641,34 +3467,34 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="D63" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H63" s="26" t="b">
+        <v>118</v>
+      </c>
+      <c r="H63" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J63" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K63">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="L63" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -3676,34 +3502,34 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="D64" t="s">
-        <v>232</v>
+        <v>137</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="H64" s="26" t="b">
+        <v>117</v>
+      </c>
+      <c r="H64" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>162</v>
+        <v>80</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="K64">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="L64" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3711,34 +3537,37 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H65" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J65" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="J65" t="s">
+        <v>79</v>
       </c>
       <c r="K65">
         <v>2016</v>
       </c>
       <c r="L65" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -3746,34 +3575,34 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="H66" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J66" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="K66">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="L66" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3781,34 +3610,34 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="H67" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="J67" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="K67">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="L67" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3816,37 +3645,34 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>23</v>
+        <v>225</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H68" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="J68" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K68">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L68" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3854,34 +3680,34 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D69" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H69" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="J69" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K69">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L69" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -3889,34 +3715,34 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s">
-        <v>193</v>
+        <v>13</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H70" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="J70" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K70">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L70" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -3924,34 +3750,37 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="D71" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>78</v>
+        <v>170</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="H71" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>110</v>
+        <v>218</v>
       </c>
       <c r="J71" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="K71">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="L71" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -3959,34 +3788,37 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="D72" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>79</v>
+        <v>173</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
       <c r="H72" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>110</v>
+        <v>218</v>
       </c>
       <c r="J72" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="K72">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="L72" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -3994,34 +3826,37 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s">
-        <v>26</v>
+        <v>223</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H73" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="J73" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="K73">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="L73" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
@@ -4029,34 +3864,31 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D74" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H74" s="25" t="b">
-        <v>0</v>
+        <v>159</v>
+      </c>
+      <c r="H74" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="J74" t="s">
-        <v>111</v>
+        <v>80</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="K74">
-        <v>2019</v>
-      </c>
-      <c r="L74" t="s">
-        <v>112</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
@@ -4064,300 +3896,737 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C75" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H75" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J75" t="s">
+        <v>86</v>
+      </c>
+      <c r="K75">
+        <v>2017</v>
+      </c>
+      <c r="L75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>193</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" t="s">
+        <v>224</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H76" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K76">
+        <v>2020</v>
+      </c>
+      <c r="L76" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H77" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J77" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K77">
+        <v>2016</v>
+      </c>
+      <c r="L77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>193</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D78" t="s">
+        <v>139</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H78" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J78" t="s">
+        <v>88</v>
+      </c>
+      <c r="K78">
+        <v>2015</v>
+      </c>
+      <c r="L78" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H79" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J79" t="s">
+        <v>109</v>
+      </c>
+      <c r="K79">
+        <v>2019</v>
+      </c>
+      <c r="L79" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H80" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J80" t="s">
+        <v>109</v>
+      </c>
+      <c r="K80">
+        <v>2019</v>
+      </c>
+      <c r="L80" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>193</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" t="s">
+        <v>25</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H81" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J81" t="s">
+        <v>109</v>
+      </c>
+      <c r="K81">
+        <v>2019</v>
+      </c>
+      <c r="L81" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>193</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" t="s">
+        <v>189</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H82" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J82" t="s">
+        <v>109</v>
+      </c>
+      <c r="K82">
+        <v>2019</v>
+      </c>
+      <c r="L82" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H83" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J83" t="s">
+        <v>109</v>
+      </c>
+      <c r="K83">
+        <v>2019</v>
+      </c>
+      <c r="L83" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H84" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J84" t="s">
+        <v>109</v>
+      </c>
+      <c r="K84">
+        <v>2019</v>
+      </c>
+      <c r="L84" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H85" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J85" t="s">
+        <v>109</v>
+      </c>
+      <c r="K85">
+        <v>2019</v>
+      </c>
+      <c r="L85" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>193</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D86" t="s">
+        <v>27</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H86" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J86" t="s">
+        <v>109</v>
+      </c>
+      <c r="K86">
+        <v>2019</v>
+      </c>
+      <c r="L86" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87" t="s">
         <v>28</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H75" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I75" s="12" t="s">
+      <c r="E87" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H87" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J87" t="s">
+        <v>109</v>
+      </c>
+      <c r="K87">
+        <v>2019</v>
+      </c>
+      <c r="L87" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G90" s="22"/>
+      <c r="H90" s="22"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G93" s="23"/>
+      <c r="H93" s="23"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B95" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B96" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J75" t="s">
-        <v>111</v>
-      </c>
-      <c r="K75">
-        <v>2019</v>
-      </c>
-      <c r="L75" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G78" s="22"/>
-      <c r="H78" s="22"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G79" s="23"/>
-      <c r="H79" s="23"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G80" s="24"/>
-      <c r="H80" s="24"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G81" s="23"/>
-      <c r="H81" s="23"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="17" t="s">
-        <v>113</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L61">
-    <sortCondition ref="B2:B61"/>
-    <sortCondition ref="C2:C61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L73">
+    <sortCondition ref="B2:B73"/>
+    <sortCondition ref="C2:C73"/>
   </sortState>
-  <conditionalFormatting sqref="H21:H32 H65:H72 H76:H1046772 H37:H38 H34:H35 H1:H4 H40:H46 H48:H63 H6:H19">
-    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="H33:H44 H77:H84 H88:H1046784 H49:H50 H46:H47 H1:H4 H52:H58 H60:H75 H6:H31">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H64">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H64)))</formula>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H64)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H76)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H20)))</formula>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H20)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H73:H75">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H73)))</formula>
+  <conditionalFormatting sqref="H85:H87">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H73)))</formula>
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H85)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H47)))</formula>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H47)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H36)))</formula>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H36)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H39)))</formula>
+  <conditionalFormatting sqref="H51">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H39)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H33)))</formula>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H33)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F29" r:id="rId1"/>
-    <hyperlink ref="F68" r:id="rId2"/>
-    <hyperlink ref="E26" r:id="rId3" location="mutation-data-submission"/>
-    <hyperlink ref="E40" r:id="rId4"/>
-    <hyperlink ref="E2" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="E11" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="E17" r:id="rId9"/>
-    <hyperlink ref="E53" r:id="rId10"/>
-    <hyperlink ref="E54" r:id="rId11"/>
-    <hyperlink ref="E50" r:id="rId12"/>
-    <hyperlink ref="E48" r:id="rId13"/>
-    <hyperlink ref="E49" r:id="rId14"/>
-    <hyperlink ref="E51" r:id="rId15"/>
-    <hyperlink ref="E46" r:id="rId16"/>
-    <hyperlink ref="E61" r:id="rId17"/>
-    <hyperlink ref="E62" r:id="rId18"/>
-    <hyperlink ref="E63" r:id="rId19"/>
-    <hyperlink ref="E65" r:id="rId20"/>
-    <hyperlink ref="E52" r:id="rId21"/>
-    <hyperlink ref="E66" r:id="rId22"/>
-    <hyperlink ref="E23" r:id="rId23"/>
-    <hyperlink ref="E56" r:id="rId24"/>
-    <hyperlink ref="E57" r:id="rId25"/>
-    <hyperlink ref="E58" r:id="rId26"/>
-    <hyperlink ref="E37" r:id="rId27"/>
-    <hyperlink ref="E34" r:id="rId28"/>
-    <hyperlink ref="E35" r:id="rId29"/>
-    <hyperlink ref="E38" r:id="rId30"/>
-    <hyperlink ref="E42" r:id="rId31"/>
-    <hyperlink ref="E30" r:id="rId32"/>
-    <hyperlink ref="E31" r:id="rId33"/>
-    <hyperlink ref="E27" r:id="rId34"/>
-    <hyperlink ref="E29" r:id="rId35"/>
-    <hyperlink ref="E28" r:id="rId36"/>
-    <hyperlink ref="E22" r:id="rId37"/>
-    <hyperlink ref="E24" r:id="rId38"/>
-    <hyperlink ref="E25" r:id="rId39"/>
-    <hyperlink ref="E21" r:id="rId40"/>
-    <hyperlink ref="E20" r:id="rId41"/>
-    <hyperlink ref="E19" r:id="rId42"/>
-    <hyperlink ref="E67" r:id="rId43"/>
-    <hyperlink ref="E68" r:id="rId44"/>
-    <hyperlink ref="E69" r:id="rId45"/>
-    <hyperlink ref="E73" r:id="rId46" location="truncations"/>
-    <hyperlink ref="E74" r:id="rId47" location="fusions"/>
-    <hyperlink ref="E75" r:id="rId48" location="loopdeletions"/>
-    <hyperlink ref="E70" r:id="rId49"/>
-    <hyperlink ref="E71" r:id="rId50"/>
-    <hyperlink ref="E72" r:id="rId51" location="mutations"/>
-    <hyperlink ref="G25" r:id="rId52"/>
-    <hyperlink ref="G24" r:id="rId53"/>
-    <hyperlink ref="G46" r:id="rId54"/>
-    <hyperlink ref="G22" r:id="rId55"/>
-    <hyperlink ref="G51" r:id="rId56"/>
-    <hyperlink ref="G49" r:id="rId57"/>
-    <hyperlink ref="G61" r:id="rId58"/>
-    <hyperlink ref="G53" r:id="rId59"/>
-    <hyperlink ref="G54" r:id="rId60"/>
-    <hyperlink ref="G50" r:id="rId61"/>
-    <hyperlink ref="G26" r:id="rId62" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G27" r:id="rId63" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G23" r:id="rId64" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="G63" r:id="rId65"/>
-    <hyperlink ref="G30" r:id="rId66"/>
-    <hyperlink ref="G31" r:id="rId67"/>
-    <hyperlink ref="G67" r:id="rId68"/>
-    <hyperlink ref="G68" r:id="rId69"/>
-    <hyperlink ref="G69" r:id="rId70"/>
-    <hyperlink ref="G73" r:id="rId71"/>
-    <hyperlink ref="G74" r:id="rId72"/>
-    <hyperlink ref="G75" r:id="rId73"/>
-    <hyperlink ref="G70" r:id="rId74"/>
-    <hyperlink ref="G71" r:id="rId75"/>
-    <hyperlink ref="G72" r:id="rId76"/>
-    <hyperlink ref="G37" r:id="rId77"/>
-    <hyperlink ref="G38" r:id="rId78"/>
-    <hyperlink ref="G32" r:id="rId79"/>
-    <hyperlink ref="G21" r:id="rId80"/>
-    <hyperlink ref="G20" r:id="rId81"/>
-    <hyperlink ref="G19" r:id="rId82"/>
-    <hyperlink ref="G66" r:id="rId83"/>
-    <hyperlink ref="G48" r:id="rId84"/>
-    <hyperlink ref="G65" r:id="rId85"/>
-    <hyperlink ref="G52" r:id="rId86"/>
-    <hyperlink ref="G29" r:id="rId87"/>
-    <hyperlink ref="G28" r:id="rId88"/>
-    <hyperlink ref="E41" r:id="rId89"/>
-    <hyperlink ref="E13" r:id="rId90"/>
-    <hyperlink ref="E55" r:id="rId91"/>
-    <hyperlink ref="G55" r:id="rId92"/>
-    <hyperlink ref="E64" r:id="rId93"/>
-    <hyperlink ref="G44" r:id="rId94"/>
-    <hyperlink ref="E59" r:id="rId95"/>
-    <hyperlink ref="E60" r:id="rId96"/>
-    <hyperlink ref="G59" r:id="rId97"/>
-    <hyperlink ref="E47" r:id="rId98"/>
-    <hyperlink ref="G47" r:id="rId99"/>
-    <hyperlink ref="E36" r:id="rId100"/>
-    <hyperlink ref="E39" r:id="rId101"/>
-    <hyperlink ref="E33" r:id="rId102"/>
-    <hyperlink ref="E5" r:id="rId103"/>
-    <hyperlink ref="E6" r:id="rId104"/>
-    <hyperlink ref="E7" r:id="rId105"/>
-    <hyperlink ref="E4" r:id="rId106"/>
-    <hyperlink ref="E43" r:id="rId107"/>
-    <hyperlink ref="F60" r:id="rId108"/>
-    <hyperlink ref="G33" r:id="rId109"/>
-    <hyperlink ref="G34" r:id="rId110"/>
-    <hyperlink ref="G35" r:id="rId111"/>
-    <hyperlink ref="G36" r:id="rId112"/>
-    <hyperlink ref="G39" r:id="rId113"/>
-    <hyperlink ref="G40" r:id="rId114"/>
-    <hyperlink ref="G41" r:id="rId115"/>
-    <hyperlink ref="G42" r:id="rId116"/>
-    <hyperlink ref="G43" r:id="rId117"/>
-    <hyperlink ref="G60" r:id="rId118"/>
-    <hyperlink ref="E8" r:id="rId119"/>
-    <hyperlink ref="E9" r:id="rId120"/>
-    <hyperlink ref="E10" r:id="rId121"/>
-    <hyperlink ref="E18" r:id="rId122"/>
-    <hyperlink ref="E14" r:id="rId123"/>
-    <hyperlink ref="E15" r:id="rId124"/>
-    <hyperlink ref="E16" r:id="rId125"/>
+    <hyperlink ref="F41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F80" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E38" r:id="rId3" location="mutation-data-submission" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E52" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E65" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E66" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E62" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E60" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E61" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E63" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E58" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E73" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E74" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E75" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E77" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E64" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E78" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E35" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E68" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E69" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E70" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E49" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E46" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E47" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E50" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E54" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E39" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E41" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E40" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E34" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E33" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E31" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E79" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E80" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E81" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E85" r:id="rId45" location="truncations" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E86" r:id="rId46" location="fusions" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E87" r:id="rId47" location="loopdeletions" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E82" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E83" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E84" r:id="rId50" location="mutations" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="G37" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G36" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G34" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G61" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G73" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G65" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="G66" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G38" r:id="rId61" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G39" r:id="rId62" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="G35" r:id="rId63" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="G75" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G43" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G79" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G80" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G81" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G85" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G86" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G87" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G82" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G83" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G84" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G49" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G50" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G44" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G33" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="G32" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="G31" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="G78" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="G60" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="G77" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="G64" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="G41" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="G40" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E53" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="E67" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="G67" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E76" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="G56" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E71" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E72" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="G71" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="E59" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="G59" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="E48" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E51" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="E45" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E5" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="E6" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E7" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="E4" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E55" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="F72" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="G45" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="G46" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="G47" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="G48" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="G51" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="G52" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="G53" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="G54" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="G55" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="G72" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="E8" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="E9" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="E10" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="E30" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="E12" r:id="rId121" xr:uid="{974BCAB2-C4FF-8148-8DE5-AA154B75976E}"/>
+    <hyperlink ref="E13" r:id="rId122" xr:uid="{84150DFC-2346-5340-BDFD-A2CAB875D051}"/>
+    <hyperlink ref="E25:E28" r:id="rId123" display="https://biasedsignalingatlas.org/biased_signalling/" xr:uid="{51A19721-B728-AE44-8F4A-FA7109C56E4F}"/>
+    <hyperlink ref="E19" r:id="rId124" xr:uid="{D3C15512-5481-A743-83D2-6387CB2DF6C6}"/>
+    <hyperlink ref="E14" r:id="rId125" xr:uid="{3C43702F-EDAF-3F44-8EF4-06E317D71579}"/>
+    <hyperlink ref="E15" r:id="rId126" xr:uid="{62C2AEF1-60EB-5E4F-AAB4-79C304167D00}"/>
+    <hyperlink ref="E16" r:id="rId127" xr:uid="{233EB1B3-079B-A443-96AB-99BCABB14F5D}"/>
+    <hyperlink ref="E17" r:id="rId128" xr:uid="{071921C9-D9A2-E64B-880E-4D8D01F6D8F0}"/>
+    <hyperlink ref="E18" r:id="rId129" xr:uid="{B6EA8645-C2D7-9144-963F-504BDA309FA1}"/>
+    <hyperlink ref="E20" r:id="rId130" xr:uid="{D146FC13-3761-FC4E-A230-D2CC5054345B}"/>
+    <hyperlink ref="E21" r:id="rId131" xr:uid="{5688CC30-A4FC-C94A-9119-A0093F4D17D3}"/>
+    <hyperlink ref="E22" r:id="rId132" xr:uid="{1BC67574-F75C-B349-A956-1F4F3511C494}"/>
+    <hyperlink ref="E23" r:id="rId133" xr:uid="{459BE4A2-DC08-034E-995C-21C3BF77CB99}"/>
+    <hyperlink ref="E24" r:id="rId134" xr:uid="{560E66B9-0459-2C4B-9844-6E4B9D3BB65E}"/>
+    <hyperlink ref="E25" r:id="rId135" xr:uid="{C2BC09EA-19D8-8248-86C6-CCD53AFCDD04}"/>
+    <hyperlink ref="E26" r:id="rId136" xr:uid="{14D0D5FB-1FF3-DC4A-A77A-8FDE52FE0431}"/>
+    <hyperlink ref="E27" r:id="rId137" xr:uid="{5FEA330B-345C-3245-BB38-94D5F78D8E68}"/>
+    <hyperlink ref="E28" r:id="rId138" xr:uid="{CFF0BC74-01A6-5D4C-A2BB-E67867FBBAD3}"/>
+    <hyperlink ref="G11" r:id="rId139" xr:uid="{20511033-0478-5747-89EE-796E471A6251}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4378,13 +4647,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
@@ -4401,13 +4670,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
@@ -4421,7 +4690,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>32</v>
@@ -4430,7 +4699,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
@@ -4439,37 +4708,37 @@
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4490,46 +4759,46 @@
         <v>15</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H2" s="25" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K2">
         <v>2016</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FIX: ArrestinDb manuscript publication data
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5245EC05-10BB-CB43-8DC0-9B3F9E429F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C47F9624-7492-4846-A0D8-DA3C7F54B440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="-23580" windowWidth="34560" windowHeight="20620" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="436">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -1417,12 +1417,15 @@
   <si>
     <t>https://doi.org/10.1038/s41589-023-01292-8</t>
   </si>
+  <si>
+    <t>The arrestin database, ArrestinDb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1679,14 +1682,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1756,7 +1751,7 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1843,7 +1838,6 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -2256,7 +2250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z96"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P64" sqref="P64"/>
     </sheetView>
@@ -6973,7 +6967,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7030,9 +7024,11 @@
       <c r="D2" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="55" t="s">
         <v>179</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>435</v>
       </c>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
@@ -8201,7 +8197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59E4EFC-2B59-5D40-B259-109EE9277003}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -8223,7 +8219,7 @@
       <c r="C1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="64" t="s">
         <v>431</v>
       </c>
       <c r="E1" s="20">

</xml_diff>

<commit_message>
FIX: several issues in Site_References.xlsx
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{858745F5-D0BF-704A-8969-A978586F7C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A319E3B-EAF6-F74B-950D-7A7165C8F883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="536">
   <si>
     <t>Phylogenetic trees</t>
   </si>
@@ -862,9 +862,6 @@
   </si>
   <si>
     <t>https://gpcrdb.org/protein/*</t>
-  </si>
-  <si>
-    <t>https://gpcrdb.org/familiy/*</t>
   </si>
   <si>
     <t>Data maper</t>
@@ -1717,12 +1714,18 @@
   <si>
     <t>http://files.gpcrdb.org/GPCR-Gprotein_Mutations.xlsx</t>
   </si>
+  <si>
+    <t>https://gpcrdb.org/family/*</t>
+  </si>
+  <si>
+    <t>The arrestin database, ArrestinDb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1979,14 +1982,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2056,7 +2051,7 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2143,11 +2138,9 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2155,27 +2148,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2579,9 +2552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2656,51 +2629,51 @@
         <v>118</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q1" s="56" t="s">
+        <v>368</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="Q1" s="56" t="s">
-        <v>369</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="45"/>
       <c r="E2" s="14"/>
       <c r="F2" t="s">
+        <v>402</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -2727,7 +2700,7 @@
         <v>181</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -2742,7 +2715,7 @@
     </row>
     <row r="4" spans="1:25" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B4" t="s">
         <v>181</v>
@@ -2754,7 +2727,7 @@
         <v>181</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -2769,7 +2742,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B5" s="45" t="s">
         <v>164</v>
@@ -2779,10 +2752,10 @@
       </c>
       <c r="D5" s="45"/>
       <c r="F5" t="s">
+        <v>413</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -2795,7 +2768,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>164</v>
@@ -2805,10 +2778,10 @@
       </c>
       <c r="D6" s="45"/>
       <c r="F6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -2821,22 +2794,22 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B7" s="45" t="s">
         <v>164</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D7" s="45" t="s">
         <v>419</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="F7" t="s">
         <v>420</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -2849,22 +2822,22 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B8" s="45" t="s">
         <v>164</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>423</v>
+      </c>
+      <c r="F8" t="s">
         <v>424</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
@@ -2877,22 +2850,22 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B9" s="45" t="s">
         <v>164</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F9" t="s">
+        <v>427</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -2905,7 +2878,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>164</v>
@@ -2920,7 +2893,7 @@
         <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -2948,7 +2921,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -2976,7 +2949,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
@@ -2989,7 +2962,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B13" s="45" t="s">
         <v>164</v>
@@ -3004,7 +2977,7 @@
         <v>122</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -3017,7 +2990,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14" s="45" t="s">
         <v>164</v>
@@ -3032,7 +3005,7 @@
         <v>122</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -3045,7 +3018,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B15" s="45" t="s">
         <v>164</v>
@@ -3060,7 +3033,7 @@
         <v>174</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
@@ -3073,7 +3046,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B16" s="45" t="s">
         <v>164</v>
@@ -3088,7 +3061,7 @@
         <v>31</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -3101,7 +3074,7 @@
     </row>
     <row r="17" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>164</v>
@@ -3114,10 +3087,10 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="39" t="s">
+        <v>441</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>442</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>443</v>
       </c>
       <c r="H17" s="39" t="b">
         <v>1</v>
@@ -3130,7 +3103,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>164</v>
@@ -3139,13 +3112,13 @@
         <v>149</v>
       </c>
       <c r="D18" s="45" t="s">
+        <v>444</v>
+      </c>
+      <c r="F18" t="s">
         <v>445</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>447</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -3194,19 +3167,19 @@
         <v>79</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Q19" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S19">
         <v>2025</v>
       </c>
       <c r="T19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -3250,13 +3223,13 @@
         <v>79</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q20" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S20">
         <v>2023</v>
@@ -3264,7 +3237,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B21" s="45"/>
       <c r="D21" s="45"/>
@@ -3294,25 +3267,25 @@
         <v>79</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S21">
         <v>2023</v>
       </c>
       <c r="U21" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="W21" t="s">
         <v>395</v>
-      </c>
-      <c r="V21" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="W21" t="s">
-        <v>396</v>
       </c>
       <c r="X21">
         <v>2025</v>
@@ -3320,7 +3293,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B22" s="45" t="s">
         <v>173</v>
@@ -3359,13 +3332,13 @@
         <v>79</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S22">
         <v>2023</v>
@@ -3412,13 +3385,13 @@
         <v>79</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q23" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S23">
         <v>2023</v>
@@ -3447,7 +3420,7 @@
         <v>247</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>166</v>
@@ -3456,18 +3429,18 @@
         <v>72</v>
       </c>
       <c r="M24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N24">
         <v>2025</v>
       </c>
       <c r="O24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B25" s="45" t="s">
         <v>173</v>
@@ -3488,7 +3461,7 @@
         <v>243</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>166</v>
@@ -3497,13 +3470,13 @@
         <v>72</v>
       </c>
       <c r="M25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N25">
         <v>2025</v>
       </c>
       <c r="O25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -3524,7 +3497,7 @@
         <v>189</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>166</v>
@@ -3533,13 +3506,13 @@
         <v>72</v>
       </c>
       <c r="M26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N26">
         <v>2025</v>
       </c>
       <c r="O26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -3580,13 +3553,13 @@
         <v>2017</v>
       </c>
       <c r="P27" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R27" t="s">
         <v>395</v>
-      </c>
-      <c r="Q27" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R27" t="s">
-        <v>396</v>
       </c>
       <c r="S27">
         <v>2025</v>
@@ -3630,13 +3603,13 @@
         <v>2017</v>
       </c>
       <c r="P28" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R28" t="s">
         <v>395</v>
-      </c>
-      <c r="Q28" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R28" t="s">
-        <v>396</v>
       </c>
       <c r="S28">
         <v>2025</v>
@@ -3680,13 +3653,13 @@
         <v>2017</v>
       </c>
       <c r="P29" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q29" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R29" t="s">
         <v>395</v>
-      </c>
-      <c r="Q29" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R29" t="s">
-        <v>396</v>
       </c>
       <c r="S29">
         <v>2025</v>
@@ -3712,7 +3685,7 @@
         <v>253</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>113</v>
@@ -3730,13 +3703,13 @@
         <v>2017</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R30" t="s">
         <v>395</v>
-      </c>
-      <c r="Q30" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R30" t="s">
-        <v>396</v>
       </c>
       <c r="S30">
         <v>2025</v>
@@ -3744,7 +3717,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>173</v>
@@ -3780,13 +3753,13 @@
         <v>2017</v>
       </c>
       <c r="P31" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q31" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R31" t="s">
         <v>395</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R31" t="s">
-        <v>396</v>
       </c>
       <c r="S31">
         <v>2025</v>
@@ -3830,13 +3803,13 @@
         <v>2017</v>
       </c>
       <c r="P32" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q32" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R32" t="s">
         <v>395</v>
-      </c>
-      <c r="Q32" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R32" t="s">
-        <v>396</v>
       </c>
       <c r="S32">
         <v>2025</v>
@@ -3880,13 +3853,13 @@
         <v>2017</v>
       </c>
       <c r="P33" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q33" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R33" t="s">
         <v>395</v>
-      </c>
-      <c r="Q33" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R33" t="s">
-        <v>396</v>
       </c>
       <c r="S33">
         <v>2025</v>
@@ -3930,13 +3903,13 @@
         <v>2017</v>
       </c>
       <c r="P34" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q34" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="R34" t="s">
         <v>395</v>
-      </c>
-      <c r="Q34" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="R34" t="s">
-        <v>396</v>
       </c>
       <c r="S34">
         <v>2025</v>
@@ -4003,7 +3976,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>173</v>
@@ -4021,7 +3994,7 @@
         <v>16</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -4242,7 +4215,7 @@
         <v>85</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="1" t="s">
@@ -4325,7 +4298,7 @@
         <v>161</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>109</v>
@@ -4389,7 +4362,7 @@
     </row>
     <row r="45" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>173</v>
@@ -4407,7 +4380,7 @@
         <v>160</v>
       </c>
       <c r="G45" s="39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J45" s="39" t="s">
         <v>109</v>
@@ -4431,7 +4404,7 @@
     </row>
     <row r="46" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B46" s="47" t="s">
         <v>173</v>
@@ -4471,7 +4444,7 @@
       </c>
     </row>
     <row r="47" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="68" t="s">
+      <c r="A47" t="s">
         <v>165</v>
       </c>
       <c r="B47" s="45" t="s">
@@ -4484,14 +4457,14 @@
         <v>165</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H47" t="b">
         <v>1</v>
       </c>
       <c r="I47" s="23"/>
       <c r="J47" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K47" s="16" t="s">
         <v>165</v>
@@ -4500,20 +4473,20 @@
         <v>72</v>
       </c>
       <c r="M47" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="N47">
         <v>2024</v>
       </c>
       <c r="O47"/>
       <c r="P47" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q47" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="Q47" s="9" t="s">
+      <c r="R47" t="s">
         <v>401</v>
-      </c>
-      <c r="R47" t="s">
-        <v>402</v>
       </c>
       <c r="S47">
         <v>2022</v>
@@ -4534,17 +4507,17 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B48" s="45" t="s">
         <v>165</v>
       </c>
       <c r="D48" s="45"/>
       <c r="F48" t="s">
+        <v>451</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="H48" t="b">
         <v>1</v>
@@ -4558,22 +4531,22 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D49" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F49" t="s">
+        <v>454</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -4595,17 +4568,17 @@
         <v>165</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D50" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" t="s">
+        <v>456</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="H50" t="b">
         <v>1</v>
@@ -4621,22 +4594,22 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B51" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D51" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F51" t="s">
+        <v>458</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="H51" t="b">
         <v>1</v>
@@ -4652,22 +4625,22 @@
     </row>
     <row r="52" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B52" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D52" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F52" t="s">
+        <v>461</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="H52" t="b">
         <v>1</v>
@@ -4679,22 +4652,22 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B53" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D53" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F53" t="s">
+        <v>463</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="H53" t="b">
         <v>1</v>
@@ -4706,7 +4679,7 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B54" s="45" t="s">
         <v>165</v>
@@ -4721,7 +4694,7 @@
         <v>30</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H54" t="b">
         <v>1</v>
@@ -4733,7 +4706,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B55" s="45" t="s">
         <v>165</v>
@@ -4748,7 +4721,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H55" t="b">
         <v>1</v>
@@ -4760,7 +4733,7 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B56" s="45" t="s">
         <v>165</v>
@@ -4775,7 +4748,7 @@
         <v>30</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H56" t="b">
         <v>1</v>
@@ -4787,7 +4760,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B57" s="45" t="s">
         <v>165</v>
@@ -4802,7 +4775,7 @@
         <v>122</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H57" t="b">
         <v>1</v>
@@ -4814,7 +4787,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B58" s="45" t="s">
         <v>165</v>
@@ -4829,7 +4802,7 @@
         <v>122</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H58" t="b">
         <v>1</v>
@@ -4843,7 +4816,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B59" s="45" t="s">
         <v>165</v>
@@ -4858,7 +4831,7 @@
         <v>174</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H59" t="b">
         <v>1</v>
@@ -4872,7 +4845,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B60" s="45" t="s">
         <v>165</v>
@@ -4887,7 +4860,7 @@
         <v>31</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H60" t="b">
         <v>1</v>
@@ -4901,7 +4874,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B61" s="45" t="s">
         <v>165</v>
@@ -4913,10 +4886,10 @@
         <v>31</v>
       </c>
       <c r="F61" t="s">
+        <v>476</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="H61" t="b">
         <v>1</v>
@@ -4930,7 +4903,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B62" s="45" t="s">
         <v>165</v>
@@ -4942,10 +4915,10 @@
         <v>31</v>
       </c>
       <c r="F62" t="s">
+        <v>479</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>481</v>
       </c>
       <c r="H62" t="b">
         <v>1</v>
@@ -4959,7 +4932,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B63" s="45" t="s">
         <v>165</v>
@@ -4971,10 +4944,10 @@
         <v>31</v>
       </c>
       <c r="F63" t="s">
+        <v>481</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="H63" t="b">
         <v>1</v>
@@ -4986,7 +4959,7 @@
     </row>
     <row r="64" spans="1:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="38" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B64" s="46" t="s">
         <v>165</v>
@@ -4999,10 +4972,10 @@
       </c>
       <c r="E64" s="40"/>
       <c r="F64" s="39" t="s">
-        <v>482</v>
-      </c>
-      <c r="G64" s="66" t="s">
-        <v>496</v>
+        <v>481</v>
+      </c>
+      <c r="G64" s="65" t="s">
+        <v>495</v>
       </c>
       <c r="H64" s="39" t="b">
         <v>1</v>
@@ -5015,22 +4988,22 @@
     </row>
     <row r="65" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B65" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C65" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>484</v>
+      </c>
+      <c r="F65" t="s">
         <v>485</v>
       </c>
-      <c r="D65" s="45" t="s">
-        <v>485</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="G65" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>487</v>
       </c>
       <c r="H65" t="b">
         <v>1</v>
@@ -5048,16 +5021,16 @@
         <v>165</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F66" t="s">
         <v>7</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H66" t="b">
         <v>1</v>
@@ -5069,22 +5042,22 @@
     </row>
     <row r="67" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B67" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D67" s="45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F67" t="s">
         <v>7</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H67" t="b">
         <v>1</v>
@@ -5096,22 +5069,22 @@
     </row>
     <row r="68" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B68" s="45" t="s">
         <v>165</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D68" s="45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F68" t="s">
         <v>7</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H68" t="b">
         <v>1</v>
@@ -5123,7 +5096,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B69" s="45" t="s">
         <v>165</v>
@@ -5135,10 +5108,10 @@
         <v>150</v>
       </c>
       <c r="F69" t="s">
+        <v>492</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="H69" t="b">
         <v>1</v>
@@ -5150,7 +5123,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B70" s="45" t="s">
         <v>165</v>
@@ -5162,10 +5135,10 @@
         <v>150</v>
       </c>
       <c r="F70" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H70" t="b">
         <v>1</v>
@@ -5176,8 +5149,8 @@
       </c>
     </row>
     <row r="71" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="67" t="s">
-        <v>328</v>
+      <c r="A71" s="66" t="s">
+        <v>327</v>
       </c>
       <c r="B71" s="47" t="s">
         <v>165</v>
@@ -5190,10 +5163,10 @@
       </c>
       <c r="E71" s="21"/>
       <c r="F71" s="20" t="s">
+        <v>532</v>
+      </c>
+      <c r="G71" s="22" t="s">
         <v>533</v>
-      </c>
-      <c r="G71" s="22" t="s">
-        <v>534</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>170</v>
@@ -5219,7 +5192,7 @@
     </row>
     <row r="72" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B72" s="45" t="s">
         <v>166</v>
@@ -5256,24 +5229,24 @@
         <v>73</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q72" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R72" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S72">
         <v>2014</v>
       </c>
       <c r="T72" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="73" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B73" s="45" t="s">
         <v>166</v>
@@ -5311,34 +5284,34 @@
         <v>73</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q73" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R73" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S73">
         <v>2014</v>
       </c>
       <c r="T73" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="27" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B74" s="45" t="s">
         <v>166</v>
       </c>
       <c r="D74" s="45"/>
       <c r="F74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>272</v>
+        <v>534</v>
       </c>
       <c r="H74" t="b">
         <v>1</v>
@@ -5363,41 +5336,41 @@
         <v>73</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q74" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R74" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S74">
         <v>2014</v>
       </c>
       <c r="T74" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="75" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B75" s="45" t="s">
         <v>166</v>
       </c>
       <c r="D75" s="45"/>
       <c r="E75" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="F75" t="s">
         <v>273</v>
       </c>
-      <c r="F75" t="s">
-        <v>274</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K75" s="16" t="s">
         <v>166</v>
@@ -5406,34 +5379,34 @@
         <v>72</v>
       </c>
       <c r="M75" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N75">
         <v>2025</v>
       </c>
       <c r="O75" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B76" s="45" t="s">
         <v>166</v>
       </c>
       <c r="D76" s="45"/>
       <c r="E76" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F76" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K76" s="16" t="s">
         <v>166</v>
@@ -5442,34 +5415,34 @@
         <v>72</v>
       </c>
       <c r="M76" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N76">
         <v>2025</v>
       </c>
       <c r="O76" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="27" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B77" s="45" t="s">
         <v>166</v>
       </c>
       <c r="D77" s="45"/>
       <c r="E77" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H77" t="b">
         <v>1</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K77" s="16" t="s">
         <v>166</v>
@@ -5478,18 +5451,18 @@
         <v>72</v>
       </c>
       <c r="M77" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N77">
         <v>2025</v>
       </c>
       <c r="O77" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B78" s="45" t="s">
         <v>166</v>
@@ -5529,7 +5502,7 @@
         <v>73</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q78" s="9" t="s">
         <v>72</v>
@@ -5541,12 +5514,12 @@
         <v>2021</v>
       </c>
       <c r="T78" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B79" s="45" t="s">
         <v>166</v>
@@ -5561,7 +5534,7 @@
         <v>30</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -5584,7 +5557,7 @@
         <v>73</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q79" s="9" t="s">
         <v>72</v>
@@ -5596,12 +5569,12 @@
         <v>2021</v>
       </c>
       <c r="T79" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B80" s="45" t="s">
         <v>166</v>
@@ -5616,7 +5589,7 @@
         <v>30</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H80" t="b">
         <v>1</v>
@@ -5641,7 +5614,7 @@
         <v>73</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q80" s="9" t="s">
         <v>72</v>
@@ -5653,12 +5626,12 @@
         <v>2021</v>
       </c>
       <c r="T80" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B81" s="45" t="s">
         <v>166</v>
@@ -5695,13 +5668,13 @@
         <v>73</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q81" s="9" t="s">
         <v>81</v>
       </c>
       <c r="R81" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S81">
         <v>2015</v>
@@ -5712,7 +5685,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B82" s="45" t="s">
         <v>166</v>
@@ -5727,7 +5700,7 @@
         <v>122</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="2"/>
@@ -5750,13 +5723,13 @@
         <v>73</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q82" s="9" t="s">
         <v>81</v>
       </c>
       <c r="R82" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S82">
         <v>2015</v>
@@ -5767,7 +5740,7 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B83" s="45" t="s">
         <v>166</v>
@@ -5806,7 +5779,7 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B84" s="45" t="s">
         <v>166</v>
@@ -5815,10 +5788,10 @@
         <v>156</v>
       </c>
       <c r="D84" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F84" t="s">
         <v>123</v>
@@ -5855,7 +5828,7 @@
         <v>76</v>
       </c>
       <c r="R84" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S84">
         <v>2016</v>
@@ -5882,7 +5855,7 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B85" s="45" t="s">
         <v>166</v>
@@ -5891,16 +5864,16 @@
         <v>156</v>
       </c>
       <c r="D85" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F85" t="s">
         <v>123</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="2"/>
@@ -5929,7 +5902,7 @@
         <v>76</v>
       </c>
       <c r="R85" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S85">
         <v>2016</v>
@@ -5940,7 +5913,7 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B86" s="45" t="s">
         <v>166</v>
@@ -5949,16 +5922,16 @@
         <v>156</v>
       </c>
       <c r="D86" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F86" t="s">
         <v>123</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="2"/>
@@ -5987,7 +5960,7 @@
         <v>76</v>
       </c>
       <c r="R86" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S86">
         <v>2016</v>
@@ -5998,7 +5971,7 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B87" s="45" t="s">
         <v>166</v>
@@ -6007,16 +5980,16 @@
         <v>156</v>
       </c>
       <c r="D87" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F87" t="s">
         <v>123</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="2"/>
@@ -6045,7 +6018,7 @@
         <v>76</v>
       </c>
       <c r="R87" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S87">
         <v>2016</v>
@@ -6056,7 +6029,7 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B88" s="45" t="s">
         <v>166</v>
@@ -6065,10 +6038,10 @@
         <v>156</v>
       </c>
       <c r="D88" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F88" t="s">
         <v>124</v>
@@ -6102,7 +6075,7 @@
         <v>76</v>
       </c>
       <c r="R88" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S88">
         <v>2016</v>
@@ -6113,7 +6086,7 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B89" s="45" t="s">
         <v>166</v>
@@ -6122,16 +6095,16 @@
         <v>156</v>
       </c>
       <c r="D89" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F89" t="s">
         <v>124</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H89" s="1"/>
       <c r="J89" s="1" t="s">
@@ -6159,7 +6132,7 @@
         <v>76</v>
       </c>
       <c r="R89" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S89">
         <v>2016</v>
@@ -6170,7 +6143,7 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B90" s="45" t="s">
         <v>166</v>
@@ -6179,10 +6152,10 @@
         <v>156</v>
       </c>
       <c r="D90" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F90" t="s">
         <v>0</v>
@@ -6216,7 +6189,7 @@
         <v>76</v>
       </c>
       <c r="R90" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S90">
         <v>2016</v>
@@ -6227,7 +6200,7 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B91" s="45" t="s">
         <v>166</v>
@@ -6236,16 +6209,16 @@
         <v>156</v>
       </c>
       <c r="D91" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F91" t="s">
         <v>0</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H91" s="1"/>
       <c r="J91" s="1" t="s">
@@ -6273,7 +6246,7 @@
         <v>76</v>
       </c>
       <c r="R91" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S91">
         <v>2016</v>
@@ -6284,7 +6257,7 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B92" s="45" t="s">
         <v>166</v>
@@ -6293,10 +6266,10 @@
         <v>156</v>
       </c>
       <c r="D92" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F92" t="s">
         <v>125</v>
@@ -6330,7 +6303,7 @@
         <v>76</v>
       </c>
       <c r="R92" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S92">
         <v>2016</v>
@@ -6341,7 +6314,7 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B93" s="45" t="s">
         <v>166</v>
@@ -6350,16 +6323,16 @@
         <v>156</v>
       </c>
       <c r="D93" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F93" t="s">
         <v>125</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H93" s="1"/>
       <c r="J93" s="1" t="s">
@@ -6387,7 +6360,7 @@
         <v>76</v>
       </c>
       <c r="R93" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S93">
         <v>2016</v>
@@ -6398,7 +6371,7 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B94" s="45" t="s">
         <v>166</v>
@@ -6407,16 +6380,16 @@
         <v>156</v>
       </c>
       <c r="D94" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F94" t="s">
         <v>125</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H94" s="1"/>
       <c r="J94" s="1" t="s">
@@ -6444,7 +6417,7 @@
         <v>76</v>
       </c>
       <c r="R94" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S94">
         <v>2016</v>
@@ -6455,7 +6428,7 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B95" s="45" t="s">
         <v>166</v>
@@ -6464,7 +6437,7 @@
         <v>156</v>
       </c>
       <c r="D95" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F95" t="s">
         <v>126</v>
@@ -6494,7 +6467,7 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B96" s="45" t="s">
         <v>166</v>
@@ -6503,13 +6476,13 @@
         <v>156</v>
       </c>
       <c r="D96" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F96" t="s">
         <v>126</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>107</v>
@@ -6532,7 +6505,7 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B97" s="45" t="s">
         <v>166</v>
@@ -6541,13 +6514,13 @@
         <v>156</v>
       </c>
       <c r="D97" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F97" t="s">
         <v>126</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>107</v>
@@ -6570,7 +6543,7 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B98" s="45" t="s">
         <v>166</v>
@@ -6612,7 +6585,7 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B99" s="45" t="s">
         <v>166</v>
@@ -6646,27 +6619,27 @@
         <v>2021</v>
       </c>
       <c r="O99" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q99" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R99" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S99">
         <v>2014</v>
       </c>
       <c r="T99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B100" s="45" t="s">
         <v>166</v>
@@ -6678,10 +6651,10 @@
         <v>31</v>
       </c>
       <c r="F100" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H100" s="1"/>
       <c r="J100" s="1" t="s">
@@ -6700,27 +6673,27 @@
         <v>2021</v>
       </c>
       <c r="O100" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P100" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q100" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R100" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S100">
         <v>2014</v>
       </c>
       <c r="T100" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B101" s="45" t="s">
         <v>166</v>
@@ -6732,10 +6705,10 @@
         <v>31</v>
       </c>
       <c r="F101" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H101" s="1"/>
       <c r="J101" s="1" t="s">
@@ -6754,27 +6727,27 @@
         <v>2021</v>
       </c>
       <c r="O101" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q101" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R101" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S101">
         <v>2014</v>
       </c>
       <c r="T101" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B102" s="45" t="s">
         <v>166</v>
@@ -6786,10 +6759,10 @@
         <v>31</v>
       </c>
       <c r="F102" t="s">
+        <v>309</v>
+      </c>
+      <c r="G102" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="H102" s="1"/>
       <c r="J102" s="1" t="s">
@@ -6808,27 +6781,27 @@
         <v>2021</v>
       </c>
       <c r="O102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q102" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R102" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S102">
         <v>2014</v>
       </c>
       <c r="T102" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B103" s="45" t="s">
         <v>166</v>
@@ -6840,10 +6813,10 @@
         <v>31</v>
       </c>
       <c r="F103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H103" s="1"/>
       <c r="J103" s="1" t="s">
@@ -6862,22 +6835,22 @@
         <v>2021</v>
       </c>
       <c r="O103" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q103" s="9" t="s">
         <v>72</v>
       </c>
       <c r="R103" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S103">
         <v>2014</v>
       </c>
       <c r="T103" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="U103" s="1" t="s">
         <v>107</v>
@@ -6900,7 +6873,7 @@
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B104" s="45" t="s">
         <v>166</v>
@@ -6912,14 +6885,14 @@
         <v>31</v>
       </c>
       <c r="F104" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H104" s="1"/>
       <c r="J104" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K104" s="16" t="s">
         <v>166</v>
@@ -6928,7 +6901,7 @@
         <v>72</v>
       </c>
       <c r="M104" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N104">
         <v>2023</v>
@@ -6936,7 +6909,7 @@
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B105" s="45" t="s">
         <v>166</v>
@@ -6948,14 +6921,14 @@
         <v>31</v>
       </c>
       <c r="F105" t="s">
+        <v>301</v>
+      </c>
+      <c r="G105" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="H105" s="1"/>
       <c r="J105" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K105" s="16" t="s">
         <v>166</v>
@@ -6964,18 +6937,18 @@
         <v>72</v>
       </c>
       <c r="M105" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N105">
         <v>2025</v>
       </c>
       <c r="O105" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B106" s="45" t="s">
         <v>166</v>
@@ -6984,7 +6957,7 @@
         <v>149</v>
       </c>
       <c r="D106" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F106" t="s">
         <v>151</v>
@@ -7017,7 +6990,7 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B107" s="45" t="s">
         <v>166</v>
@@ -7026,7 +6999,7 @@
         <v>149</v>
       </c>
       <c r="D107" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F107" t="s">
         <v>154</v>
@@ -7059,7 +7032,7 @@
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B108" s="45" t="s">
         <v>166</v>
@@ -7068,7 +7041,7 @@
         <v>149</v>
       </c>
       <c r="D108" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
@@ -7098,7 +7071,7 @@
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B109" s="45" t="s">
         <v>166</v>
@@ -7107,13 +7080,13 @@
         <v>149</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F109" t="s">
         <v>7</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H109" s="1"/>
       <c r="J109" s="1" t="s">
@@ -7137,7 +7110,7 @@
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="27" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B110" s="45" t="s">
         <v>166</v>
@@ -7146,13 +7119,13 @@
         <v>149</v>
       </c>
       <c r="D110" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F110" t="s">
         <v>7</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H110" s="1"/>
       <c r="J110" s="1" t="s">
@@ -7176,7 +7149,7 @@
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B111" s="45" t="s">
         <v>166</v>
@@ -7185,13 +7158,13 @@
         <v>149</v>
       </c>
       <c r="D111" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F111" t="s">
+        <v>321</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>107</v>
@@ -7214,7 +7187,7 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B112" s="45" t="s">
         <v>166</v>
@@ -7223,7 +7196,7 @@
         <v>149</v>
       </c>
       <c r="D112" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F112" t="s">
         <v>128</v>
@@ -7267,7 +7240,7 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B113" s="45" t="s">
         <v>166</v>
@@ -7276,13 +7249,13 @@
         <v>149</v>
       </c>
       <c r="D113" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F113" t="s">
         <v>128</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J113" s="1" t="s">
         <v>107</v>
@@ -7305,7 +7278,7 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B114" s="45" t="s">
         <v>166</v>
@@ -7314,13 +7287,13 @@
         <v>149</v>
       </c>
       <c r="D114" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F114" t="s">
         <v>128</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J114" s="1" t="s">
         <v>107</v>
@@ -7343,7 +7316,7 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B115" s="45" t="s">
         <v>166</v>
@@ -7355,7 +7328,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F115" t="s">
         <v>21</v>
@@ -7384,7 +7357,7 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B116" s="45" t="s">
         <v>166</v>
@@ -7396,7 +7369,7 @@
         <v>20</v>
       </c>
       <c r="E116" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F116" t="s">
         <v>22</v>
@@ -7428,7 +7401,7 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B117" s="45" t="s">
         <v>166</v>
@@ -7440,13 +7413,13 @@
         <v>20</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F117" t="s">
         <v>22</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1" t="s">
@@ -7470,7 +7443,7 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B118" s="45" t="s">
         <v>166</v>
@@ -7482,7 +7455,7 @@
         <v>20</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F118" t="s">
         <v>24</v>
@@ -7511,7 +7484,7 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B119" s="45" t="s">
         <v>166</v>
@@ -7523,7 +7496,7 @@
         <v>20</v>
       </c>
       <c r="E119" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F119" t="s">
         <v>25</v>
@@ -7555,7 +7528,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B120" s="45" t="s">
         <v>166</v>
@@ -7567,7 +7540,7 @@
         <v>20</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F120" t="s">
         <v>26</v>
@@ -7599,7 +7572,7 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B121" s="45" t="s">
         <v>166</v>
@@ -7611,7 +7584,7 @@
         <v>20</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F121" t="s">
         <v>27</v>
@@ -7643,7 +7616,7 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B122" s="45" t="s">
         <v>166</v>
@@ -7655,7 +7628,7 @@
         <v>20</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F122" t="s">
         <v>163</v>
@@ -7684,7 +7657,7 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B123" s="45" t="s">
         <v>166</v>
@@ -7696,7 +7669,7 @@
         <v>20</v>
       </c>
       <c r="E123" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F123" t="s">
         <v>28</v>
@@ -7725,7 +7698,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B124" s="45" t="s">
         <v>166</v>
@@ -7737,7 +7710,7 @@
         <v>20</v>
       </c>
       <c r="E124" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F124" t="s">
         <v>29</v>
@@ -7766,7 +7739,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B125" s="45" t="s">
         <v>166</v>
@@ -7799,12 +7772,12 @@
         <v>2021</v>
       </c>
       <c r="O125" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B126" s="45" t="s">
         <v>166</v>
@@ -7819,7 +7792,7 @@
         <v>157</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J126" s="1" t="s">
         <v>142</v>
@@ -7837,12 +7810,12 @@
         <v>2021</v>
       </c>
       <c r="O126" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B127" s="45" t="s">
         <v>166</v>
@@ -7857,7 +7830,7 @@
         <v>157</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J127" s="1" t="s">
         <v>142</v>
@@ -7875,12 +7848,12 @@
         <v>2021</v>
       </c>
       <c r="O127" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B128" s="45" t="s">
         <v>166</v>
@@ -7895,7 +7868,7 @@
         <v>157</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J128" s="1" t="s">
         <v>142</v>
@@ -7913,12 +7886,12 @@
         <v>2021</v>
       </c>
       <c r="O128" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B129" s="45" t="s">
         <v>166</v>
@@ -7933,7 +7906,7 @@
         <v>157</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H129" t="b">
         <v>1</v>
@@ -7954,12 +7927,12 @@
         <v>2021</v>
       </c>
       <c r="O129" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B130" s="45" t="s">
         <v>166</v>
@@ -7971,7 +7944,7 @@
         <v>150</v>
       </c>
       <c r="F130" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>158</v>
@@ -7997,7 +7970,7 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G131" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>171</v>
@@ -8036,28 +8009,20 @@
     <sortCondition ref="C19:C98"/>
   </sortState>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="K1:K70 K72:K1046825">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="K1:K1046825">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V103">
-    <cfRule type="containsText" dxfId="11" priority="29" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",V103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="30" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="8" priority="30" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",V103)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K71)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -8344,6 +8309,7 @@
     <hyperlink ref="G64" r:id="rId281" xr:uid="{2862841D-A50B-6449-AE6C-1451BED85BD4}"/>
     <hyperlink ref="G71" r:id="rId282" xr:uid="{81B7CA7F-5C73-D84F-9E77-FE49F0E2EF43}"/>
     <hyperlink ref="J71" r:id="rId283" xr:uid="{BF39AFF0-2EFA-DC4C-BE56-54321A0C8D97}"/>
+    <hyperlink ref="G128" r:id="rId284" xr:uid="{76685A1D-C80C-F84C-80B4-A4BC5559831C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8398,8 +8364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA36285-19E8-D244-9D5D-ABE845366A0D}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8416,7 +8382,7 @@
         <v>70</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C1" s="59" t="s">
         <v>119</v>
@@ -8437,10 +8403,10 @@
         <v>118</v>
       </c>
       <c r="I1" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="J1" s="61" t="s">
         <v>366</v>
-      </c>
-      <c r="J1" s="61" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -8451,14 +8417,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="54" t="s">
         <v>179</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>535</v>
       </c>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
@@ -8466,7 +8434,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -8477,16 +8445,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>180</v>
       </c>
       <c r="E3" s="55" t="s">
+        <v>392</v>
+      </c>
+      <c r="F3" s="55" t="s">
         <v>393</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>394</v>
       </c>
       <c r="G3" s="55">
         <v>2023</v>
@@ -8503,7 +8471,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>166</v>
@@ -8512,13 +8480,13 @@
         <v>72</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G4" s="55">
         <v>2025</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I4" s="55"/>
       <c r="J4" s="55"/>
@@ -8531,7 +8499,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>165</v>
@@ -8540,7 +8508,7 @@
         <v>72</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G5" s="55">
         <v>2024</v>
@@ -8583,16 +8551,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>165</v>
       </c>
       <c r="E7" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="F7" s="55" t="s">
         <v>401</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>402</v>
       </c>
       <c r="G7" s="55">
         <v>2022</v>
@@ -8652,10 +8620,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H4">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9149,18 +9117,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9559,10 +9527,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K10">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9641,7 +9609,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>180</v>
@@ -9649,8 +9617,8 @@
       <c r="C1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="65" t="s">
-        <v>408</v>
+      <c r="D1" s="64" t="s">
+        <v>407</v>
       </c>
       <c r="E1" s="20">
         <v>2022</v>

</xml_diff>

<commit_message>
UPDATE: removed citation for GproteinDB
</commit_message>
<xml_diff>
--- a/common_data/Site_References.xlsx
+++ b/common_data/Site_References.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhg791/gpcrdb_data/common_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A319E3B-EAF6-F74B-950D-7A7165C8F883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F3E4BA-A290-BB4F-881C-BFD80571699B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20600" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -2552,9 +2552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z135"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8310,6 +8310,7 @@
     <hyperlink ref="G71" r:id="rId282" xr:uid="{81B7CA7F-5C73-D84F-9E77-FE49F0E2EF43}"/>
     <hyperlink ref="J71" r:id="rId283" xr:uid="{BF39AFF0-2EFA-DC4C-BE56-54321A0C8D97}"/>
     <hyperlink ref="G128" r:id="rId284" xr:uid="{76685A1D-C80C-F84C-80B4-A4BC5559831C}"/>
+    <hyperlink ref="G50" r:id="rId285" xr:uid="{473658F1-D093-1246-A2FE-E4BDB68FC2CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8362,10 +8363,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA36285-19E8-D244-9D5D-ABE845366A0D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8543,38 +8544,11 @@
       <c r="I6" s="55"/>
       <c r="J6" s="55"/>
     </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>400</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>401</v>
-      </c>
-      <c r="G7" s="55">
-        <v>2022</v>
-      </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{39B07FB9-EFC7-0B40-A513-B395F548E339}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{98D34980-C0E6-6647-B4EF-20D6D641C525}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{27592559-DADD-434E-A36F-01B0A753C48B}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{7EAE46CE-CEC4-884F-A327-67155D44087D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9555,15 +9529,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A319B161-96D8-2F4D-8D79-4370C9A8D76B}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -9582,10 +9560,33 @@
       <c r="F1" s="55" t="s">
         <v>140</v>
       </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>401</v>
+      </c>
+      <c r="E2" s="55">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{E62F3315-5205-D849-AE92-4F11E4ACB4A0}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{7EAE46CE-CEC4-884F-A327-67155D44087D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>